<commit_message>
Aggiunte analisi su CodeGPT, modificati i requirements, presentazione sui risultati
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/AnalisiCodeGPT.xlsx
+++ b/HE/W_in_progress/AnalisiCodeGPT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0804D0CF-96CB-4E46-B72E-A25F2A852A92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BD4C6E2-73BB-421E-85BD-A6B4966594FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="918">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="927">
   <si>
     <t>IN</t>
   </si>
@@ -870,12 +870,18 @@
     <t>out_signal &lt;= data1 or data2;</t>
   </si>
   <si>
+    <t>Non fa la nor</t>
+  </si>
+  <si>
     <t>set tempq0 signal to the first element of temp_p signal</t>
   </si>
   <si>
     <t>temp_p &lt;= temp_p(0); temp_q &lt;= temp_q(1);</t>
   </si>
   <si>
+    <t>Nomi sbagliati, ma bene o male fa quello richiesto</t>
+  </si>
+  <si>
     <t>the signal out_data is set to the OR operation between dividend and divisor</t>
   </si>
   <si>
@@ -906,6 +912,9 @@
     <t>output &lt;= operand1 or operand2;</t>
   </si>
   <si>
+    <t>Non fa la and</t>
+  </si>
+  <si>
     <t>define the signal TbClockB so that it changes its state after TbPeriodB</t>
   </si>
   <si>
@@ -939,6 +948,9 @@
     <t>FF_D &lt;= clock; if (rising_edge(clock)) then if (reset = '1') then y &lt;= '0'; else y &lt;= d; end if;</t>
   </si>
   <si>
+    <t>Non è un process</t>
+  </si>
+  <si>
     <t>generate the clock signal clk_tb with period clk_period</t>
   </si>
   <si>
@@ -957,6 +969,9 @@
     <t>if rising_edge(clk_in) then if( reset_n = '1') then temp := 25; start_sig &lt;= '1'; end if; end if;</t>
   </si>
   <si>
+    <t>Non fa il decremento</t>
+  </si>
+  <si>
     <t>on the rising edge of clk, if rst_n signal is '0', set tick_o_reg to '0', reset reg_count_reg signal to 0</t>
   </si>
   <si>
@@ -993,6 +1008,12 @@
     <t>i_start_counter &lt;= 0; t_start &lt;= '0'; t_stb &lt;= '0';</t>
   </si>
   <si>
+    <t>Non c'è l'if</t>
+  </si>
+  <si>
+    <t>Assegnazione invertita</t>
+  </si>
+  <si>
     <t>set sda_o signal to i_sda when rst_n_i signal is high, otherwise set it to low</t>
   </si>
   <si>
@@ -1173,6 +1194,9 @@
     <t>entity deglitcher_testbench is port (clk : in std_logic; rst : in std_logic; clkB : in std_logic; rstA : in std_logic; clkBB : in std_logic; rstA_in : in std_logic; rstB : in std_logic; sclk : in std_logic; sclkB : in std_logic; sclkB_in : in std_logic; sclkB_out : out std_logic); end deglitcher_testbench;</t>
   </si>
   <si>
+    <t>Definisce un entità, ha dei parametri a caso, ma tutto sommato va bene</t>
+  </si>
+  <si>
     <t>Encoder_onBoard is an entity with switch as input std_logic_vector of 10 bit, led as output std_logic_vector signal of 4 bit, catodi as output std_logic_vector signal of 8 bit, anodi as output std_logic_vector signal of 8 bit</t>
   </si>
   <si>
@@ -1186,6 +1210,9 @@
   </si>
   <si>
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity IEEE_STD_LOGIC_1164 is Generic (N : natural := 8); Port ( N : natural := 8 ); end IEEE_STD_LOGIC_1164; architecture Behavioral of IEEE_STD_LOGIC_1164 is begin process (N) begin if (N = '1') then ; end if ; end process ; end Behavioral;</t>
+  </si>
+  <si>
+    <t>Non include la libreria richiesta</t>
   </si>
   <si>
     <t>define the entity add_round_key with round_key_in, data_in as input 64 std_logic_vector, data_out as output 64 std_logic_vector</t>
@@ -3157,8 +3184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
-      <selection activeCell="H310" sqref="H310"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="G142" sqref="G142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5283,6 +5310,9 @@
       <c r="G86">
         <v>0</v>
       </c>
+      <c r="H86" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="87" spans="1:8">
       <c r="A87" t="s">
@@ -5332,6 +5362,9 @@
       <c r="G88">
         <v>0</v>
       </c>
+      <c r="H88" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
@@ -5355,6 +5388,9 @@
       <c r="G89">
         <v>0</v>
       </c>
+      <c r="H89" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="90" spans="1:8">
       <c r="A90" t="s">
@@ -5376,7 +5412,10 @@
         <v>0.52394366197183095</v>
       </c>
       <c r="G90">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H90" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -5399,7 +5438,10 @@
         <v>0.71556122448979587</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H91" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -5424,6 +5466,9 @@
       <c r="G92">
         <v>0</v>
       </c>
+      <c r="H92" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="93" spans="1:8">
       <c r="A93" t="s">
@@ -5445,7 +5490,10 @@
         <v>0.52394366197183095</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H93" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -5491,7 +5539,10 @@
         <v>0.73390894819466246</v>
       </c>
       <c r="G95">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H95" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -5539,16 +5590,19 @@
       <c r="G97">
         <v>0</v>
       </c>
+      <c r="H97" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B98" t="s">
         <v>241</v>
       </c>
       <c r="C98" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -5560,12 +5614,15 @@
         <v>0.65051020408163263</v>
       </c>
       <c r="G98">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H98" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="99" spans="1:8">
       <c r="A99" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B99" t="s">
         <v>275</v>
@@ -5588,13 +5645,13 @@
     </row>
     <row r="100" spans="1:8">
       <c r="A100" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B100" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C100" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -5608,16 +5665,19 @@
       <c r="G100">
         <v>0</v>
       </c>
+      <c r="H100" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="101" spans="1:8">
       <c r="A101" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="B101" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C101" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -5629,18 +5689,21 @@
         <v>0.62</v>
       </c>
       <c r="G101">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H101" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="102" spans="1:8">
       <c r="A102" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B102" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C102" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -5654,16 +5717,19 @@
       <c r="G102">
         <v>0</v>
       </c>
+      <c r="H102" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="103" spans="1:8">
       <c r="A103" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B103" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C103" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -5677,16 +5743,19 @@
       <c r="G103">
         <v>0</v>
       </c>
+      <c r="H103" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="104" spans="1:8">
       <c r="A104" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B104" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C104" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D104">
         <v>0</v>
@@ -5698,15 +5767,18 @@
         <v>0.91496967882009439</v>
       </c>
       <c r="G104">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H104" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="105" spans="1:8">
       <c r="A105" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B105" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C105" t="s">
         <v>53</v>
@@ -5729,13 +5801,13 @@
     </row>
     <row r="106" spans="1:8">
       <c r="A106" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B106" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C106" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -5749,16 +5821,19 @@
       <c r="G106">
         <v>0</v>
       </c>
+      <c r="H106" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="107" spans="1:8">
       <c r="A107" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="B107" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C107" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -5772,16 +5847,19 @@
       <c r="G107">
         <v>0</v>
       </c>
+      <c r="H107" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="108" spans="1:8">
       <c r="A108" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B108" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="C108" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -5795,16 +5873,19 @@
       <c r="G108">
         <v>0</v>
       </c>
+      <c r="H108" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="109" spans="1:8">
       <c r="A109" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="B109" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="C109" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="D109">
         <v>0</v>
@@ -5816,18 +5897,21 @@
         <v>0.73081647940074912</v>
       </c>
       <c r="G109">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H109" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="110" spans="1:8">
       <c r="A110" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="B110" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="C110" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="D110">
         <v>0</v>
@@ -5841,16 +5925,19 @@
       <c r="G110">
         <v>0</v>
       </c>
+      <c r="H110" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="111" spans="1:8">
       <c r="A111" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="B111" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="C111" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="D111">
         <v>0</v>
@@ -5862,18 +5949,18 @@
         <v>0.84378103858623321</v>
       </c>
       <c r="G111">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:8">
       <c r="A112" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="B112" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="C112" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="D112">
         <v>0</v>
@@ -5887,16 +5974,19 @@
       <c r="G112">
         <v>0</v>
       </c>
+      <c r="H112" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="113" spans="1:8">
       <c r="A113" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="B113" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="C113" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -5910,16 +6000,19 @@
       <c r="G113">
         <v>0</v>
       </c>
+      <c r="H113" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="114" spans="1:8">
       <c r="A114" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="B114" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="C114" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="D114">
         <v>0</v>
@@ -5933,16 +6026,19 @@
       <c r="G114">
         <v>0</v>
       </c>
+      <c r="H114" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="115" spans="1:8">
       <c r="A115" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="B115" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="C115" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="D115">
         <v>1</v>
@@ -5959,13 +6055,13 @@
     </row>
     <row r="116" spans="1:8">
       <c r="A116" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="B116" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="C116" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -5979,13 +6075,16 @@
       <c r="G116">
         <v>0</v>
       </c>
+      <c r="H116" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="117" spans="1:8">
       <c r="A117" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="B117" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="C117" t="s">
         <v>53</v>
@@ -6008,13 +6107,13 @@
     </row>
     <row r="118" spans="1:8">
       <c r="A118" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="B118" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="C118" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -6028,16 +6127,19 @@
       <c r="G118">
         <v>0</v>
       </c>
+      <c r="H118" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="119" spans="1:8">
       <c r="A119" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="B119" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="C119" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -6051,16 +6153,19 @@
       <c r="G119">
         <v>0</v>
       </c>
+      <c r="H119" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="120" spans="1:8">
       <c r="A120" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="B120" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="C120" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="D120">
         <v>0</v>
@@ -6072,18 +6177,18 @@
         <v>0.94993074792243781</v>
       </c>
       <c r="G120">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:8">
       <c r="A121" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="B121" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="C121" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="D121">
         <v>0</v>
@@ -6097,16 +6202,19 @@
       <c r="G121">
         <v>0</v>
       </c>
+      <c r="H121" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="122" spans="1:8">
       <c r="A122" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="B122" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="C122" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="D122">
         <v>0</v>
@@ -6118,15 +6226,15 @@
         <v>0.99997155211652256</v>
       </c>
       <c r="G122">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:8">
       <c r="A123" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="B123" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="C123" t="s">
         <v>53</v>
@@ -6149,13 +6257,13 @@
     </row>
     <row r="124" spans="1:8">
       <c r="A124" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="B124" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="C124" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="D124">
         <v>0</v>
@@ -6169,13 +6277,16 @@
       <c r="G124">
         <v>0</v>
       </c>
+      <c r="H124" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="125" spans="1:8">
       <c r="A125" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="B125" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="C125" t="s">
         <v>53</v>
@@ -6198,13 +6309,13 @@
     </row>
     <row r="126" spans="1:8">
       <c r="A126" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="B126" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="C126" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="D126">
         <v>0</v>
@@ -6216,18 +6327,21 @@
         <v>0.4508928571428571</v>
       </c>
       <c r="G126">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H126" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="127" spans="1:8">
       <c r="A127" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="B127" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="C127" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="D127">
         <v>0</v>
@@ -6241,16 +6355,19 @@
       <c r="G127">
         <v>0</v>
       </c>
+      <c r="H127" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="128" spans="1:8">
       <c r="A128" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="B128" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="C128" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="D128">
         <v>0</v>
@@ -6264,16 +6381,19 @@
       <c r="G128">
         <v>0</v>
       </c>
+      <c r="H128" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="129" spans="1:8">
       <c r="A129" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="B129" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="C129" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="D129">
         <v>0</v>
@@ -6287,16 +6407,19 @@
       <c r="G129">
         <v>0</v>
       </c>
+      <c r="H129" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="130" spans="1:8">
       <c r="A130" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="B130" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="C130" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="D130">
         <v>0</v>
@@ -6310,16 +6433,19 @@
       <c r="G130">
         <v>0</v>
       </c>
+      <c r="H130" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="131" spans="1:8">
       <c r="A131" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="B131" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="C131" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="D131">
         <v>0</v>
@@ -6333,16 +6459,19 @@
       <c r="G131">
         <v>0</v>
       </c>
+      <c r="H131" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="132" spans="1:8">
       <c r="A132" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="B132" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="C132" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="D132">
         <v>0</v>
@@ -6356,16 +6485,19 @@
       <c r="G132">
         <v>0</v>
       </c>
+      <c r="H132" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="133" spans="1:8">
       <c r="A133" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="B133" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="C133" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="D133">
         <v>0</v>
@@ -6379,16 +6511,19 @@
       <c r="G133">
         <v>0</v>
       </c>
+      <c r="H133" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="134" spans="1:8">
       <c r="A134" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="B134" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="C134" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="D134">
         <v>0</v>
@@ -6402,16 +6537,19 @@
       <c r="G134">
         <v>0</v>
       </c>
+      <c r="H134" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="135" spans="1:8">
       <c r="A135" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="B135" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="C135" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="D135">
         <v>0</v>
@@ -6423,15 +6561,18 @@
         <v>0.40244969378827639</v>
       </c>
       <c r="G135">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H135" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="136" spans="1:8">
       <c r="A136" t="s">
-        <v>380</v>
+        <v>388</v>
       </c>
       <c r="B136" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="C136" t="s">
         <v>53</v>
@@ -6454,13 +6595,13 @@
     </row>
     <row r="137" spans="1:8">
       <c r="A137" t="s">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="B137" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="C137" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="D137">
         <v>0</v>
@@ -6474,16 +6615,19 @@
       <c r="G137">
         <v>0</v>
       </c>
+      <c r="H137" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="138" spans="1:8">
       <c r="A138" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="B138" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="C138" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="D138">
         <v>0</v>
@@ -6495,18 +6639,18 @@
         <v>0.99999157099748814</v>
       </c>
       <c r="G138">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:8">
       <c r="A139" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="B139" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="C139" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="D139">
         <v>0</v>
@@ -6518,18 +6662,18 @@
         <v>0.63487544483985781</v>
       </c>
       <c r="G139">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:8">
       <c r="A140" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="B140" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="C140" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="D140">
         <v>0</v>
@@ -6541,18 +6685,18 @@
         <v>0.94540816326530619</v>
       </c>
       <c r="G140">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:8">
       <c r="A141" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="B141" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="C141" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
       <c r="D141">
         <v>0</v>
@@ -6564,18 +6708,18 @@
         <v>0.99999157099748814</v>
       </c>
       <c r="G141">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:8">
       <c r="A142" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="B142" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="C142" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="D142">
         <v>1</v>
@@ -6592,13 +6736,13 @@
     </row>
     <row r="143" spans="1:8">
       <c r="A143" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="B143" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="C143" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="D143">
         <v>0</v>
@@ -6615,13 +6759,13 @@
     </row>
     <row r="144" spans="1:8">
       <c r="A144" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="B144" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="C144" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="D144">
         <v>0</v>
@@ -6638,10 +6782,10 @@
     </row>
     <row r="145" spans="1:8">
       <c r="A145" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
       <c r="B145" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="C145" t="s">
         <v>53</v>
@@ -6664,13 +6808,13 @@
     </row>
     <row r="146" spans="1:8">
       <c r="A146" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
       <c r="B146" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="C146" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="D146">
         <v>0</v>
@@ -6687,13 +6831,13 @@
     </row>
     <row r="147" spans="1:8">
       <c r="A147" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
       <c r="B147" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="C147" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
       <c r="D147">
         <v>0</v>
@@ -6710,13 +6854,13 @@
     </row>
     <row r="148" spans="1:8">
       <c r="A148" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
       <c r="B148" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
       <c r="C148" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="D148">
         <v>0</v>
@@ -6733,13 +6877,13 @@
     </row>
     <row r="149" spans="1:8">
       <c r="A149" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="B149" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="C149" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="D149">
         <v>0</v>
@@ -6756,13 +6900,13 @@
     </row>
     <row r="150" spans="1:8">
       <c r="A150" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="B150" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="C150" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
       <c r="D150">
         <v>0</v>
@@ -6779,10 +6923,10 @@
     </row>
     <row r="151" spans="1:8">
       <c r="A151" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
       <c r="B151" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
       <c r="C151" t="s">
         <v>53</v>
@@ -6805,13 +6949,13 @@
     </row>
     <row r="152" spans="1:8">
       <c r="A152" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
       <c r="B152" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
       <c r="C152" t="s">
-        <v>425</v>
+        <v>434</v>
       </c>
       <c r="D152">
         <v>0</v>
@@ -6828,13 +6972,13 @@
     </row>
     <row r="153" spans="1:8">
       <c r="A153" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
       <c r="B153" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="C153" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
       <c r="D153">
         <v>0</v>
@@ -6851,13 +6995,13 @@
     </row>
     <row r="154" spans="1:8">
       <c r="A154" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="B154" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="C154" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="D154">
         <v>0</v>
@@ -6874,13 +7018,13 @@
     </row>
     <row r="155" spans="1:8">
       <c r="A155" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
       <c r="B155" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="C155" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
       <c r="D155">
         <v>0</v>
@@ -6897,10 +7041,10 @@
     </row>
     <row r="156" spans="1:8">
       <c r="A156" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="B156" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
       <c r="C156" t="s">
         <v>53</v>
@@ -6923,13 +7067,13 @@
     </row>
     <row r="157" spans="1:8">
       <c r="A157" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="B157" t="s">
-        <v>438</v>
+        <v>447</v>
       </c>
       <c r="C157" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
       <c r="D157">
         <v>0</v>
@@ -6946,13 +7090,13 @@
     </row>
     <row r="158" spans="1:8">
       <c r="A158" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
       <c r="B158" t="s">
-        <v>441</v>
+        <v>450</v>
       </c>
       <c r="C158" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
       <c r="D158">
         <v>0</v>
@@ -6969,13 +7113,13 @@
     </row>
     <row r="159" spans="1:8">
       <c r="A159" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
       <c r="B159" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
       <c r="C159" t="s">
-        <v>445</v>
+        <v>454</v>
       </c>
       <c r="D159">
         <v>0</v>
@@ -6992,13 +7136,13 @@
     </row>
     <row r="160" spans="1:8">
       <c r="A160" t="s">
-        <v>446</v>
+        <v>455</v>
       </c>
       <c r="B160" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="C160" t="s">
-        <v>448</v>
+        <v>457</v>
       </c>
       <c r="D160">
         <v>0</v>
@@ -7015,13 +7159,13 @@
     </row>
     <row r="161" spans="1:8">
       <c r="A161" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
       <c r="B161" t="s">
-        <v>450</v>
+        <v>459</v>
       </c>
       <c r="C161" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
       <c r="D161">
         <v>0</v>
@@ -7038,13 +7182,13 @@
     </row>
     <row r="162" spans="1:8">
       <c r="A162" t="s">
-        <v>452</v>
+        <v>461</v>
       </c>
       <c r="B162" t="s">
-        <v>453</v>
+        <v>462</v>
       </c>
       <c r="C162" t="s">
-        <v>453</v>
+        <v>462</v>
       </c>
       <c r="D162">
         <v>1</v>
@@ -7061,13 +7205,13 @@
     </row>
     <row r="163" spans="1:8">
       <c r="A163" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
       <c r="B163" t="s">
-        <v>455</v>
+        <v>464</v>
       </c>
       <c r="C163" t="s">
-        <v>456</v>
+        <v>465</v>
       </c>
       <c r="D163">
         <v>0</v>
@@ -7084,10 +7228,10 @@
     </row>
     <row r="164" spans="1:8">
       <c r="A164" t="s">
-        <v>457</v>
+        <v>466</v>
       </c>
       <c r="B164" t="s">
-        <v>458</v>
+        <v>467</v>
       </c>
       <c r="C164" t="s">
         <v>53</v>
@@ -7110,10 +7254,10 @@
     </row>
     <row r="165" spans="1:8">
       <c r="A165" t="s">
-        <v>459</v>
+        <v>468</v>
       </c>
       <c r="B165" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
       <c r="C165" t="s">
         <v>53</v>
@@ -7136,13 +7280,13 @@
     </row>
     <row r="166" spans="1:8">
       <c r="A166" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="B166" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="C166" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
       <c r="D166">
         <v>0</v>
@@ -7159,13 +7303,13 @@
     </row>
     <row r="167" spans="1:8">
       <c r="A167" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
       <c r="B167" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
       <c r="C167" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
       <c r="D167">
         <v>0</v>
@@ -7182,13 +7326,13 @@
     </row>
     <row r="168" spans="1:8">
       <c r="A168" t="s">
-        <v>467</v>
+        <v>476</v>
       </c>
       <c r="B168" t="s">
-        <v>468</v>
+        <v>477</v>
       </c>
       <c r="C168" t="s">
-        <v>468</v>
+        <v>477</v>
       </c>
       <c r="D168">
         <v>1</v>
@@ -7205,13 +7349,13 @@
     </row>
     <row r="169" spans="1:8">
       <c r="A169" t="s">
-        <v>469</v>
+        <v>478</v>
       </c>
       <c r="B169" t="s">
-        <v>470</v>
+        <v>479</v>
       </c>
       <c r="C169" t="s">
-        <v>471</v>
+        <v>480</v>
       </c>
       <c r="D169">
         <v>0</v>
@@ -7228,13 +7372,13 @@
     </row>
     <row r="170" spans="1:8">
       <c r="A170" t="s">
-        <v>472</v>
+        <v>481</v>
       </c>
       <c r="B170" t="s">
-        <v>473</v>
+        <v>482</v>
       </c>
       <c r="C170" t="s">
-        <v>473</v>
+        <v>482</v>
       </c>
       <c r="D170">
         <v>1</v>
@@ -7251,13 +7395,13 @@
     </row>
     <row r="171" spans="1:8">
       <c r="A171" t="s">
-        <v>474</v>
+        <v>483</v>
       </c>
       <c r="B171" t="s">
-        <v>475</v>
+        <v>484</v>
       </c>
       <c r="C171" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
       <c r="D171">
         <v>0</v>
@@ -7274,13 +7418,13 @@
     </row>
     <row r="172" spans="1:8">
       <c r="A172" t="s">
-        <v>477</v>
+        <v>486</v>
       </c>
       <c r="B172" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
       <c r="C172" t="s">
-        <v>478</v>
+        <v>487</v>
       </c>
       <c r="D172">
         <v>0</v>
@@ -7297,13 +7441,13 @@
     </row>
     <row r="173" spans="1:8">
       <c r="A173" t="s">
-        <v>479</v>
+        <v>488</v>
       </c>
       <c r="B173" t="s">
-        <v>480</v>
+        <v>489</v>
       </c>
       <c r="C173" t="s">
-        <v>480</v>
+        <v>489</v>
       </c>
       <c r="D173">
         <v>1</v>
@@ -7320,13 +7464,13 @@
     </row>
     <row r="174" spans="1:8">
       <c r="A174" t="s">
-        <v>481</v>
+        <v>490</v>
       </c>
       <c r="B174" t="s">
-        <v>482</v>
+        <v>491</v>
       </c>
       <c r="C174" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
       <c r="D174">
         <v>0</v>
@@ -7343,13 +7487,13 @@
     </row>
     <row r="175" spans="1:8">
       <c r="A175" t="s">
-        <v>484</v>
+        <v>493</v>
       </c>
       <c r="B175" t="s">
-        <v>485</v>
+        <v>494</v>
       </c>
       <c r="C175" t="s">
-        <v>486</v>
+        <v>495</v>
       </c>
       <c r="D175">
         <v>0</v>
@@ -7366,13 +7510,13 @@
     </row>
     <row r="176" spans="1:8">
       <c r="A176" t="s">
-        <v>487</v>
+        <v>496</v>
       </c>
       <c r="B176" t="s">
-        <v>488</v>
+        <v>497</v>
       </c>
       <c r="C176" t="s">
-        <v>489</v>
+        <v>498</v>
       </c>
       <c r="D176">
         <v>0</v>
@@ -7389,13 +7533,13 @@
     </row>
     <row r="177" spans="1:7">
       <c r="A177" t="s">
-        <v>490</v>
+        <v>499</v>
       </c>
       <c r="B177" t="s">
         <v>135</v>
       </c>
       <c r="C177" t="s">
-        <v>491</v>
+        <v>500</v>
       </c>
       <c r="D177">
         <v>0</v>
@@ -7412,13 +7556,13 @@
     </row>
     <row r="178" spans="1:7">
       <c r="A178" t="s">
-        <v>492</v>
+        <v>501</v>
       </c>
       <c r="B178" t="s">
-        <v>493</v>
+        <v>502</v>
       </c>
       <c r="C178" t="s">
-        <v>494</v>
+        <v>503</v>
       </c>
       <c r="D178">
         <v>0</v>
@@ -7435,13 +7579,13 @@
     </row>
     <row r="179" spans="1:7">
       <c r="A179" t="s">
-        <v>495</v>
+        <v>504</v>
       </c>
       <c r="B179" t="s">
-        <v>496</v>
+        <v>505</v>
       </c>
       <c r="C179" t="s">
-        <v>497</v>
+        <v>506</v>
       </c>
       <c r="D179">
         <v>0</v>
@@ -7458,13 +7602,13 @@
     </row>
     <row r="180" spans="1:7">
       <c r="A180" t="s">
-        <v>498</v>
+        <v>507</v>
       </c>
       <c r="B180" t="s">
-        <v>493</v>
+        <v>502</v>
       </c>
       <c r="C180" t="s">
-        <v>499</v>
+        <v>508</v>
       </c>
       <c r="D180">
         <v>0</v>
@@ -7481,13 +7625,13 @@
     </row>
     <row r="181" spans="1:7">
       <c r="A181" t="s">
-        <v>500</v>
+        <v>509</v>
       </c>
       <c r="B181" t="s">
-        <v>501</v>
+        <v>510</v>
       </c>
       <c r="C181" t="s">
-        <v>502</v>
+        <v>511</v>
       </c>
       <c r="D181">
         <v>0</v>
@@ -7504,13 +7648,13 @@
     </row>
     <row r="182" spans="1:7">
       <c r="A182" t="s">
-        <v>503</v>
+        <v>512</v>
       </c>
       <c r="B182" t="s">
-        <v>504</v>
+        <v>513</v>
       </c>
       <c r="C182" t="s">
-        <v>505</v>
+        <v>514</v>
       </c>
       <c r="D182">
         <v>0</v>
@@ -7527,13 +7671,13 @@
     </row>
     <row r="183" spans="1:7">
       <c r="A183" t="s">
-        <v>506</v>
+        <v>515</v>
       </c>
       <c r="B183" t="s">
-        <v>507</v>
+        <v>516</v>
       </c>
       <c r="C183" t="s">
-        <v>507</v>
+        <v>516</v>
       </c>
       <c r="D183">
         <v>1</v>
@@ -7550,13 +7694,13 @@
     </row>
     <row r="184" spans="1:7">
       <c r="A184" t="s">
-        <v>508</v>
+        <v>517</v>
       </c>
       <c r="B184" t="s">
-        <v>509</v>
+        <v>518</v>
       </c>
       <c r="C184" t="s">
-        <v>510</v>
+        <v>519</v>
       </c>
       <c r="D184">
         <v>0</v>
@@ -7573,13 +7717,13 @@
     </row>
     <row r="185" spans="1:7">
       <c r="A185" t="s">
-        <v>511</v>
+        <v>520</v>
       </c>
       <c r="B185" t="s">
-        <v>512</v>
+        <v>521</v>
       </c>
       <c r="C185" t="s">
-        <v>513</v>
+        <v>522</v>
       </c>
       <c r="D185">
         <v>0</v>
@@ -7596,13 +7740,13 @@
     </row>
     <row r="186" spans="1:7">
       <c r="A186" t="s">
-        <v>514</v>
+        <v>523</v>
       </c>
       <c r="B186" t="s">
-        <v>515</v>
+        <v>524</v>
       </c>
       <c r="C186" t="s">
-        <v>516</v>
+        <v>525</v>
       </c>
       <c r="D186">
         <v>0</v>
@@ -7619,13 +7763,13 @@
     </row>
     <row r="187" spans="1:7">
       <c r="A187" t="s">
-        <v>517</v>
+        <v>526</v>
       </c>
       <c r="B187" t="s">
-        <v>518</v>
+        <v>527</v>
       </c>
       <c r="C187" t="s">
-        <v>519</v>
+        <v>528</v>
       </c>
       <c r="D187">
         <v>0</v>
@@ -7642,13 +7786,13 @@
     </row>
     <row r="188" spans="1:7">
       <c r="A188" t="s">
-        <v>520</v>
+        <v>529</v>
       </c>
       <c r="B188" t="s">
-        <v>521</v>
+        <v>530</v>
       </c>
       <c r="C188" t="s">
-        <v>522</v>
+        <v>531</v>
       </c>
       <c r="D188">
         <v>0</v>
@@ -7665,13 +7809,13 @@
     </row>
     <row r="189" spans="1:7">
       <c r="A189" t="s">
-        <v>523</v>
+        <v>532</v>
       </c>
       <c r="B189" t="s">
-        <v>524</v>
+        <v>533</v>
       </c>
       <c r="C189" t="s">
-        <v>525</v>
+        <v>534</v>
       </c>
       <c r="D189">
         <v>0</v>
@@ -7688,13 +7832,13 @@
     </row>
     <row r="190" spans="1:7">
       <c r="A190" t="s">
-        <v>526</v>
+        <v>535</v>
       </c>
       <c r="B190" t="s">
-        <v>527</v>
+        <v>536</v>
       </c>
       <c r="C190" t="s">
-        <v>528</v>
+        <v>537</v>
       </c>
       <c r="D190">
         <v>0</v>
@@ -7711,13 +7855,13 @@
     </row>
     <row r="191" spans="1:7">
       <c r="A191" t="s">
-        <v>529</v>
+        <v>538</v>
       </c>
       <c r="B191" t="s">
-        <v>530</v>
+        <v>539</v>
       </c>
       <c r="C191" t="s">
-        <v>530</v>
+        <v>539</v>
       </c>
       <c r="D191">
         <v>1</v>
@@ -7734,13 +7878,13 @@
     </row>
     <row r="192" spans="1:7">
       <c r="A192" t="s">
-        <v>531</v>
+        <v>540</v>
       </c>
       <c r="B192" t="s">
-        <v>532</v>
+        <v>541</v>
       </c>
       <c r="C192" t="s">
-        <v>533</v>
+        <v>542</v>
       </c>
       <c r="D192">
         <v>0</v>
@@ -7757,10 +7901,10 @@
     </row>
     <row r="193" spans="1:8">
       <c r="A193" t="s">
-        <v>534</v>
+        <v>543</v>
       </c>
       <c r="B193" t="s">
-        <v>535</v>
+        <v>544</v>
       </c>
       <c r="C193" t="s">
         <v>53</v>
@@ -7783,13 +7927,13 @@
     </row>
     <row r="194" spans="1:8">
       <c r="A194" t="s">
-        <v>536</v>
+        <v>545</v>
       </c>
       <c r="B194" t="s">
-        <v>537</v>
+        <v>546</v>
       </c>
       <c r="C194" t="s">
-        <v>538</v>
+        <v>547</v>
       </c>
       <c r="D194">
         <v>0</v>
@@ -7806,10 +7950,10 @@
     </row>
     <row r="195" spans="1:8">
       <c r="A195" t="s">
-        <v>539</v>
+        <v>548</v>
       </c>
       <c r="B195" t="s">
-        <v>540</v>
+        <v>549</v>
       </c>
       <c r="C195" t="s">
         <v>53</v>
@@ -7832,13 +7976,13 @@
     </row>
     <row r="196" spans="1:8">
       <c r="A196" t="s">
-        <v>541</v>
+        <v>550</v>
       </c>
       <c r="B196" t="s">
-        <v>542</v>
+        <v>551</v>
       </c>
       <c r="C196" t="s">
-        <v>543</v>
+        <v>552</v>
       </c>
       <c r="D196">
         <v>0</v>
@@ -7855,13 +7999,13 @@
     </row>
     <row r="197" spans="1:8">
       <c r="A197" t="s">
-        <v>544</v>
+        <v>553</v>
       </c>
       <c r="B197" t="s">
-        <v>545</v>
+        <v>554</v>
       </c>
       <c r="C197" t="s">
-        <v>546</v>
+        <v>555</v>
       </c>
       <c r="D197">
         <v>0</v>
@@ -7878,13 +8022,13 @@
     </row>
     <row r="198" spans="1:8">
       <c r="A198" t="s">
-        <v>547</v>
+        <v>556</v>
       </c>
       <c r="B198" t="s">
-        <v>548</v>
+        <v>557</v>
       </c>
       <c r="C198" t="s">
-        <v>549</v>
+        <v>558</v>
       </c>
       <c r="D198">
         <v>0</v>
@@ -7901,13 +8045,13 @@
     </row>
     <row r="199" spans="1:8">
       <c r="A199" t="s">
-        <v>550</v>
+        <v>559</v>
       </c>
       <c r="B199" t="s">
-        <v>551</v>
+        <v>560</v>
       </c>
       <c r="C199" t="s">
-        <v>552</v>
+        <v>561</v>
       </c>
       <c r="D199">
         <v>0</v>
@@ -7924,13 +8068,13 @@
     </row>
     <row r="200" spans="1:8">
       <c r="A200" t="s">
-        <v>553</v>
+        <v>562</v>
       </c>
       <c r="B200" t="s">
-        <v>554</v>
+        <v>563</v>
       </c>
       <c r="C200" t="s">
-        <v>555</v>
+        <v>564</v>
       </c>
       <c r="D200">
         <v>0</v>
@@ -7947,13 +8091,13 @@
     </row>
     <row r="201" spans="1:8">
       <c r="A201" t="s">
-        <v>556</v>
+        <v>565</v>
       </c>
       <c r="B201" t="s">
-        <v>557</v>
+        <v>566</v>
       </c>
       <c r="C201" t="s">
-        <v>558</v>
+        <v>567</v>
       </c>
       <c r="D201">
         <v>0</v>
@@ -7970,13 +8114,13 @@
     </row>
     <row r="202" spans="1:8">
       <c r="A202" t="s">
-        <v>559</v>
+        <v>568</v>
       </c>
       <c r="B202" t="s">
-        <v>560</v>
+        <v>569</v>
       </c>
       <c r="C202" t="s">
-        <v>561</v>
+        <v>570</v>
       </c>
       <c r="D202">
         <v>0</v>
@@ -7993,13 +8137,13 @@
     </row>
     <row r="203" spans="1:8">
       <c r="A203" t="s">
-        <v>562</v>
+        <v>571</v>
       </c>
       <c r="B203" t="s">
-        <v>563</v>
+        <v>572</v>
       </c>
       <c r="C203" t="s">
-        <v>564</v>
+        <v>573</v>
       </c>
       <c r="D203">
         <v>0</v>
@@ -8016,13 +8160,13 @@
     </row>
     <row r="204" spans="1:8">
       <c r="A204" t="s">
-        <v>565</v>
+        <v>574</v>
       </c>
       <c r="B204" t="s">
-        <v>566</v>
+        <v>575</v>
       </c>
       <c r="C204" t="s">
-        <v>567</v>
+        <v>576</v>
       </c>
       <c r="D204">
         <v>0</v>
@@ -8039,13 +8183,13 @@
     </row>
     <row r="205" spans="1:8">
       <c r="A205" t="s">
-        <v>568</v>
+        <v>577</v>
       </c>
       <c r="B205" t="s">
-        <v>569</v>
+        <v>578</v>
       </c>
       <c r="C205" t="s">
-        <v>570</v>
+        <v>579</v>
       </c>
       <c r="D205">
         <v>0</v>
@@ -8062,13 +8206,13 @@
     </row>
     <row r="206" spans="1:8">
       <c r="A206" t="s">
-        <v>571</v>
+        <v>580</v>
       </c>
       <c r="B206" t="s">
-        <v>572</v>
+        <v>581</v>
       </c>
       <c r="C206" t="s">
-        <v>573</v>
+        <v>582</v>
       </c>
       <c r="D206">
         <v>0</v>
@@ -8085,13 +8229,13 @@
     </row>
     <row r="207" spans="1:8">
       <c r="A207" t="s">
-        <v>574</v>
+        <v>583</v>
       </c>
       <c r="B207" t="s">
-        <v>572</v>
+        <v>581</v>
       </c>
       <c r="C207" t="s">
-        <v>573</v>
+        <v>582</v>
       </c>
       <c r="D207">
         <v>0</v>
@@ -8108,13 +8252,13 @@
     </row>
     <row r="208" spans="1:8">
       <c r="A208" t="s">
-        <v>575</v>
+        <v>584</v>
       </c>
       <c r="B208" t="s">
-        <v>576</v>
+        <v>585</v>
       </c>
       <c r="C208" t="s">
-        <v>577</v>
+        <v>586</v>
       </c>
       <c r="D208">
         <v>0</v>
@@ -8131,13 +8275,13 @@
     </row>
     <row r="209" spans="1:8">
       <c r="A209" t="s">
-        <v>578</v>
+        <v>587</v>
       </c>
       <c r="B209" t="s">
-        <v>579</v>
+        <v>588</v>
       </c>
       <c r="C209" t="s">
-        <v>580</v>
+        <v>589</v>
       </c>
       <c r="D209">
         <v>0</v>
@@ -8154,13 +8298,13 @@
     </row>
     <row r="210" spans="1:8">
       <c r="A210" t="s">
-        <v>581</v>
+        <v>590</v>
       </c>
       <c r="B210" t="s">
-        <v>582</v>
+        <v>591</v>
       </c>
       <c r="C210" t="s">
-        <v>583</v>
+        <v>592</v>
       </c>
       <c r="D210">
         <v>0</v>
@@ -8177,13 +8321,13 @@
     </row>
     <row r="211" spans="1:8">
       <c r="A211" t="s">
-        <v>584</v>
+        <v>593</v>
       </c>
       <c r="B211" t="s">
-        <v>585</v>
+        <v>594</v>
       </c>
       <c r="C211" t="s">
-        <v>585</v>
+        <v>594</v>
       </c>
       <c r="D211">
         <v>1</v>
@@ -8200,13 +8344,13 @@
     </row>
     <row r="212" spans="1:8">
       <c r="A212" t="s">
-        <v>586</v>
+        <v>595</v>
       </c>
       <c r="B212" t="s">
-        <v>587</v>
+        <v>596</v>
       </c>
       <c r="C212" t="s">
-        <v>587</v>
+        <v>596</v>
       </c>
       <c r="D212">
         <v>1</v>
@@ -8223,13 +8367,13 @@
     </row>
     <row r="213" spans="1:8">
       <c r="A213" t="s">
-        <v>588</v>
+        <v>597</v>
       </c>
       <c r="B213" t="s">
-        <v>589</v>
+        <v>598</v>
       </c>
       <c r="C213" t="s">
-        <v>590</v>
+        <v>599</v>
       </c>
       <c r="D213">
         <v>0</v>
@@ -8246,13 +8390,13 @@
     </row>
     <row r="214" spans="1:8">
       <c r="A214" t="s">
-        <v>591</v>
+        <v>600</v>
       </c>
       <c r="B214" t="s">
-        <v>592</v>
+        <v>601</v>
       </c>
       <c r="C214" t="s">
-        <v>592</v>
+        <v>601</v>
       </c>
       <c r="D214">
         <v>1</v>
@@ -8269,13 +8413,13 @@
     </row>
     <row r="215" spans="1:8">
       <c r="A215" t="s">
-        <v>593</v>
+        <v>602</v>
       </c>
       <c r="B215" t="s">
-        <v>594</v>
+        <v>603</v>
       </c>
       <c r="C215" t="s">
-        <v>595</v>
+        <v>604</v>
       </c>
       <c r="D215">
         <v>0</v>
@@ -8292,13 +8436,13 @@
     </row>
     <row r="216" spans="1:8">
       <c r="A216" t="s">
-        <v>596</v>
+        <v>605</v>
       </c>
       <c r="B216" t="s">
-        <v>597</v>
+        <v>606</v>
       </c>
       <c r="C216" t="s">
-        <v>597</v>
+        <v>606</v>
       </c>
       <c r="D216">
         <v>1</v>
@@ -8315,13 +8459,13 @@
     </row>
     <row r="217" spans="1:8">
       <c r="A217" t="s">
-        <v>598</v>
+        <v>607</v>
       </c>
       <c r="B217" t="s">
-        <v>599</v>
+        <v>608</v>
       </c>
       <c r="C217" t="s">
-        <v>600</v>
+        <v>609</v>
       </c>
       <c r="D217">
         <v>0</v>
@@ -8338,13 +8482,13 @@
     </row>
     <row r="218" spans="1:8">
       <c r="A218" t="s">
-        <v>601</v>
+        <v>610</v>
       </c>
       <c r="B218" t="s">
-        <v>602</v>
+        <v>611</v>
       </c>
       <c r="C218" t="s">
-        <v>602</v>
+        <v>611</v>
       </c>
       <c r="D218">
         <v>1</v>
@@ -8361,13 +8505,13 @@
     </row>
     <row r="219" spans="1:8">
       <c r="A219" t="s">
-        <v>603</v>
+        <v>612</v>
       </c>
       <c r="B219" t="s">
-        <v>604</v>
+        <v>613</v>
       </c>
       <c r="C219" t="s">
-        <v>604</v>
+        <v>613</v>
       </c>
       <c r="D219">
         <v>1</v>
@@ -8384,13 +8528,13 @@
     </row>
     <row r="220" spans="1:8">
       <c r="A220" t="s">
-        <v>605</v>
+        <v>614</v>
       </c>
       <c r="B220" t="s">
-        <v>606</v>
+        <v>615</v>
       </c>
       <c r="C220" t="s">
-        <v>606</v>
+        <v>615</v>
       </c>
       <c r="D220">
         <v>1</v>
@@ -8407,10 +8551,10 @@
     </row>
     <row r="221" spans="1:8">
       <c r="A221" t="s">
-        <v>607</v>
+        <v>616</v>
       </c>
       <c r="B221" t="s">
-        <v>608</v>
+        <v>617</v>
       </c>
       <c r="C221" t="s">
         <v>53</v>
@@ -8433,13 +8577,13 @@
     </row>
     <row r="222" spans="1:8">
       <c r="A222" t="s">
-        <v>609</v>
+        <v>618</v>
       </c>
       <c r="B222" t="s">
-        <v>610</v>
+        <v>619</v>
       </c>
       <c r="C222" t="s">
-        <v>611</v>
+        <v>620</v>
       </c>
       <c r="D222">
         <v>0</v>
@@ -8456,13 +8600,13 @@
     </row>
     <row r="223" spans="1:8">
       <c r="A223" t="s">
-        <v>612</v>
+        <v>621</v>
       </c>
       <c r="B223" t="s">
-        <v>613</v>
+        <v>622</v>
       </c>
       <c r="C223" t="s">
-        <v>614</v>
+        <v>623</v>
       </c>
       <c r="D223">
         <v>0</v>
@@ -8479,13 +8623,13 @@
     </row>
     <row r="224" spans="1:8">
       <c r="A224" t="s">
-        <v>615</v>
+        <v>624</v>
       </c>
       <c r="B224" t="s">
-        <v>616</v>
+        <v>625</v>
       </c>
       <c r="C224" t="s">
-        <v>617</v>
+        <v>626</v>
       </c>
       <c r="D224">
         <v>0</v>
@@ -8502,13 +8646,13 @@
     </row>
     <row r="225" spans="1:8">
       <c r="A225" t="s">
-        <v>618</v>
+        <v>627</v>
       </c>
       <c r="B225" t="s">
-        <v>619</v>
+        <v>628</v>
       </c>
       <c r="C225" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
       <c r="D225">
         <v>0</v>
@@ -8525,13 +8669,13 @@
     </row>
     <row r="226" spans="1:8">
       <c r="A226" t="s">
-        <v>621</v>
+        <v>630</v>
       </c>
       <c r="B226" t="s">
-        <v>622</v>
+        <v>631</v>
       </c>
       <c r="C226" t="s">
-        <v>623</v>
+        <v>632</v>
       </c>
       <c r="D226">
         <v>0</v>
@@ -8548,13 +8692,13 @@
     </row>
     <row r="227" spans="1:8">
       <c r="A227" t="s">
-        <v>624</v>
+        <v>633</v>
       </c>
       <c r="B227" t="s">
-        <v>625</v>
+        <v>634</v>
       </c>
       <c r="C227" t="s">
-        <v>626</v>
+        <v>635</v>
       </c>
       <c r="D227">
         <v>0</v>
@@ -8571,13 +8715,13 @@
     </row>
     <row r="228" spans="1:8">
       <c r="A228" t="s">
-        <v>627</v>
+        <v>636</v>
       </c>
       <c r="B228" t="s">
-        <v>628</v>
+        <v>637</v>
       </c>
       <c r="C228" t="s">
-        <v>629</v>
+        <v>638</v>
       </c>
       <c r="D228">
         <v>0</v>
@@ -8594,10 +8738,10 @@
     </row>
     <row r="229" spans="1:8">
       <c r="A229" t="s">
-        <v>630</v>
+        <v>639</v>
       </c>
       <c r="B229" t="s">
-        <v>631</v>
+        <v>640</v>
       </c>
       <c r="C229" t="s">
         <v>53</v>
@@ -8620,13 +8764,13 @@
     </row>
     <row r="230" spans="1:8">
       <c r="A230" t="s">
-        <v>632</v>
+        <v>641</v>
       </c>
       <c r="B230" t="s">
-        <v>633</v>
+        <v>642</v>
       </c>
       <c r="C230" t="s">
-        <v>634</v>
+        <v>643</v>
       </c>
       <c r="D230">
         <v>0</v>
@@ -8643,13 +8787,13 @@
     </row>
     <row r="231" spans="1:8">
       <c r="A231" t="s">
-        <v>635</v>
+        <v>644</v>
       </c>
       <c r="B231" t="s">
-        <v>636</v>
+        <v>645</v>
       </c>
       <c r="C231" t="s">
-        <v>637</v>
+        <v>646</v>
       </c>
       <c r="D231">
         <v>0</v>
@@ -8666,13 +8810,13 @@
     </row>
     <row r="232" spans="1:8">
       <c r="A232" t="s">
-        <v>638</v>
+        <v>647</v>
       </c>
       <c r="B232" t="s">
-        <v>639</v>
+        <v>648</v>
       </c>
       <c r="C232" t="s">
-        <v>640</v>
+        <v>649</v>
       </c>
       <c r="D232">
         <v>0</v>
@@ -8689,13 +8833,13 @@
     </row>
     <row r="233" spans="1:8">
       <c r="A233" t="s">
-        <v>641</v>
+        <v>650</v>
       </c>
       <c r="B233" t="s">
-        <v>642</v>
+        <v>651</v>
       </c>
       <c r="C233" t="s">
-        <v>643</v>
+        <v>652</v>
       </c>
       <c r="D233">
         <v>0</v>
@@ -8712,13 +8856,13 @@
     </row>
     <row r="234" spans="1:8">
       <c r="A234" t="s">
-        <v>644</v>
+        <v>653</v>
       </c>
       <c r="B234" t="s">
-        <v>645</v>
+        <v>654</v>
       </c>
       <c r="C234" t="s">
-        <v>646</v>
+        <v>655</v>
       </c>
       <c r="D234">
         <v>0</v>
@@ -8735,13 +8879,13 @@
     </row>
     <row r="235" spans="1:8">
       <c r="A235" t="s">
-        <v>647</v>
+        <v>656</v>
       </c>
       <c r="B235" t="s">
-        <v>648</v>
+        <v>657</v>
       </c>
       <c r="C235" t="s">
-        <v>649</v>
+        <v>658</v>
       </c>
       <c r="D235">
         <v>0</v>
@@ -8758,13 +8902,13 @@
     </row>
     <row r="236" spans="1:8">
       <c r="A236" t="s">
-        <v>650</v>
+        <v>659</v>
       </c>
       <c r="B236" t="s">
-        <v>651</v>
+        <v>660</v>
       </c>
       <c r="C236" t="s">
-        <v>652</v>
+        <v>661</v>
       </c>
       <c r="D236">
         <v>0</v>
@@ -8781,13 +8925,13 @@
     </row>
     <row r="237" spans="1:8">
       <c r="A237" t="s">
-        <v>653</v>
+        <v>662</v>
       </c>
       <c r="B237" t="s">
-        <v>654</v>
+        <v>663</v>
       </c>
       <c r="C237" t="s">
-        <v>655</v>
+        <v>664</v>
       </c>
       <c r="D237">
         <v>0</v>
@@ -8804,13 +8948,13 @@
     </row>
     <row r="238" spans="1:8">
       <c r="A238" t="s">
-        <v>656</v>
+        <v>665</v>
       </c>
       <c r="B238" t="s">
-        <v>657</v>
+        <v>666</v>
       </c>
       <c r="C238" t="s">
-        <v>658</v>
+        <v>667</v>
       </c>
       <c r="D238">
         <v>0</v>
@@ -8827,13 +8971,13 @@
     </row>
     <row r="239" spans="1:8">
       <c r="A239" t="s">
-        <v>659</v>
+        <v>668</v>
       </c>
       <c r="B239" t="s">
-        <v>660</v>
+        <v>669</v>
       </c>
       <c r="C239" t="s">
-        <v>661</v>
+        <v>670</v>
       </c>
       <c r="D239">
         <v>0</v>
@@ -8850,13 +8994,13 @@
     </row>
     <row r="240" spans="1:8">
       <c r="A240" t="s">
-        <v>662</v>
+        <v>671</v>
       </c>
       <c r="B240" t="s">
-        <v>663</v>
+        <v>672</v>
       </c>
       <c r="C240" t="s">
-        <v>664</v>
+        <v>673</v>
       </c>
       <c r="D240">
         <v>0</v>
@@ -8873,13 +9017,13 @@
     </row>
     <row r="241" spans="1:7">
       <c r="A241" t="s">
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="B241" t="s">
-        <v>666</v>
+        <v>675</v>
       </c>
       <c r="C241" t="s">
-        <v>667</v>
+        <v>676</v>
       </c>
       <c r="D241">
         <v>0</v>
@@ -8896,13 +9040,13 @@
     </row>
     <row r="242" spans="1:7">
       <c r="A242" t="s">
-        <v>668</v>
+        <v>677</v>
       </c>
       <c r="B242" t="s">
-        <v>669</v>
+        <v>678</v>
       </c>
       <c r="C242" t="s">
-        <v>670</v>
+        <v>679</v>
       </c>
       <c r="D242">
         <v>0</v>
@@ -8919,13 +9063,13 @@
     </row>
     <row r="243" spans="1:7">
       <c r="A243" t="s">
-        <v>671</v>
+        <v>680</v>
       </c>
       <c r="B243" t="s">
-        <v>672</v>
+        <v>681</v>
       </c>
       <c r="C243" t="s">
-        <v>673</v>
+        <v>682</v>
       </c>
       <c r="D243">
         <v>0</v>
@@ -8942,13 +9086,13 @@
     </row>
     <row r="244" spans="1:7">
       <c r="A244" t="s">
-        <v>674</v>
+        <v>683</v>
       </c>
       <c r="B244" t="s">
-        <v>675</v>
+        <v>684</v>
       </c>
       <c r="C244" t="s">
-        <v>676</v>
+        <v>685</v>
       </c>
       <c r="D244">
         <v>0</v>
@@ -8965,13 +9109,13 @@
     </row>
     <row r="245" spans="1:7">
       <c r="A245" t="s">
-        <v>677</v>
+        <v>686</v>
       </c>
       <c r="B245" t="s">
-        <v>678</v>
+        <v>687</v>
       </c>
       <c r="C245" t="s">
-        <v>679</v>
+        <v>688</v>
       </c>
       <c r="D245">
         <v>0</v>
@@ -8988,13 +9132,13 @@
     </row>
     <row r="246" spans="1:7">
       <c r="A246" t="s">
-        <v>680</v>
+        <v>689</v>
       </c>
       <c r="B246" t="s">
-        <v>681</v>
+        <v>690</v>
       </c>
       <c r="C246" t="s">
-        <v>682</v>
+        <v>691</v>
       </c>
       <c r="D246">
         <v>0</v>
@@ -9011,13 +9155,13 @@
     </row>
     <row r="247" spans="1:7">
       <c r="A247" t="s">
-        <v>683</v>
+        <v>692</v>
       </c>
       <c r="B247" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="C247" t="s">
-        <v>685</v>
+        <v>694</v>
       </c>
       <c r="D247">
         <v>0</v>
@@ -9034,13 +9178,13 @@
     </row>
     <row r="248" spans="1:7">
       <c r="A248" t="s">
-        <v>686</v>
+        <v>695</v>
       </c>
       <c r="B248" t="s">
-        <v>687</v>
+        <v>696</v>
       </c>
       <c r="C248" t="s">
-        <v>688</v>
+        <v>697</v>
       </c>
       <c r="D248">
         <v>0</v>
@@ -9057,13 +9201,13 @@
     </row>
     <row r="249" spans="1:7">
       <c r="A249" t="s">
-        <v>689</v>
+        <v>698</v>
       </c>
       <c r="B249" t="s">
-        <v>690</v>
+        <v>699</v>
       </c>
       <c r="C249" t="s">
-        <v>691</v>
+        <v>700</v>
       </c>
       <c r="D249">
         <v>0</v>
@@ -9080,13 +9224,13 @@
     </row>
     <row r="250" spans="1:7">
       <c r="A250" t="s">
-        <v>692</v>
+        <v>701</v>
       </c>
       <c r="B250" t="s">
-        <v>693</v>
+        <v>702</v>
       </c>
       <c r="C250" t="s">
-        <v>694</v>
+        <v>703</v>
       </c>
       <c r="D250">
         <v>0</v>
@@ -9103,13 +9247,13 @@
     </row>
     <row r="251" spans="1:7">
       <c r="A251" t="s">
-        <v>695</v>
+        <v>704</v>
       </c>
       <c r="B251" t="s">
-        <v>696</v>
+        <v>705</v>
       </c>
       <c r="C251" t="s">
-        <v>697</v>
+        <v>706</v>
       </c>
       <c r="D251">
         <v>0</v>
@@ -9126,13 +9270,13 @@
     </row>
     <row r="252" spans="1:7">
       <c r="A252" t="s">
-        <v>698</v>
+        <v>707</v>
       </c>
       <c r="B252" t="s">
-        <v>699</v>
+        <v>708</v>
       </c>
       <c r="C252" t="s">
-        <v>700</v>
+        <v>709</v>
       </c>
       <c r="D252">
         <v>0</v>
@@ -9149,13 +9293,13 @@
     </row>
     <row r="253" spans="1:7">
       <c r="A253" t="s">
-        <v>701</v>
+        <v>710</v>
       </c>
       <c r="B253" t="s">
-        <v>702</v>
+        <v>711</v>
       </c>
       <c r="C253" t="s">
-        <v>703</v>
+        <v>712</v>
       </c>
       <c r="D253">
         <v>0</v>
@@ -9172,13 +9316,13 @@
     </row>
     <row r="254" spans="1:7">
       <c r="A254" t="s">
-        <v>704</v>
+        <v>713</v>
       </c>
       <c r="B254" t="s">
-        <v>705</v>
+        <v>714</v>
       </c>
       <c r="C254" t="s">
-        <v>706</v>
+        <v>715</v>
       </c>
       <c r="D254">
         <v>0</v>
@@ -9195,13 +9339,13 @@
     </row>
     <row r="255" spans="1:7">
       <c r="A255" t="s">
-        <v>707</v>
+        <v>716</v>
       </c>
       <c r="B255" t="s">
-        <v>708</v>
+        <v>717</v>
       </c>
       <c r="C255" t="s">
-        <v>709</v>
+        <v>718</v>
       </c>
       <c r="D255">
         <v>0</v>
@@ -9218,13 +9362,13 @@
     </row>
     <row r="256" spans="1:7">
       <c r="A256" t="s">
-        <v>710</v>
+        <v>719</v>
       </c>
       <c r="B256" t="s">
-        <v>711</v>
+        <v>720</v>
       </c>
       <c r="C256" t="s">
-        <v>712</v>
+        <v>721</v>
       </c>
       <c r="D256">
         <v>0</v>
@@ -9241,13 +9385,13 @@
     </row>
     <row r="257" spans="1:7">
       <c r="A257" t="s">
-        <v>713</v>
+        <v>722</v>
       </c>
       <c r="B257" t="s">
-        <v>714</v>
+        <v>723</v>
       </c>
       <c r="C257" t="s">
-        <v>715</v>
+        <v>724</v>
       </c>
       <c r="D257">
         <v>0</v>
@@ -9264,13 +9408,13 @@
     </row>
     <row r="258" spans="1:7">
       <c r="A258" t="s">
-        <v>716</v>
+        <v>725</v>
       </c>
       <c r="B258" t="s">
-        <v>717</v>
+        <v>726</v>
       </c>
       <c r="C258" t="s">
-        <v>718</v>
+        <v>727</v>
       </c>
       <c r="D258">
         <v>0</v>
@@ -9287,13 +9431,13 @@
     </row>
     <row r="259" spans="1:7">
       <c r="A259" t="s">
-        <v>719</v>
+        <v>728</v>
       </c>
       <c r="B259" t="s">
-        <v>720</v>
+        <v>729</v>
       </c>
       <c r="C259" t="s">
-        <v>721</v>
+        <v>730</v>
       </c>
       <c r="D259">
         <v>0</v>
@@ -9310,13 +9454,13 @@
     </row>
     <row r="260" spans="1:7">
       <c r="A260" t="s">
-        <v>722</v>
+        <v>731</v>
       </c>
       <c r="B260" t="s">
-        <v>723</v>
+        <v>732</v>
       </c>
       <c r="C260" t="s">
-        <v>724</v>
+        <v>733</v>
       </c>
       <c r="D260">
         <v>0</v>
@@ -9333,13 +9477,13 @@
     </row>
     <row r="261" spans="1:7">
       <c r="A261" t="s">
-        <v>725</v>
+        <v>734</v>
       </c>
       <c r="B261" t="s">
-        <v>726</v>
+        <v>735</v>
       </c>
       <c r="C261" t="s">
-        <v>727</v>
+        <v>736</v>
       </c>
       <c r="D261">
         <v>0</v>
@@ -9356,13 +9500,13 @@
     </row>
     <row r="262" spans="1:7">
       <c r="A262" t="s">
-        <v>728</v>
+        <v>737</v>
       </c>
       <c r="B262" t="s">
-        <v>729</v>
+        <v>738</v>
       </c>
       <c r="C262" t="s">
-        <v>730</v>
+        <v>739</v>
       </c>
       <c r="D262">
         <v>0</v>
@@ -9379,13 +9523,13 @@
     </row>
     <row r="263" spans="1:7">
       <c r="A263" t="s">
-        <v>731</v>
+        <v>740</v>
       </c>
       <c r="B263" t="s">
-        <v>732</v>
+        <v>741</v>
       </c>
       <c r="C263" t="s">
-        <v>733</v>
+        <v>742</v>
       </c>
       <c r="D263">
         <v>0</v>
@@ -9402,13 +9546,13 @@
     </row>
     <row r="264" spans="1:7">
       <c r="A264" t="s">
-        <v>734</v>
+        <v>743</v>
       </c>
       <c r="B264" t="s">
-        <v>735</v>
+        <v>744</v>
       </c>
       <c r="C264" t="s">
-        <v>736</v>
+        <v>745</v>
       </c>
       <c r="D264">
         <v>0</v>
@@ -9425,13 +9569,13 @@
     </row>
     <row r="265" spans="1:7">
       <c r="A265" t="s">
-        <v>737</v>
+        <v>746</v>
       </c>
       <c r="B265" t="s">
-        <v>738</v>
+        <v>747</v>
       </c>
       <c r="C265" t="s">
-        <v>739</v>
+        <v>748</v>
       </c>
       <c r="D265">
         <v>0</v>
@@ -9448,13 +9592,13 @@
     </row>
     <row r="266" spans="1:7">
       <c r="A266" t="s">
-        <v>740</v>
+        <v>749</v>
       </c>
       <c r="B266" t="s">
-        <v>741</v>
+        <v>750</v>
       </c>
       <c r="C266" t="s">
-        <v>742</v>
+        <v>751</v>
       </c>
       <c r="D266">
         <v>0</v>
@@ -9471,13 +9615,13 @@
     </row>
     <row r="267" spans="1:7">
       <c r="A267" t="s">
-        <v>743</v>
+        <v>752</v>
       </c>
       <c r="B267" t="s">
-        <v>744</v>
+        <v>753</v>
       </c>
       <c r="C267" t="s">
-        <v>745</v>
+        <v>754</v>
       </c>
       <c r="D267">
         <v>0</v>
@@ -9494,13 +9638,13 @@
     </row>
     <row r="268" spans="1:7">
       <c r="A268" t="s">
-        <v>746</v>
+        <v>755</v>
       </c>
       <c r="B268" t="s">
-        <v>747</v>
+        <v>756</v>
       </c>
       <c r="C268" t="s">
-        <v>748</v>
+        <v>757</v>
       </c>
       <c r="D268">
         <v>0</v>
@@ -9517,13 +9661,13 @@
     </row>
     <row r="269" spans="1:7">
       <c r="A269" t="s">
-        <v>749</v>
+        <v>758</v>
       </c>
       <c r="B269" t="s">
-        <v>750</v>
+        <v>759</v>
       </c>
       <c r="C269" t="s">
-        <v>751</v>
+        <v>760</v>
       </c>
       <c r="D269">
         <v>0</v>
@@ -9540,13 +9684,13 @@
     </row>
     <row r="270" spans="1:7">
       <c r="A270" t="s">
-        <v>752</v>
+        <v>761</v>
       </c>
       <c r="B270" t="s">
-        <v>753</v>
+        <v>762</v>
       </c>
       <c r="C270" t="s">
-        <v>754</v>
+        <v>763</v>
       </c>
       <c r="D270">
         <v>0</v>
@@ -9563,13 +9707,13 @@
     </row>
     <row r="271" spans="1:7">
       <c r="A271" t="s">
-        <v>755</v>
+        <v>764</v>
       </c>
       <c r="B271" t="s">
-        <v>756</v>
+        <v>765</v>
       </c>
       <c r="C271" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="D271">
         <v>0</v>
@@ -9586,13 +9730,13 @@
     </row>
     <row r="272" spans="1:7">
       <c r="A272" t="s">
-        <v>758</v>
+        <v>767</v>
       </c>
       <c r="B272" t="s">
-        <v>759</v>
+        <v>768</v>
       </c>
       <c r="C272" t="s">
-        <v>760</v>
+        <v>769</v>
       </c>
       <c r="D272">
         <v>0</v>
@@ -9609,13 +9753,13 @@
     </row>
     <row r="273" spans="1:8">
       <c r="A273" t="s">
-        <v>761</v>
+        <v>770</v>
       </c>
       <c r="B273" t="s">
-        <v>762</v>
+        <v>771</v>
       </c>
       <c r="C273" t="s">
-        <v>763</v>
+        <v>772</v>
       </c>
       <c r="D273">
         <v>0</v>
@@ -9632,13 +9776,13 @@
     </row>
     <row r="274" spans="1:8">
       <c r="A274" t="s">
-        <v>764</v>
+        <v>773</v>
       </c>
       <c r="B274" t="s">
-        <v>765</v>
+        <v>774</v>
       </c>
       <c r="C274" t="s">
-        <v>766</v>
+        <v>775</v>
       </c>
       <c r="D274">
         <v>0</v>
@@ -9655,13 +9799,13 @@
     </row>
     <row r="275" spans="1:8">
       <c r="A275" t="s">
-        <v>767</v>
+        <v>776</v>
       </c>
       <c r="B275" t="s">
-        <v>768</v>
+        <v>777</v>
       </c>
       <c r="C275" t="s">
-        <v>769</v>
+        <v>778</v>
       </c>
       <c r="D275">
         <v>0</v>
@@ -9678,13 +9822,13 @@
     </row>
     <row r="276" spans="1:8">
       <c r="A276" t="s">
-        <v>770</v>
+        <v>779</v>
       </c>
       <c r="B276" t="s">
-        <v>771</v>
+        <v>780</v>
       </c>
       <c r="C276" t="s">
-        <v>772</v>
+        <v>781</v>
       </c>
       <c r="D276">
         <v>0</v>
@@ -9701,13 +9845,13 @@
     </row>
     <row r="277" spans="1:8">
       <c r="A277" t="s">
-        <v>773</v>
+        <v>782</v>
       </c>
       <c r="B277" t="s">
-        <v>774</v>
+        <v>783</v>
       </c>
       <c r="C277" t="s">
-        <v>775</v>
+        <v>784</v>
       </c>
       <c r="D277">
         <v>0</v>
@@ -9724,13 +9868,13 @@
     </row>
     <row r="278" spans="1:8">
       <c r="A278" t="s">
-        <v>776</v>
+        <v>785</v>
       </c>
       <c r="B278" t="s">
-        <v>777</v>
+        <v>786</v>
       </c>
       <c r="C278" t="s">
-        <v>778</v>
+        <v>787</v>
       </c>
       <c r="D278">
         <v>0</v>
@@ -9747,10 +9891,10 @@
     </row>
     <row r="279" spans="1:8">
       <c r="A279" t="s">
-        <v>779</v>
+        <v>788</v>
       </c>
       <c r="B279" t="s">
-        <v>780</v>
+        <v>789</v>
       </c>
       <c r="C279" t="s">
         <v>53</v>
@@ -9773,13 +9917,13 @@
     </row>
     <row r="280" spans="1:8">
       <c r="A280" t="s">
-        <v>781</v>
+        <v>790</v>
       </c>
       <c r="B280" t="s">
-        <v>782</v>
+        <v>791</v>
       </c>
       <c r="C280" t="s">
-        <v>783</v>
+        <v>792</v>
       </c>
       <c r="D280">
         <v>0</v>
@@ -9796,13 +9940,13 @@
     </row>
     <row r="281" spans="1:8">
       <c r="A281" t="s">
-        <v>784</v>
+        <v>793</v>
       </c>
       <c r="B281" t="s">
-        <v>785</v>
+        <v>794</v>
       </c>
       <c r="C281" t="s">
-        <v>786</v>
+        <v>795</v>
       </c>
       <c r="D281">
         <v>0</v>
@@ -9819,13 +9963,13 @@
     </row>
     <row r="282" spans="1:8">
       <c r="A282" t="s">
-        <v>787</v>
+        <v>796</v>
       </c>
       <c r="B282" t="s">
-        <v>788</v>
+        <v>797</v>
       </c>
       <c r="C282" t="s">
-        <v>789</v>
+        <v>798</v>
       </c>
       <c r="D282">
         <v>0</v>
@@ -9842,13 +9986,13 @@
     </row>
     <row r="283" spans="1:8">
       <c r="A283" t="s">
-        <v>790</v>
+        <v>799</v>
       </c>
       <c r="B283" t="s">
-        <v>791</v>
+        <v>800</v>
       </c>
       <c r="C283" t="s">
-        <v>792</v>
+        <v>801</v>
       </c>
       <c r="D283">
         <v>0</v>
@@ -9865,13 +10009,13 @@
     </row>
     <row r="284" spans="1:8">
       <c r="A284" t="s">
-        <v>793</v>
+        <v>802</v>
       </c>
       <c r="B284" t="s">
-        <v>794</v>
+        <v>803</v>
       </c>
       <c r="C284" t="s">
-        <v>795</v>
+        <v>804</v>
       </c>
       <c r="D284">
         <v>0</v>
@@ -9888,13 +10032,13 @@
     </row>
     <row r="285" spans="1:8">
       <c r="A285" t="s">
-        <v>796</v>
+        <v>805</v>
       </c>
       <c r="B285" t="s">
-        <v>797</v>
+        <v>806</v>
       </c>
       <c r="C285" t="s">
-        <v>798</v>
+        <v>807</v>
       </c>
       <c r="D285">
         <v>0</v>
@@ -9911,13 +10055,13 @@
     </row>
     <row r="286" spans="1:8">
       <c r="A286" t="s">
-        <v>799</v>
+        <v>808</v>
       </c>
       <c r="B286" t="s">
-        <v>800</v>
+        <v>809</v>
       </c>
       <c r="C286" t="s">
-        <v>801</v>
+        <v>810</v>
       </c>
       <c r="D286">
         <v>0</v>
@@ -9934,13 +10078,13 @@
     </row>
     <row r="287" spans="1:8">
       <c r="A287" t="s">
-        <v>802</v>
+        <v>811</v>
       </c>
       <c r="B287" t="s">
-        <v>803</v>
+        <v>812</v>
       </c>
       <c r="C287" t="s">
-        <v>804</v>
+        <v>813</v>
       </c>
       <c r="D287">
         <v>0</v>
@@ -9957,13 +10101,13 @@
     </row>
     <row r="288" spans="1:8">
       <c r="A288" t="s">
-        <v>805</v>
+        <v>814</v>
       </c>
       <c r="B288" t="s">
-        <v>806</v>
+        <v>815</v>
       </c>
       <c r="C288" t="s">
-        <v>807</v>
+        <v>816</v>
       </c>
       <c r="D288">
         <v>0</v>
@@ -9980,10 +10124,10 @@
     </row>
     <row r="289" spans="1:8">
       <c r="A289" t="s">
-        <v>808</v>
+        <v>817</v>
       </c>
       <c r="B289" t="s">
-        <v>809</v>
+        <v>818</v>
       </c>
       <c r="C289" t="s">
         <v>53</v>
@@ -10006,13 +10150,13 @@
     </row>
     <row r="290" spans="1:8">
       <c r="A290" t="s">
-        <v>810</v>
+        <v>819</v>
       </c>
       <c r="B290" t="s">
-        <v>811</v>
+        <v>820</v>
       </c>
       <c r="C290" t="s">
-        <v>812</v>
+        <v>821</v>
       </c>
       <c r="D290">
         <v>0</v>
@@ -10029,13 +10173,13 @@
     </row>
     <row r="291" spans="1:8">
       <c r="A291" t="s">
-        <v>813</v>
+        <v>822</v>
       </c>
       <c r="B291" t="s">
-        <v>814</v>
+        <v>823</v>
       </c>
       <c r="C291" t="s">
-        <v>815</v>
+        <v>824</v>
       </c>
       <c r="D291">
         <v>0</v>
@@ -10052,13 +10196,13 @@
     </row>
     <row r="292" spans="1:8">
       <c r="A292" t="s">
-        <v>816</v>
+        <v>825</v>
       </c>
       <c r="B292" t="s">
-        <v>817</v>
+        <v>826</v>
       </c>
       <c r="C292" t="s">
-        <v>818</v>
+        <v>827</v>
       </c>
       <c r="D292">
         <v>0</v>
@@ -10075,13 +10219,13 @@
     </row>
     <row r="293" spans="1:8">
       <c r="A293" t="s">
-        <v>819</v>
+        <v>828</v>
       </c>
       <c r="B293" t="s">
-        <v>820</v>
+        <v>829</v>
       </c>
       <c r="C293" t="s">
-        <v>820</v>
+        <v>829</v>
       </c>
       <c r="D293">
         <v>1</v>
@@ -10098,13 +10242,13 @@
     </row>
     <row r="294" spans="1:8">
       <c r="A294" t="s">
-        <v>821</v>
+        <v>830</v>
       </c>
       <c r="B294" t="s">
-        <v>822</v>
+        <v>831</v>
       </c>
       <c r="C294" t="s">
-        <v>823</v>
+        <v>832</v>
       </c>
       <c r="D294">
         <v>0</v>
@@ -10121,13 +10265,13 @@
     </row>
     <row r="295" spans="1:8">
       <c r="A295" t="s">
-        <v>824</v>
+        <v>833</v>
       </c>
       <c r="B295" t="s">
-        <v>825</v>
+        <v>834</v>
       </c>
       <c r="C295" t="s">
-        <v>826</v>
+        <v>835</v>
       </c>
       <c r="D295">
         <v>0</v>
@@ -10144,13 +10288,13 @@
     </row>
     <row r="296" spans="1:8">
       <c r="A296" t="s">
-        <v>827</v>
+        <v>836</v>
       </c>
       <c r="B296" t="s">
-        <v>828</v>
+        <v>837</v>
       </c>
       <c r="C296" t="s">
-        <v>829</v>
+        <v>838</v>
       </c>
       <c r="D296">
         <v>0</v>
@@ -10167,10 +10311,10 @@
     </row>
     <row r="297" spans="1:8">
       <c r="A297" t="s">
-        <v>830</v>
+        <v>839</v>
       </c>
       <c r="B297" t="s">
-        <v>831</v>
+        <v>840</v>
       </c>
       <c r="C297" t="s">
         <v>53</v>
@@ -10193,13 +10337,13 @@
     </row>
     <row r="298" spans="1:8">
       <c r="A298" t="s">
-        <v>832</v>
+        <v>841</v>
       </c>
       <c r="B298" t="s">
-        <v>833</v>
+        <v>842</v>
       </c>
       <c r="C298" t="s">
-        <v>834</v>
+        <v>843</v>
       </c>
       <c r="D298">
         <v>0</v>
@@ -10216,10 +10360,10 @@
     </row>
     <row r="299" spans="1:8">
       <c r="A299" t="s">
-        <v>835</v>
+        <v>844</v>
       </c>
       <c r="B299" t="s">
-        <v>836</v>
+        <v>845</v>
       </c>
       <c r="C299" t="s">
         <v>53</v>
@@ -10242,13 +10386,13 @@
     </row>
     <row r="300" spans="1:8">
       <c r="A300" t="s">
-        <v>837</v>
+        <v>846</v>
       </c>
       <c r="B300" t="s">
-        <v>838</v>
+        <v>847</v>
       </c>
       <c r="C300" t="s">
-        <v>839</v>
+        <v>848</v>
       </c>
       <c r="D300">
         <v>0</v>
@@ -10265,13 +10409,13 @@
     </row>
     <row r="301" spans="1:8">
       <c r="A301" t="s">
-        <v>840</v>
+        <v>849</v>
       </c>
       <c r="B301" t="s">
-        <v>841</v>
+        <v>850</v>
       </c>
       <c r="C301" t="s">
-        <v>842</v>
+        <v>851</v>
       </c>
       <c r="D301">
         <v>0</v>
@@ -10288,10 +10432,10 @@
     </row>
     <row r="302" spans="1:8">
       <c r="A302" t="s">
-        <v>843</v>
+        <v>852</v>
       </c>
       <c r="B302" t="s">
-        <v>844</v>
+        <v>853</v>
       </c>
       <c r="C302" t="s">
         <v>53</v>
@@ -10314,13 +10458,13 @@
     </row>
     <row r="303" spans="1:8">
       <c r="A303" t="s">
-        <v>845</v>
+        <v>854</v>
       </c>
       <c r="B303" t="s">
-        <v>846</v>
+        <v>855</v>
       </c>
       <c r="C303" t="s">
-        <v>847</v>
+        <v>856</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -10337,13 +10481,13 @@
     </row>
     <row r="304" spans="1:8">
       <c r="A304" t="s">
-        <v>848</v>
+        <v>857</v>
       </c>
       <c r="B304" t="s">
-        <v>849</v>
+        <v>858</v>
       </c>
       <c r="C304" t="s">
-        <v>850</v>
+        <v>859</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -10360,13 +10504,13 @@
     </row>
     <row r="305" spans="1:8">
       <c r="A305" t="s">
-        <v>851</v>
+        <v>860</v>
       </c>
       <c r="B305" t="s">
-        <v>852</v>
+        <v>861</v>
       </c>
       <c r="C305" t="s">
-        <v>853</v>
+        <v>862</v>
       </c>
       <c r="D305">
         <v>0</v>
@@ -10383,13 +10527,13 @@
     </row>
     <row r="306" spans="1:8">
       <c r="A306" t="s">
-        <v>854</v>
+        <v>863</v>
       </c>
       <c r="B306" t="s">
-        <v>855</v>
+        <v>864</v>
       </c>
       <c r="C306" t="s">
-        <v>856</v>
+        <v>865</v>
       </c>
       <c r="D306">
         <v>0</v>
@@ -10406,13 +10550,13 @@
     </row>
     <row r="307" spans="1:8">
       <c r="A307" t="s">
-        <v>857</v>
+        <v>866</v>
       </c>
       <c r="B307" t="s">
-        <v>858</v>
+        <v>867</v>
       </c>
       <c r="C307" t="s">
-        <v>859</v>
+        <v>868</v>
       </c>
       <c r="D307">
         <v>0</v>
@@ -10429,13 +10573,13 @@
     </row>
     <row r="308" spans="1:8">
       <c r="A308" t="s">
-        <v>860</v>
+        <v>869</v>
       </c>
       <c r="B308" t="s">
-        <v>861</v>
+        <v>870</v>
       </c>
       <c r="C308" t="s">
-        <v>862</v>
+        <v>871</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -10452,13 +10596,13 @@
     </row>
     <row r="309" spans="1:8">
       <c r="A309" t="s">
-        <v>863</v>
+        <v>872</v>
       </c>
       <c r="B309" t="s">
-        <v>864</v>
+        <v>873</v>
       </c>
       <c r="C309" t="s">
-        <v>865</v>
+        <v>874</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -10475,10 +10619,10 @@
     </row>
     <row r="310" spans="1:8">
       <c r="A310" t="s">
-        <v>866</v>
+        <v>875</v>
       </c>
       <c r="B310" t="s">
-        <v>867</v>
+        <v>876</v>
       </c>
       <c r="C310" t="s">
         <v>53</v>
@@ -10501,13 +10645,13 @@
     </row>
     <row r="311" spans="1:8">
       <c r="A311" t="s">
-        <v>868</v>
+        <v>877</v>
       </c>
       <c r="B311" t="s">
-        <v>869</v>
+        <v>878</v>
       </c>
       <c r="C311" t="s">
-        <v>870</v>
+        <v>879</v>
       </c>
       <c r="D311">
         <v>0</v>
@@ -10524,13 +10668,13 @@
     </row>
     <row r="312" spans="1:8">
       <c r="A312" t="s">
-        <v>871</v>
+        <v>880</v>
       </c>
       <c r="B312" t="s">
-        <v>872</v>
+        <v>881</v>
       </c>
       <c r="C312" t="s">
-        <v>873</v>
+        <v>882</v>
       </c>
       <c r="D312">
         <v>0</v>
@@ -10547,13 +10691,13 @@
     </row>
     <row r="313" spans="1:8">
       <c r="A313" t="s">
-        <v>874</v>
+        <v>883</v>
       </c>
       <c r="B313" t="s">
-        <v>875</v>
+        <v>884</v>
       </c>
       <c r="C313" t="s">
-        <v>876</v>
+        <v>885</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -10570,13 +10714,13 @@
     </row>
     <row r="314" spans="1:8">
       <c r="A314" t="s">
-        <v>877</v>
+        <v>886</v>
       </c>
       <c r="B314" t="s">
-        <v>878</v>
+        <v>887</v>
       </c>
       <c r="C314" t="s">
-        <v>879</v>
+        <v>888</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -10593,13 +10737,13 @@
     </row>
     <row r="315" spans="1:8">
       <c r="A315" t="s">
-        <v>880</v>
+        <v>889</v>
       </c>
       <c r="B315" t="s">
-        <v>881</v>
+        <v>890</v>
       </c>
       <c r="C315" t="s">
-        <v>882</v>
+        <v>891</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -10616,13 +10760,13 @@
     </row>
     <row r="316" spans="1:8">
       <c r="A316" t="s">
-        <v>883</v>
+        <v>892</v>
       </c>
       <c r="B316" t="s">
-        <v>884</v>
+        <v>893</v>
       </c>
       <c r="C316" t="s">
-        <v>885</v>
+        <v>894</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -10639,13 +10783,13 @@
     </row>
     <row r="317" spans="1:8">
       <c r="A317" t="s">
-        <v>886</v>
+        <v>895</v>
       </c>
       <c r="B317" t="s">
-        <v>887</v>
+        <v>896</v>
       </c>
       <c r="C317" t="s">
-        <v>888</v>
+        <v>897</v>
       </c>
       <c r="D317">
         <v>0</v>
@@ -10662,13 +10806,13 @@
     </row>
     <row r="318" spans="1:8">
       <c r="A318" t="s">
-        <v>889</v>
+        <v>898</v>
       </c>
       <c r="B318" t="s">
-        <v>890</v>
+        <v>899</v>
       </c>
       <c r="C318" t="s">
-        <v>891</v>
+        <v>900</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -10685,13 +10829,13 @@
     </row>
     <row r="319" spans="1:8">
       <c r="A319" t="s">
-        <v>892</v>
+        <v>901</v>
       </c>
       <c r="B319" t="s">
-        <v>893</v>
+        <v>902</v>
       </c>
       <c r="C319" t="s">
-        <v>894</v>
+        <v>903</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -10708,13 +10852,13 @@
     </row>
     <row r="320" spans="1:8">
       <c r="A320" t="s">
-        <v>895</v>
+        <v>904</v>
       </c>
       <c r="B320" t="s">
-        <v>896</v>
+        <v>905</v>
       </c>
       <c r="C320" t="s">
-        <v>897</v>
+        <v>906</v>
       </c>
       <c r="D320">
         <v>0</v>
@@ -10731,13 +10875,13 @@
     </row>
     <row r="321" spans="1:7">
       <c r="A321" t="s">
-        <v>898</v>
+        <v>907</v>
       </c>
       <c r="B321" t="s">
-        <v>899</v>
+        <v>908</v>
       </c>
       <c r="C321" t="s">
-        <v>900</v>
+        <v>909</v>
       </c>
       <c r="D321">
         <v>0</v>
@@ -10754,13 +10898,13 @@
     </row>
     <row r="322" spans="1:7">
       <c r="A322" t="s">
-        <v>901</v>
+        <v>910</v>
       </c>
       <c r="B322" t="s">
-        <v>902</v>
+        <v>911</v>
       </c>
       <c r="C322" t="s">
-        <v>903</v>
+        <v>912</v>
       </c>
       <c r="D322">
         <v>0</v>
@@ -10777,13 +10921,13 @@
     </row>
     <row r="323" spans="1:7">
       <c r="A323" t="s">
-        <v>904</v>
+        <v>913</v>
       </c>
       <c r="B323" t="s">
-        <v>905</v>
+        <v>914</v>
       </c>
       <c r="C323" t="s">
-        <v>906</v>
+        <v>915</v>
       </c>
       <c r="D323">
         <v>0</v>
@@ -10800,13 +10944,13 @@
     </row>
     <row r="324" spans="1:7">
       <c r="A324" t="s">
-        <v>907</v>
+        <v>916</v>
       </c>
       <c r="B324" t="s">
-        <v>908</v>
+        <v>917</v>
       </c>
       <c r="C324" t="s">
-        <v>909</v>
+        <v>918</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -10823,13 +10967,13 @@
     </row>
     <row r="325" spans="1:7">
       <c r="A325" t="s">
-        <v>910</v>
+        <v>919</v>
       </c>
       <c r="B325" t="s">
-        <v>911</v>
+        <v>920</v>
       </c>
       <c r="C325" t="s">
-        <v>912</v>
+        <v>921</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -10846,13 +10990,13 @@
     </row>
     <row r="326" spans="1:7">
       <c r="A326" t="s">
-        <v>913</v>
+        <v>922</v>
       </c>
       <c r="B326" t="s">
-        <v>914</v>
+        <v>923</v>
       </c>
       <c r="C326" t="s">
-        <v>914</v>
+        <v>923</v>
       </c>
       <c r="D326">
         <v>1</v>
@@ -10869,13 +11013,13 @@
     </row>
     <row r="327" spans="1:7">
       <c r="A327" t="s">
-        <v>915</v>
+        <v>924</v>
       </c>
       <c r="B327" t="s">
-        <v>916</v>
+        <v>925</v>
       </c>
       <c r="C327" t="s">
-        <v>917</v>
+        <v>926</v>
       </c>
       <c r="D327">
         <v>0</v>

</xml_diff>

<commit_message>
Aggiunte nuove analisi a CodeGPT
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/AnalisiCodeGPT.xlsx
+++ b/HE/W_in_progress/AnalisiCodeGPT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BD4C6E2-73BB-421E-85BD-A6B4966594FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{95340D39-3610-42DF-A9C8-691BBBF39B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="927">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="969">
   <si>
     <t>IN</t>
   </si>
@@ -1266,6 +1266,9 @@
     <t>component clock_mod8 port ( clock : in STD_LOGIC; reset : in STD_LOGIC; enable : in STD_LOGIC; counter : out STD_LOGIC_VECTOR (2 downto 0); enable_count : out STD_LOGIC_VECTOR (3 downto 0)); end component;</t>
   </si>
   <si>
+    <t>Parametro in più ma va bene</t>
+  </si>
+  <si>
     <t>component abox is made up of data_in as input std_logic_vector of 4 bit and data_out as output std_logic_vector of 4 bit</t>
   </si>
   <si>
@@ -1287,6 +1290,9 @@
     <t>component cathodes_manager port ( dot : in STD_LOGIC_VECTOR (3 downto 0); cathodes_dot : out STD_LOGIC_VECTOR (7 downto 0)); end component;</t>
   </si>
   <si>
+    <t>Manca un parametro</t>
+  </si>
+  <si>
     <t>input_handler is a component with generic COUNT_MAX of type integer with default 500000, with signals row_sel, clk, reset as input std_logic_vector and std_logic signals respectively, key_out, col_sel, keypress_out as output std_logic_vector signals</t>
   </si>
   <si>
@@ -1314,6 +1320,9 @@
     <t>component read_pointer port ( rptr : in STD_LOGIC_VECTOR (2 downto 0); fifo_rd : out STD_LOGIC_VECTOR (2 downto 0)); fifo_rd &lt;= rptr(0); fifo_rd &lt;= fifo_rd(0); clk : in STD</t>
   </si>
   <si>
+    <t>I parametri sono sbagliati</t>
+  </si>
+  <si>
     <t>ROM is a component with RST, ADDR and DATA signals as described.</t>
   </si>
   <si>
@@ -1338,6 +1347,9 @@
     <t>button_debouncer_plaintext_btn: button_debouncer port map(clk_period =&gt; 10, btn_noise_time =&gt; 10000000, rst, clock, btn_plainText_in, t_btn_plainText);</t>
   </si>
   <si>
+    <t>Non fa l'stanziazione a button_dbouncer</t>
+  </si>
+  <si>
     <t>uut is an instance of Riconoscitore_Mealy with signal i mapped to signal i, CLK mapped to CLK, RST mapped to RST, Y mapped to Y</t>
   </si>
   <si>
@@ -1389,6 +1401,9 @@
     <t>myFA: myFA port map(OP_A =&gt; OP_A_RCA, OP_B =&gt; OP_B_RCA, CIN =&gt; CIN_RCA, S =&gt; S_int, COUT =&gt; cout_int);</t>
   </si>
   <si>
+    <t>I vettori non sono indicizzati</t>
+  </si>
+  <si>
     <t>debouncer is an instance of ButtonDebouncer with generics CLK_period set to 10, btn_noise_time set to 10000000, RST signal mapped to reset_n, CLK signal mapped to clock_in, BTN signal mapped to addr_strobe_in, CLEARED_BTN signal mapped to read_strobe</t>
   </si>
   <si>
@@ -1452,6 +1467,9 @@
     <t>constant constant x : std_logic_vector(6 downto 0) := "1000000";</t>
   </si>
   <si>
+    <t>Nome sbaliato ma va bene</t>
+  </si>
+  <si>
     <t>define a constant called TbClockB of type time initialized to 40 ns</t>
   </si>
   <si>
@@ -1491,6 +1509,9 @@
     <t>constant s : time := 550 ns; constant s : std_logic_vector(DAC_D_OUT_LEN - 1 downto 0);</t>
   </si>
   <si>
+    <t>Nome sbaliato e codice in più ma va bene</t>
+  </si>
+  <si>
     <t>Define a constant named TbClockB with type time and initialize to 40 ns</t>
   </si>
   <si>
@@ -1521,6 +1542,9 @@
     <t>for i in 0 to 4 generate inst_IDDR : IDDR generic(i) port(i) port(Q1 : in STD_LOGIC; Q2 : in STD_LOGIC; C : in STD_LOGIC; CE : in STD_LOGIC; D : in STD_LOGIC; R : in STD_LOGIC; S : in STD_LOGIC; I : in STD_LOGIC; O : in STD_LOGIC); end generate;</t>
   </si>
   <si>
+    <t>Non fa tutte le inizializzazioni</t>
+  </si>
+  <si>
     <t>gen_num is a for generate statement on variable N over LOOP_COUNT range that generates component rd_gen_inst2 that is an instance of fifo_rng with generic signals WIDTH initialized to 8, SEED initialized to TB_SEED+N and port signals CLK initialized to RD_CLK, RESET initialized to RESET, RANDOM_NUM initialized to elements of rand_num with indices from 8*(N+1)-1 down to 8*N, ENABLE initialized to pr_r_en</t>
   </si>
   <si>
@@ -1536,6 +1560,9 @@
     <t>signal round_keys: array (0 to 3) of dataArrayType;</t>
   </si>
   <si>
+    <t>Sbagliato</t>
+  </si>
+  <si>
     <t>Declare type hsv_function as an array with 256 elements of integer data type</t>
   </si>
   <si>
@@ -1545,6 +1572,9 @@
     <t>type hsv_function is array (0 to 255) of integer range 0 to 255;</t>
   </si>
   <si>
+    <t>Mette il range, ma va bene</t>
+  </si>
+  <si>
     <t>define an array type xhdl_17 with 64 elements of type std_logic</t>
   </si>
   <si>
@@ -1554,6 +1584,9 @@
     <t>type xhdl_17 is array (0 to 63) of std_logic_vector(31 downto 0);</t>
   </si>
   <si>
+    <t xml:space="preserve">Dichiara praticamente una matrice </t>
+  </si>
+  <si>
     <t>define an array hsv_function of 256 bit of integer</t>
   </si>
   <si>
@@ -1569,6 +1602,9 @@
     <t>outrotl(7 downto 1) &lt;= outrotl(6 downto 0) &amp; portArotl(7 downto 0) &amp; portArotl(7 downto 1);</t>
   </si>
   <si>
+    <t>non ho richiesto la AND</t>
+  </si>
+  <si>
     <t>access and display the fourth element of an array named x</t>
   </si>
   <si>
@@ -1602,6 +1638,9 @@
     <t>signal clock_multiplier : integer range 0 to 10000000;</t>
   </si>
   <si>
+    <t>Non ho chiesto un range</t>
+  </si>
+  <si>
     <t>the element of memory_ram with index address_a converted into n unsigned, increased by index and than converted into a standard integer, is set equal to he elements of data_in_a from the indices ((ram_word_size)*(index + 1) - 1) to ((ram_word_size)*index)</t>
   </si>
   <si>
@@ -1611,6 +1650,9 @@
     <t>memory_ram(index) &lt;= data_in_a(index - 1 downto 0);</t>
   </si>
   <si>
+    <t>Non fa le conversioni</t>
+  </si>
+  <si>
     <t>Create a 32x32 memory array matrix_mem, define a 32-bit signal row_data, and assign the contents of the 25th row of matrix_mem to row_data</t>
   </si>
   <si>
@@ -1629,6 +1671,9 @@
     <t>addr &lt;= ADR_I(10 downto 0) &amp; ADR_I(0) &amp; ADR_I(1);</t>
   </si>
   <si>
+    <t>Non ho chiesto una AND</t>
+  </si>
+  <si>
     <t>Define a 168-bit signal data_block, create a 21-bit signal eighth, and set eighth to bits 125 downto 105 of data_block</t>
   </si>
   <si>
@@ -1647,6 +1692,9 @@
     <t>ram_font: in std_logic_vector(unsigned(font_address)) port map(to_integer(unsigned(font_address)) =&gt; integer(font_width), to_integer(unsigned(font_address)) =&gt; integer(font_size));</t>
   </si>
   <si>
+    <t>Non fa l'assegnazione</t>
+  </si>
+  <si>
     <t>Define a 256-bit signal mega_packet, create a 64-bit signal quarter, and set quarter to bits 191 downto 128 of mega_packet</t>
   </si>
   <si>
@@ -1692,6 +1740,9 @@
     <t>shifted_data &lt;= data_in when shift_amount = "000", data_in when shift_amount = "001" else data_in(6 downto 0) &amp; '0' when shift_amount = "010" else data_in(5 downto 0) &amp; "00" when shift_amount = "011" else "----";</t>
   </si>
   <si>
+    <t>Ci sono delle And non richieste</t>
+  </si>
+  <si>
     <t>Use selected signal assignment to set signal y to '1000' when signal a is '00', '0100' when signal a is '01', '0010' when signal a is '10', and '0001' when signal a is '11'. Otherwise, set y to all don't care.</t>
   </si>
   <si>
@@ -1710,6 +1761,9 @@
     <t>clk_out &lt;= clk_in when clk_div_sel = "00", clk_div2 when clk_div_sel = "01", clk_div4 when clk_div_sel = "10", clk_div8;</t>
   </si>
   <si>
+    <t>Errori sintattici, ma idea buona</t>
+  </si>
+  <si>
     <t>Ensure 'data_valid' is never high when 'clock_enable' is low</t>
   </si>
   <si>
@@ -1728,6 +1782,9 @@
     <t>if rising_edge(clk) then if enable = '1' then output &lt;= '0'; else output &lt;= '1'; end if; end if;</t>
   </si>
   <si>
+    <t>Non fa l'assertion</t>
+  </si>
+  <si>
     <t>Ensure 'reset' pulse width is at least 10 ns</t>
   </si>
   <si>
@@ -1782,6 +1839,9 @@
     <t>entity half_adder is port ( A : in STD_LOGIC; B : in STD_LOGIC; Carry_In : in STD_LOGIC; Carry_Out : out STD_LOGIC; Carry_Out_nxt : out STD_LOGIC); end half_adder;</t>
   </si>
   <si>
+    <t>Roba in più però va bene</t>
+  </si>
+  <si>
     <t>define the entity of the half adder</t>
   </si>
   <si>
@@ -1794,6 +1854,9 @@
     <t>component multiplexer port (left_in : in STD_LOGIC; right_in : in STD_LOGIC; y : out STD_LOGIC); end component;</t>
   </si>
   <si>
+    <t>Ci può stare</t>
+  </si>
+  <si>
     <t>define the entity of a decoder with two inputs and 4 outputs</t>
   </si>
   <si>
@@ -1803,6 +1866,9 @@
     <t>entity decoder is port (a0 : in STD_LOGIC; a1 : in STD_LOGIC; y : out STD_LOGIC); end decoder;</t>
   </si>
   <si>
+    <t>non ci sono i 4 output</t>
+  </si>
+  <si>
     <t>define the entity for a multiplier 8 bit</t>
   </si>
   <si>
@@ -1812,6 +1878,9 @@
     <t>entity multiplier_8_out is port(clk : in STD_LOGIC; rst : in STD_LOGIC; enable : in STD_LOGIC; multiplier64 : in STD_LOGIC_VECTOR (7 downto 0); multiplier64_out : out STD_LOGIC_VECTOR (7 downto 0)); end multiplier_8_out;; entity multiplier64_out64 is port(clk, rst, enable, multiplier6464 : in STD_LOGIC_VECTOR (7 downto 0)); end multiplier64_8_out64;; end entity;</t>
   </si>
   <si>
+    <t>Non è il moltiplicatore che ho chiesto</t>
+  </si>
+  <si>
     <t>define the variable size of type integer with values from 10 to 10000 and initialize it to 1000</t>
   </si>
   <si>
@@ -1848,6 +1917,9 @@
     <t>SampledBits &lt;= SampledBits(SampledBits'length - 2 downto 0) &amp; RxD_i;</t>
   </si>
   <si>
+    <t>Più o meno ci sta</t>
+  </si>
+  <si>
     <t>right shift by 1 bit i_data_5_out and add the value of i_data_0</t>
   </si>
   <si>
@@ -1914,6 +1986,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity glitch_filter is Port ( Noise_In : in STD_LOGIC; Filtered_Out : out STD_LOGIC); end glitch_filter; architecture Behavioral of glitch_filter is signal noisy_in : STD_LOGIC := '0'; begin process (Noise_In) begin if rising_edge(Noise_In) then filtered_out &lt;= noisy_in; end if ; end process ; Filtered_Out &lt;= filtered_out; end Behavioral;</t>
   </si>
   <si>
+    <t>Più o meno c'è l'idea</t>
+  </si>
+  <si>
     <t>Implement a basic moving average filter with circular buffer</t>
   </si>
   <si>
@@ -1923,6 +1998,9 @@
     <t>process(clk) begin if rising_edge(clk) then if rst = '1' then sum &lt;= sum - buffer; else sum &lt;= sum + buffer; end if; end if; end process;</t>
   </si>
   <si>
+    <t>Non realizza una media mobile</t>
+  </si>
+  <si>
     <t>Implement a Manchester decoder using a process.</t>
   </si>
   <si>
@@ -1932,6 +2010,9 @@
     <t>process(clk) begin if rising_edge(clk) then if rst = '1' then if count = 0 then count &lt;= 0; else count &lt;= count + 1; end if; end if; end process;</t>
   </si>
   <si>
+    <t>Non è un  Manchester decoder</t>
+  </si>
+  <si>
     <t>Define a register of N-bit with the signals clock, reset, enable, and D (N-bit) as input and the signal Q (N-bit) as output.</t>
   </si>
   <si>
@@ -1941,6 +2022,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity register_n is Generic (N : natural := 8); Port ( Clock : in STD_LOGIC; Reset : in STD_LOGIC; Enable : in STD_LOGIC; D : in STD_LOGIC_VECTOR (N-1 downto 0); Q : out STD_LOGIC_VECTOR (N-1 downto 0)); end register_n; architecture Behavioral of register_n is signal reg : std_logic_vector(N-1 downto 0); begin process (Clock, Reset) begin if Reset = '1' then reg &lt;= (others =&gt; '0'); elsif rising_edge(Clock) then if Enable = '1' then reg &lt;= reg(N-2 downto 0) &amp; reg(N-1); elsif D = '1' then reg &lt;= reg(N-3 downto 0) &amp; reg(N-2); end if ; end if ; end process ; Q &lt;= reg; end Behavioral;</t>
   </si>
   <si>
+    <t>Un po ambiguo ma attinente</t>
+  </si>
+  <si>
     <t>Create a simple 4-bit comparator</t>
   </si>
   <si>
@@ -1950,6 +2034,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity 4-BitComparator is Generic(Bitwidth-1 downto 0); Port ( A : in STD_LOGIC_VECTOR (Bitwidth-1 downto 0); B : in STD_LOGIC_VECTOR (Bitwidth-1 downto 0); C : in STD_LOGIC_VECTOR (Bitwidth-1 downto 0); Sum : out STD_LOGIC_VECTOR (Bitwidth-1 downto 0); Carry_Out : out STD_LOGIC); end 4-BitComparator; architecture Behavioral of 4-BitComparator is begin process (A, B, C) variable carry : std_logic := '0'; begin if (A = '1') then Sum &lt;= '0'; Carry_Out &lt;= '1'; elsif (B = '1') then Sum &lt;= '1'; Carry_Out &lt;= '0'; elsif (C = '1') then Sum &lt;= '0'; Carry_Out &lt;= '1'; elsif (C = '0') then Sum &lt;= '0'; Carry_Out &lt;= '0'; else Sum &lt;= '1'; Carry_Out &lt;= '0'; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non è un comparatore</t>
+  </si>
+  <si>
     <t>Implement an SPI slave using a process.</t>
   </si>
   <si>
@@ -1965,6 +2052,9 @@
     <t>process(clk,rst)begin if rst='1'then count&lt;=0;elsif rising_edge(clk)then count&lt;=count+1;end if;end process;</t>
   </si>
   <si>
+    <t>Frequency counter, un po strano, ma frequency counter</t>
+  </si>
+  <si>
     <t>Write a parallel to serial converter of N-bit with the signals clk, parallel_in (N-bit), and load_en as input and the signal serial_out as output.</t>
   </si>
   <si>
@@ -1992,6 +2082,9 @@
     <t>process(clk) begin if rising_edge(clk) then if rst = '1' then memory_out &lt;= memory_in; elsif write = '1' then memory_out &lt;= memory_out + memory_in; end if; end if; end process;</t>
   </si>
   <si>
+    <t>Fa solo accumuli, non esegue operazioni di memoria</t>
+  </si>
+  <si>
     <t>Define a frequency divider with the signals clock, reset, and divide_ratio (N-bit) as input and the signal divided_clock as output.</t>
   </si>
   <si>
@@ -2001,6 +2094,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity FrequencyDivider is Generic(N : natural := 8); Port ( Clock : in STD_LOGIC; Reset : in STD_LOGIC; Divide_Ratio : in STD_LOGIC_VECTOR (N-1 downto 0); Divided_Clock : out STD_LOGIC); end FrequencyDivider; architecture Behavioral of FrequencyDivider is signal divided_clock, divided_reset : STD_LOGIC; begin process (Clock, Reset) begin if Reset = '1' then divided_clock &lt;= Clock; divided_reset &lt;= '0'; elsif rising_edge(Clock) then divided_clock &lt;= Clock(N-1); divided_reset &lt;= '0'; end if ; end process ; Divided_Reset &lt;= divided_reset; end Behavioral;</t>
   </si>
   <si>
+    <t>Non fa il divisore di frequenza</t>
+  </si>
+  <si>
     <t>Create a basic SPI (Serial Peripheral Interface) master with multiple slave select</t>
   </si>
   <si>
@@ -2010,6 +2106,9 @@
     <t>process(clk) begin if rising_edge(clk) then if rst = '1' then data_out &lt;= '0'; elsif enable = '1' then data_out &lt;= data_out + data_out - 1; end if; end if; end process;</t>
   </si>
   <si>
+    <t>Non gestisce il protocollo SPI</t>
+  </si>
+  <si>
     <t>Create a basic PWM (Pulse Width Modulation) generator with variable frequency</t>
   </si>
   <si>
@@ -2019,6 +2118,9 @@
     <t>process(clk) begin if rising_edge(clk) then if rst = '1' then pwm &lt;= '1'; elsif duty_cycle = 5 ns then pwm &lt;= '0'; end if; end if; end process;</t>
   </si>
   <si>
+    <t>Non ha logica sul duty cycle</t>
+  </si>
+  <si>
     <t>Generate a CRC checker of N-bit with the signals data_in (N-bit), received_CRC (M-bit), and polynomial (M-bit) as input and the signal CRC_match as output.</t>
   </si>
   <si>
@@ -2028,6 +2130,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity CRC_checker is Generic (N : natural := 8); Port ( Data_In : in STD_LOGIC_VECTOR (N-1 downto 0); Received_CRC : in STD_LOGIC_VECTOR (M-1 downto 0); Polynomial : in STD_LOGIC_VECTOR (M-1 downto 0); CRC_Match : out STD_LOGIC); end CRC_checker; architecture Behavioral of CRC_checker is begin process (Data_In, Received_CRC, Polynomial) variable temp : STD_LOGIC_VECTOR (N-1 downto 0); begin temp := Data_In; for i in 0 to N-1 loop temp(i) := received_CRC(i); if temp(i) = '1' then CRC_Match := '1'; else CRC_Match := '0'; end if ; end loop ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non fa una verifica sul CRC</t>
+  </si>
+  <si>
     <t>Define a fixed-point divider of N-bit with the signals dividend (N-bit) and divisor (N-bit) as input and the signals quotient (N-bit) and remainder (N-bit) as output.</t>
   </si>
   <si>
@@ -2037,6 +2142,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity fixed_point_divider is Generic (N : natural := 8); Port (Dividend : in signed(N-1 downto 0); Divisor : in signed(N-1 downto 0); Quotient : out signed(N-1 downto 0)); end fixed_point_divider; architecture Behavioral of fixed_point_divider is signal quotient : unsigned(N-1 downto 0); signal remainder : unsigned(N-1 downto 0); begin process (Dividend, Divisor) begin if dividend = '1' then quotient &lt;= 0; remainder &lt;= 0; elsif divisor = '1' then quotient &lt;= quotient + 1; remainder &lt;= remainder + 1; end if ; end process ; Quotient &lt;= quotient; Remainder &lt;= remainder; end Behavioral;</t>
   </si>
   <si>
+    <t>Non effettua una divisione</t>
+  </si>
+  <si>
     <t>Write a 2-bit magnitude comparator with the signals A1, A0, B1, and B0 as input and the signals A_greater, A_equal, and A_smaller as output.</t>
   </si>
   <si>
@@ -2046,6 +2154,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity magnitude_comparator is Port ( A1 : in STD_LOGIC; A0 : in STD_LOGIC; B1 : in STD_LOGIC; B0 : in STD_LOGIC; A_greater : out STD_LOGIC; A_equal : out STD_LOGIC; A_smaller : out STD_LOGIC); end magnitude_comparator; architecture Behavioral of magnitude_comparator is begin process (A1, A0, B1, B0) variable temp : STD_LOGIC; begin temp := A1; temp := A0; if (A_greater = '1') then temp := A0; elsif (A_equal = '1') then temp := A1; else temp := A0; end if ; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non effettua il confronto</t>
+  </si>
+  <si>
     <t>Write a binary to gray converter of N-bit with the signal binary (N-bit) as input and the signal gray_code (N-bit) as output.</t>
   </si>
   <si>
@@ -2055,6 +2166,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity gray_to_gray is Generic (N : natural := 8); Port ( Binary : in STD_LOGIC_VECTOR (N-1 downto 0); Gray_Code : out STD_LOGIC_VECTOR (N-1 downto 0)); end gray_to_gray; architecture Behavioral of gray_to_gray is begin process (Binary) variable gray_code : std_logic_vector(N-1 downto 0); begin gray_code := binary(N); gray_code := gray_code(N); end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non vi è la logica di conversione</t>
+  </si>
+  <si>
     <t>Implement a basic quadrature encoder interface</t>
   </si>
   <si>
@@ -2064,6 +2178,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity basic_quadrature_encoder is Port ( Clock : in STD_LOGIC; Reset : in STD_LOGIC; Shift_Register : in STD_LOGIC; Shift_Value : out STD_LOGIC_VECTOR (7 downto 0)); end basic_quadrature_encoder; architecture Behavioral of basic_quadrature_encoder is begin process (Clock, Reset) variable shift_reg : std_logic_vector(7 downto 0); begin if (Reset = '1') then shift_reg &lt;= (others =&gt; '0'); elsif (rising_edge(Clock)) then shift_reg &lt;= (others =&gt; '0'); elsif (rising_edge(Reset)) then shift_reg &lt;= (others =&gt; '0'); end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non è un quadrature encoder</t>
+  </si>
+  <si>
     <t>Define a debouncer with the signal noisy_button as input and the signal clean_button_pulse as output.</t>
   </si>
   <si>
@@ -2073,6 +2190,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity debouncer is Port ( noisy_button : in STD_LOGIC; clean_button_pulse : out STD_LOGIC); end debouncer; architecture Behavioral of debouncer is begin process (noisy_button) variable temp : STD_LOGIC := '0'; begin if (noisy_button = '1') then temp := '1'; elsif (rising_edge(noisy_button)) then temp := '0'; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non è un debouncer</t>
+  </si>
+  <si>
     <t>Define a Johnson ring counter of N-bit with the signals clock and reset as input and the signal count (N-bit) as output.</t>
   </si>
   <si>
@@ -2082,6 +2202,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity JohnsonRingCounter is Generic(N : natural := 8); Port ( Clock : in STD_LOGIC; Reset : in STD_LOGIC; Count : out STD_LOGIC_VECTOR (N-1 downto 0)); end JohnsonRingCounter; architecture Behavioral of JohnsonRingCounter is signal count : std_logic_vector(N-1 downto 0); begin process (Clock, Reset) begin if Reset = '1' then count &lt;= (others =&gt; '0'); elsif rising_edge(Clock) then if Count = '1' then count &lt;= count + 1; end if ; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Può andare</t>
+  </si>
+  <si>
     <t>Define a pulse generator circuit with the signals clk, reset, and pulse_width (N-bit) as input and the signal pulse_out as output.</t>
   </si>
   <si>
@@ -2797,6 +2920,9 @@
   </si>
   <si>
     <t>scl_en_i : t_scl; entity Encoder_onBoard is port(switch : in STD_LOGIC_VECTOR(9 downto 0); led : out STD_LOGIC_VECTOR(3 downto 0); catodi : out STD_LOGIC_VECTOR(7 downto 0)); end Encoder_onBoard;</t>
+  </si>
+  <si>
+    <t>Mancano gli anodi e sbagliata l'assegnazione</t>
   </si>
   <si>
     <t>set i_cs_re_tk to '1' when i_cs_cpy signal is '0' and i_cs signal is '1', otherwise set it to '0'; define a variable named limit of type integer with range 0 to 255, then initialize it to 255</t>
@@ -3184,8 +3310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="G142" sqref="G142"/>
+    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
+      <selection activeCell="H245" sqref="H245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6754,18 +6880,21 @@
         <v>0.84267290900735303</v>
       </c>
       <c r="G143">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H143" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="144" spans="1:8">
       <c r="A144" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B144" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C144" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D144">
         <v>0</v>
@@ -6782,10 +6911,10 @@
     </row>
     <row r="145" spans="1:8">
       <c r="A145" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B145" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C145" t="s">
         <v>53</v>
@@ -6808,13 +6937,13 @@
     </row>
     <row r="146" spans="1:8">
       <c r="A146" t="s">
+        <v>417</v>
+      </c>
+      <c r="B146" t="s">
         <v>416</v>
       </c>
-      <c r="B146" t="s">
-        <v>415</v>
-      </c>
       <c r="C146" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D146">
         <v>0</v>
@@ -6828,16 +6957,19 @@
       <c r="G146">
         <v>0</v>
       </c>
+      <c r="H146" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="147" spans="1:8">
       <c r="A147" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B147" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C147" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="D147">
         <v>0</v>
@@ -6851,16 +6983,19 @@
       <c r="G147">
         <v>0</v>
       </c>
+      <c r="H147" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="148" spans="1:8">
       <c r="A148" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B148" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="C148" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D148">
         <v>0</v>
@@ -6874,16 +7009,19 @@
       <c r="G148">
         <v>0</v>
       </c>
+      <c r="H148" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="149" spans="1:8">
       <c r="A149" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B149" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="C149" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="D149">
         <v>0</v>
@@ -6897,16 +7035,19 @@
       <c r="G149">
         <v>0</v>
       </c>
+      <c r="H149" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="150" spans="1:8">
       <c r="A150" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="B150" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="C150" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="D150">
         <v>0</v>
@@ -6920,13 +7061,16 @@
       <c r="G150">
         <v>0</v>
       </c>
+      <c r="H150" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="151" spans="1:8">
       <c r="A151" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="B151" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C151" t="s">
         <v>53</v>
@@ -6949,13 +7093,13 @@
     </row>
     <row r="152" spans="1:8">
       <c r="A152" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="B152" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C152" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="D152">
         <v>0</v>
@@ -6969,16 +7113,19 @@
       <c r="G152">
         <v>0</v>
       </c>
+      <c r="H152" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="153" spans="1:8">
       <c r="A153" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="B153" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="C153" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="D153">
         <v>0</v>
@@ -6992,16 +7139,19 @@
       <c r="G153">
         <v>0</v>
       </c>
+      <c r="H153" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="154" spans="1:8">
       <c r="A154" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="B154" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="C154" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="D154">
         <v>0</v>
@@ -7013,18 +7163,21 @@
         <v>0.75595238095238104</v>
       </c>
       <c r="G154">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H154" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="155" spans="1:8">
       <c r="A155" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="B155" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="C155" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="D155">
         <v>0</v>
@@ -7036,15 +7189,15 @@
         <v>0.94106158088235292</v>
       </c>
       <c r="G155">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:8">
       <c r="A156" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="B156" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="C156" t="s">
         <v>53</v>
@@ -7067,13 +7220,13 @@
     </row>
     <row r="157" spans="1:8">
       <c r="A157" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="B157" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="C157" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="D157">
         <v>0</v>
@@ -7085,18 +7238,21 @@
         <v>0.8829428067523305</v>
       </c>
       <c r="G157">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H157" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="158" spans="1:8">
       <c r="A158" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="B158" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="C158" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="D158">
         <v>0</v>
@@ -7110,16 +7266,19 @@
       <c r="G158">
         <v>0</v>
       </c>
+      <c r="H158" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="159" spans="1:8">
       <c r="A159" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="B159" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c r="C159" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="D159">
         <v>0</v>
@@ -7133,16 +7292,19 @@
       <c r="G159">
         <v>0</v>
       </c>
+      <c r="H159" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="160" spans="1:8">
       <c r="A160" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="B160" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="C160" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="D160">
         <v>0</v>
@@ -7156,16 +7318,19 @@
       <c r="G160">
         <v>0</v>
       </c>
+      <c r="H160" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="161" spans="1:8">
       <c r="A161" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="B161" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="C161" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="D161">
         <v>0</v>
@@ -7177,18 +7342,18 @@
         <v>0.82942097026604067</v>
       </c>
       <c r="G161">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:8">
       <c r="A162" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="B162" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="C162" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="D162">
         <v>1</v>
@@ -7205,13 +7370,13 @@
     </row>
     <row r="163" spans="1:8">
       <c r="A163" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="B163" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="C163" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="D163">
         <v>0</v>
@@ -7225,13 +7390,16 @@
       <c r="G163">
         <v>0</v>
       </c>
+      <c r="H163" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="164" spans="1:8">
       <c r="A164" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="B164" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="C164" t="s">
         <v>53</v>
@@ -7254,10 +7422,10 @@
     </row>
     <row r="165" spans="1:8">
       <c r="A165" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="B165" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="C165" t="s">
         <v>53</v>
@@ -7280,13 +7448,13 @@
     </row>
     <row r="166" spans="1:8">
       <c r="A166" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="B166" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="C166" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="D166">
         <v>0</v>
@@ -7298,18 +7466,21 @@
         <v>0.92580078388971487</v>
       </c>
       <c r="G166">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H166" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="167" spans="1:8">
       <c r="A167" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="B167" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="C167" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="D167">
         <v>0</v>
@@ -7321,18 +7492,21 @@
         <v>0.5066964285714286</v>
       </c>
       <c r="G167">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H167" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="168" spans="1:8">
       <c r="A168" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B168" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="C168" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="D168">
         <v>1</v>
@@ -7349,13 +7523,13 @@
     </row>
     <row r="169" spans="1:8">
       <c r="A169" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="B169" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="C169" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="D169">
         <v>0</v>
@@ -7369,16 +7543,19 @@
       <c r="G169">
         <v>0</v>
       </c>
+      <c r="H169" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="170" spans="1:8">
       <c r="A170" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="B170" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="C170" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="D170">
         <v>1</v>
@@ -7395,13 +7572,13 @@
     </row>
     <row r="171" spans="1:8">
       <c r="A171" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="B171" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="C171" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="D171">
         <v>0</v>
@@ -7413,18 +7590,21 @@
         <v>0.61887254901960786</v>
       </c>
       <c r="G171">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H171" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="172" spans="1:8">
       <c r="A172" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="B172" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="C172" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="D172">
         <v>0</v>
@@ -7436,18 +7616,21 @@
         <v>0.58796296296296291</v>
       </c>
       <c r="G172">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H172" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="173" spans="1:8">
       <c r="A173" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="B173" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="C173" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="D173">
         <v>1</v>
@@ -7464,13 +7647,13 @@
     </row>
     <row r="174" spans="1:8">
       <c r="A174" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="B174" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
       <c r="C174" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="D174">
         <v>0</v>
@@ -7482,18 +7665,18 @@
         <v>0.93197278911564618</v>
       </c>
       <c r="G174">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:8">
       <c r="A175" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="B175" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="C175" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="D175">
         <v>0</v>
@@ -7507,16 +7690,19 @@
       <c r="G175">
         <v>0</v>
       </c>
+      <c r="H175" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="176" spans="1:8">
       <c r="A176" t="s">
-        <v>496</v>
+        <v>504</v>
       </c>
       <c r="B176" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="C176" t="s">
-        <v>498</v>
+        <v>506</v>
       </c>
       <c r="D176">
         <v>0</v>
@@ -7530,16 +7716,19 @@
       <c r="G176">
         <v>0</v>
       </c>
-    </row>
-    <row r="177" spans="1:7">
+      <c r="H176" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8">
       <c r="A177" t="s">
-        <v>499</v>
+        <v>507</v>
       </c>
       <c r="B177" t="s">
         <v>135</v>
       </c>
       <c r="C177" t="s">
-        <v>500</v>
+        <v>508</v>
       </c>
       <c r="D177">
         <v>0</v>
@@ -7553,16 +7742,19 @@
       <c r="G177">
         <v>0</v>
       </c>
-    </row>
-    <row r="178" spans="1:7">
+      <c r="H177" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8">
       <c r="A178" t="s">
-        <v>501</v>
+        <v>510</v>
       </c>
       <c r="B178" t="s">
-        <v>502</v>
+        <v>511</v>
       </c>
       <c r="C178" t="s">
-        <v>503</v>
+        <v>512</v>
       </c>
       <c r="D178">
         <v>0</v>
@@ -7574,18 +7766,21 @@
         <v>0.94982078853046592</v>
       </c>
       <c r="G178">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="179" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H178" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8">
       <c r="A179" t="s">
-        <v>504</v>
+        <v>514</v>
       </c>
       <c r="B179" t="s">
-        <v>505</v>
+        <v>515</v>
       </c>
       <c r="C179" t="s">
-        <v>506</v>
+        <v>516</v>
       </c>
       <c r="D179">
         <v>0</v>
@@ -7599,16 +7794,19 @@
       <c r="G179">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:7">
+      <c r="H179" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8">
       <c r="A180" t="s">
-        <v>507</v>
+        <v>518</v>
       </c>
       <c r="B180" t="s">
-        <v>502</v>
+        <v>511</v>
       </c>
       <c r="C180" t="s">
-        <v>508</v>
+        <v>519</v>
       </c>
       <c r="D180">
         <v>0</v>
@@ -7620,18 +7818,21 @@
         <v>0.57736280487804881</v>
       </c>
       <c r="G180">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H180" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8">
       <c r="A181" t="s">
-        <v>509</v>
+        <v>520</v>
       </c>
       <c r="B181" t="s">
-        <v>510</v>
+        <v>521</v>
       </c>
       <c r="C181" t="s">
-        <v>511</v>
+        <v>522</v>
       </c>
       <c r="D181">
         <v>0</v>
@@ -7645,16 +7846,19 @@
       <c r="G181">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:7">
+      <c r="H181" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8">
       <c r="A182" t="s">
-        <v>512</v>
+        <v>524</v>
       </c>
       <c r="B182" t="s">
-        <v>513</v>
+        <v>525</v>
       </c>
       <c r="C182" t="s">
-        <v>514</v>
+        <v>526</v>
       </c>
       <c r="D182">
         <v>0</v>
@@ -7668,16 +7872,19 @@
       <c r="G182">
         <v>0</v>
       </c>
-    </row>
-    <row r="183" spans="1:7">
+      <c r="H182" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8">
       <c r="A183" t="s">
-        <v>515</v>
+        <v>527</v>
       </c>
       <c r="B183" t="s">
-        <v>516</v>
+        <v>528</v>
       </c>
       <c r="C183" t="s">
-        <v>516</v>
+        <v>528</v>
       </c>
       <c r="D183">
         <v>1</v>
@@ -7692,15 +7899,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:8">
       <c r="A184" t="s">
-        <v>517</v>
+        <v>529</v>
       </c>
       <c r="B184" t="s">
-        <v>518</v>
+        <v>530</v>
       </c>
       <c r="C184" t="s">
-        <v>519</v>
+        <v>531</v>
       </c>
       <c r="D184">
         <v>0</v>
@@ -7714,16 +7921,19 @@
       <c r="G184">
         <v>0</v>
       </c>
-    </row>
-    <row r="185" spans="1:7">
+      <c r="H184" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8">
       <c r="A185" t="s">
-        <v>520</v>
+        <v>532</v>
       </c>
       <c r="B185" t="s">
-        <v>521</v>
+        <v>533</v>
       </c>
       <c r="C185" t="s">
-        <v>522</v>
+        <v>534</v>
       </c>
       <c r="D185">
         <v>0</v>
@@ -7737,16 +7947,19 @@
       <c r="G185">
         <v>0</v>
       </c>
-    </row>
-    <row r="186" spans="1:7">
+      <c r="H185" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8">
       <c r="A186" t="s">
-        <v>523</v>
+        <v>536</v>
       </c>
       <c r="B186" t="s">
-        <v>524</v>
+        <v>537</v>
       </c>
       <c r="C186" t="s">
-        <v>525</v>
+        <v>538</v>
       </c>
       <c r="D186">
         <v>0</v>
@@ -7760,16 +7973,19 @@
       <c r="G186">
         <v>0</v>
       </c>
-    </row>
-    <row r="187" spans="1:7">
+      <c r="H186" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8">
       <c r="A187" t="s">
-        <v>526</v>
+        <v>540</v>
       </c>
       <c r="B187" t="s">
-        <v>527</v>
+        <v>541</v>
       </c>
       <c r="C187" t="s">
-        <v>528</v>
+        <v>542</v>
       </c>
       <c r="D187">
         <v>0</v>
@@ -7783,16 +7999,19 @@
       <c r="G187">
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="1:7">
+      <c r="H187" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8">
       <c r="A188" t="s">
-        <v>529</v>
+        <v>543</v>
       </c>
       <c r="B188" t="s">
-        <v>530</v>
+        <v>544</v>
       </c>
       <c r="C188" t="s">
-        <v>531</v>
+        <v>545</v>
       </c>
       <c r="D188">
         <v>0</v>
@@ -7806,16 +8025,19 @@
       <c r="G188">
         <v>0</v>
       </c>
-    </row>
-    <row r="189" spans="1:7">
+      <c r="H188" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8">
       <c r="A189" t="s">
-        <v>532</v>
+        <v>547</v>
       </c>
       <c r="B189" t="s">
-        <v>533</v>
+        <v>548</v>
       </c>
       <c r="C189" t="s">
-        <v>534</v>
+        <v>549</v>
       </c>
       <c r="D189">
         <v>0</v>
@@ -7827,18 +8049,18 @@
         <v>0.95918875251342128</v>
       </c>
       <c r="G189">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8">
       <c r="A190" t="s">
-        <v>535</v>
+        <v>550</v>
       </c>
       <c r="B190" t="s">
-        <v>536</v>
+        <v>551</v>
       </c>
       <c r="C190" t="s">
-        <v>537</v>
+        <v>552</v>
       </c>
       <c r="D190">
         <v>0</v>
@@ -7852,16 +8074,19 @@
       <c r="G190">
         <v>0</v>
       </c>
-    </row>
-    <row r="191" spans="1:7">
+      <c r="H190" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8">
       <c r="A191" t="s">
-        <v>538</v>
+        <v>554</v>
       </c>
       <c r="B191" t="s">
-        <v>539</v>
+        <v>555</v>
       </c>
       <c r="C191" t="s">
-        <v>539</v>
+        <v>555</v>
       </c>
       <c r="D191">
         <v>1</v>
@@ -7876,15 +8101,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:8">
       <c r="A192" t="s">
-        <v>540</v>
+        <v>556</v>
       </c>
       <c r="B192" t="s">
-        <v>541</v>
+        <v>557</v>
       </c>
       <c r="C192" t="s">
-        <v>542</v>
+        <v>558</v>
       </c>
       <c r="D192">
         <v>0</v>
@@ -7896,15 +8121,15 @@
         <v>0.93275935374149654</v>
       </c>
       <c r="G192">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193" spans="1:8">
       <c r="A193" t="s">
-        <v>543</v>
+        <v>559</v>
       </c>
       <c r="B193" t="s">
-        <v>544</v>
+        <v>560</v>
       </c>
       <c r="C193" t="s">
         <v>53</v>
@@ -7927,13 +8152,13 @@
     </row>
     <row r="194" spans="1:8">
       <c r="A194" t="s">
-        <v>545</v>
+        <v>561</v>
       </c>
       <c r="B194" t="s">
-        <v>546</v>
+        <v>562</v>
       </c>
       <c r="C194" t="s">
-        <v>547</v>
+        <v>563</v>
       </c>
       <c r="D194">
         <v>0</v>
@@ -7945,15 +8170,15 @@
         <v>0.96408975112678819</v>
       </c>
       <c r="G194">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:8">
       <c r="A195" t="s">
-        <v>548</v>
+        <v>564</v>
       </c>
       <c r="B195" t="s">
-        <v>549</v>
+        <v>565</v>
       </c>
       <c r="C195" t="s">
         <v>53</v>
@@ -7976,13 +8201,13 @@
     </row>
     <row r="196" spans="1:8">
       <c r="A196" t="s">
-        <v>550</v>
+        <v>566</v>
       </c>
       <c r="B196" t="s">
-        <v>551</v>
+        <v>567</v>
       </c>
       <c r="C196" t="s">
-        <v>552</v>
+        <v>568</v>
       </c>
       <c r="D196">
         <v>0</v>
@@ -7996,16 +8221,19 @@
       <c r="G196">
         <v>0</v>
       </c>
+      <c r="H196" t="s">
+        <v>569</v>
+      </c>
     </row>
     <row r="197" spans="1:8">
       <c r="A197" t="s">
-        <v>553</v>
+        <v>570</v>
       </c>
       <c r="B197" t="s">
-        <v>554</v>
+        <v>571</v>
       </c>
       <c r="C197" t="s">
-        <v>555</v>
+        <v>572</v>
       </c>
       <c r="D197">
         <v>0</v>
@@ -8019,16 +8247,19 @@
       <c r="G197">
         <v>0</v>
       </c>
+      <c r="H197" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="198" spans="1:8">
       <c r="A198" t="s">
-        <v>556</v>
+        <v>573</v>
       </c>
       <c r="B198" t="s">
-        <v>557</v>
+        <v>574</v>
       </c>
       <c r="C198" t="s">
-        <v>558</v>
+        <v>575</v>
       </c>
       <c r="D198">
         <v>0</v>
@@ -8040,18 +8271,21 @@
         <v>0.81297573151443236</v>
       </c>
       <c r="G198">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H198" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="199" spans="1:8">
       <c r="A199" t="s">
-        <v>559</v>
+        <v>577</v>
       </c>
       <c r="B199" t="s">
-        <v>560</v>
+        <v>578</v>
       </c>
       <c r="C199" t="s">
-        <v>561</v>
+        <v>579</v>
       </c>
       <c r="D199">
         <v>0</v>
@@ -8065,16 +8299,19 @@
       <c r="G199">
         <v>0</v>
       </c>
+      <c r="H199" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="200" spans="1:8">
       <c r="A200" t="s">
-        <v>562</v>
+        <v>580</v>
       </c>
       <c r="B200" t="s">
-        <v>563</v>
+        <v>581</v>
       </c>
       <c r="C200" t="s">
-        <v>564</v>
+        <v>582</v>
       </c>
       <c r="D200">
         <v>0</v>
@@ -8088,16 +8325,19 @@
       <c r="G200">
         <v>0</v>
       </c>
+      <c r="H200" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="201" spans="1:8">
       <c r="A201" t="s">
-        <v>565</v>
+        <v>584</v>
       </c>
       <c r="B201" t="s">
-        <v>566</v>
+        <v>585</v>
       </c>
       <c r="C201" t="s">
-        <v>567</v>
+        <v>586</v>
       </c>
       <c r="D201">
         <v>0</v>
@@ -8111,16 +8351,19 @@
       <c r="G201">
         <v>0</v>
       </c>
+      <c r="H201" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="202" spans="1:8">
       <c r="A202" t="s">
-        <v>568</v>
+        <v>587</v>
       </c>
       <c r="B202" t="s">
-        <v>569</v>
+        <v>588</v>
       </c>
       <c r="C202" t="s">
-        <v>570</v>
+        <v>589</v>
       </c>
       <c r="D202">
         <v>0</v>
@@ -8134,16 +8377,19 @@
       <c r="G202">
         <v>0</v>
       </c>
+      <c r="H202" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="203" spans="1:8">
       <c r="A203" t="s">
-        <v>571</v>
+        <v>590</v>
       </c>
       <c r="B203" t="s">
-        <v>572</v>
+        <v>591</v>
       </c>
       <c r="C203" t="s">
-        <v>573</v>
+        <v>592</v>
       </c>
       <c r="D203">
         <v>0</v>
@@ -8157,16 +8403,19 @@
       <c r="G203">
         <v>0</v>
       </c>
+      <c r="H203" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="204" spans="1:8">
       <c r="A204" t="s">
-        <v>574</v>
+        <v>593</v>
       </c>
       <c r="B204" t="s">
-        <v>575</v>
+        <v>594</v>
       </c>
       <c r="C204" t="s">
-        <v>576</v>
+        <v>595</v>
       </c>
       <c r="D204">
         <v>0</v>
@@ -8180,16 +8429,19 @@
       <c r="G204">
         <v>0</v>
       </c>
+      <c r="H204" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="205" spans="1:8">
       <c r="A205" t="s">
-        <v>577</v>
+        <v>596</v>
       </c>
       <c r="B205" t="s">
-        <v>578</v>
+        <v>597</v>
       </c>
       <c r="C205" t="s">
-        <v>579</v>
+        <v>598</v>
       </c>
       <c r="D205">
         <v>0</v>
@@ -8203,16 +8455,19 @@
       <c r="G205">
         <v>0</v>
       </c>
+      <c r="H205" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="206" spans="1:8">
       <c r="A206" t="s">
-        <v>580</v>
+        <v>599</v>
       </c>
       <c r="B206" t="s">
-        <v>581</v>
+        <v>600</v>
       </c>
       <c r="C206" t="s">
-        <v>582</v>
+        <v>601</v>
       </c>
       <c r="D206">
         <v>0</v>
@@ -8224,18 +8479,21 @@
         <v>0.64655172413793105</v>
       </c>
       <c r="G206">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H206" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="207" spans="1:8">
       <c r="A207" t="s">
-        <v>583</v>
+        <v>603</v>
       </c>
       <c r="B207" t="s">
-        <v>581</v>
+        <v>600</v>
       </c>
       <c r="C207" t="s">
-        <v>582</v>
+        <v>601</v>
       </c>
       <c r="D207">
         <v>0</v>
@@ -8247,18 +8505,21 @@
         <v>0.64655172413793105</v>
       </c>
       <c r="G207">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H207" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="208" spans="1:8">
       <c r="A208" t="s">
-        <v>584</v>
+        <v>604</v>
       </c>
       <c r="B208" t="s">
-        <v>585</v>
+        <v>605</v>
       </c>
       <c r="C208" t="s">
-        <v>586</v>
+        <v>606</v>
       </c>
       <c r="D208">
         <v>0</v>
@@ -8270,18 +8531,21 @@
         <v>0.72436363636363632</v>
       </c>
       <c r="G208">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H208" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="209" spans="1:8">
       <c r="A209" t="s">
-        <v>587</v>
+        <v>608</v>
       </c>
       <c r="B209" t="s">
-        <v>588</v>
+        <v>609</v>
       </c>
       <c r="C209" t="s">
-        <v>589</v>
+        <v>610</v>
       </c>
       <c r="D209">
         <v>0</v>
@@ -8295,16 +8559,19 @@
       <c r="G209">
         <v>0</v>
       </c>
+      <c r="H209" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="210" spans="1:8">
       <c r="A210" t="s">
-        <v>590</v>
+        <v>612</v>
       </c>
       <c r="B210" t="s">
-        <v>591</v>
+        <v>613</v>
       </c>
       <c r="C210" t="s">
-        <v>592</v>
+        <v>614</v>
       </c>
       <c r="D210">
         <v>0</v>
@@ -8318,16 +8585,19 @@
       <c r="G210">
         <v>0</v>
       </c>
+      <c r="H210" t="s">
+        <v>615</v>
+      </c>
     </row>
     <row r="211" spans="1:8">
       <c r="A211" t="s">
-        <v>593</v>
+        <v>616</v>
       </c>
       <c r="B211" t="s">
-        <v>594</v>
+        <v>617</v>
       </c>
       <c r="C211" t="s">
-        <v>594</v>
+        <v>617</v>
       </c>
       <c r="D211">
         <v>1</v>
@@ -8344,13 +8614,13 @@
     </row>
     <row r="212" spans="1:8">
       <c r="A212" t="s">
-        <v>595</v>
+        <v>618</v>
       </c>
       <c r="B212" t="s">
-        <v>596</v>
+        <v>619</v>
       </c>
       <c r="C212" t="s">
-        <v>596</v>
+        <v>619</v>
       </c>
       <c r="D212">
         <v>1</v>
@@ -8367,13 +8637,13 @@
     </row>
     <row r="213" spans="1:8">
       <c r="A213" t="s">
-        <v>597</v>
+        <v>620</v>
       </c>
       <c r="B213" t="s">
-        <v>598</v>
+        <v>621</v>
       </c>
       <c r="C213" t="s">
-        <v>599</v>
+        <v>622</v>
       </c>
       <c r="D213">
         <v>0</v>
@@ -8387,16 +8657,19 @@
       <c r="G213">
         <v>0</v>
       </c>
+      <c r="H213" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="214" spans="1:8">
       <c r="A214" t="s">
-        <v>600</v>
+        <v>623</v>
       </c>
       <c r="B214" t="s">
-        <v>601</v>
+        <v>624</v>
       </c>
       <c r="C214" t="s">
-        <v>601</v>
+        <v>624</v>
       </c>
       <c r="D214">
         <v>1</v>
@@ -8413,13 +8686,13 @@
     </row>
     <row r="215" spans="1:8">
       <c r="A215" t="s">
-        <v>602</v>
+        <v>625</v>
       </c>
       <c r="B215" t="s">
-        <v>603</v>
+        <v>626</v>
       </c>
       <c r="C215" t="s">
-        <v>604</v>
+        <v>627</v>
       </c>
       <c r="D215">
         <v>0</v>
@@ -8431,18 +8704,21 @@
         <v>0.92688081149619617</v>
       </c>
       <c r="G215">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H215" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="216" spans="1:8">
       <c r="A216" t="s">
-        <v>605</v>
+        <v>629</v>
       </c>
       <c r="B216" t="s">
-        <v>606</v>
+        <v>630</v>
       </c>
       <c r="C216" t="s">
-        <v>606</v>
+        <v>630</v>
       </c>
       <c r="D216">
         <v>1</v>
@@ -8459,13 +8735,13 @@
     </row>
     <row r="217" spans="1:8">
       <c r="A217" t="s">
-        <v>607</v>
+        <v>631</v>
       </c>
       <c r="B217" t="s">
-        <v>608</v>
+        <v>632</v>
       </c>
       <c r="C217" t="s">
-        <v>609</v>
+        <v>633</v>
       </c>
       <c r="D217">
         <v>0</v>
@@ -8479,16 +8755,19 @@
       <c r="G217">
         <v>0</v>
       </c>
+      <c r="H217" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="218" spans="1:8">
       <c r="A218" t="s">
-        <v>610</v>
+        <v>634</v>
       </c>
       <c r="B218" t="s">
-        <v>611</v>
+        <v>635</v>
       </c>
       <c r="C218" t="s">
-        <v>611</v>
+        <v>635</v>
       </c>
       <c r="D218">
         <v>1</v>
@@ -8505,13 +8784,13 @@
     </row>
     <row r="219" spans="1:8">
       <c r="A219" t="s">
-        <v>612</v>
+        <v>636</v>
       </c>
       <c r="B219" t="s">
-        <v>613</v>
+        <v>637</v>
       </c>
       <c r="C219" t="s">
-        <v>613</v>
+        <v>637</v>
       </c>
       <c r="D219">
         <v>1</v>
@@ -8528,13 +8807,13 @@
     </row>
     <row r="220" spans="1:8">
       <c r="A220" t="s">
-        <v>614</v>
+        <v>638</v>
       </c>
       <c r="B220" t="s">
-        <v>615</v>
+        <v>639</v>
       </c>
       <c r="C220" t="s">
-        <v>615</v>
+        <v>639</v>
       </c>
       <c r="D220">
         <v>1</v>
@@ -8551,10 +8830,10 @@
     </row>
     <row r="221" spans="1:8">
       <c r="A221" t="s">
-        <v>616</v>
+        <v>640</v>
       </c>
       <c r="B221" t="s">
-        <v>617</v>
+        <v>641</v>
       </c>
       <c r="C221" t="s">
         <v>53</v>
@@ -8577,13 +8856,13 @@
     </row>
     <row r="222" spans="1:8">
       <c r="A222" t="s">
-        <v>618</v>
+        <v>642</v>
       </c>
       <c r="B222" t="s">
-        <v>619</v>
+        <v>643</v>
       </c>
       <c r="C222" t="s">
-        <v>620</v>
+        <v>644</v>
       </c>
       <c r="D222">
         <v>0</v>
@@ -8595,18 +8874,18 @@
         <v>0.98148148148148151</v>
       </c>
       <c r="G222">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223" spans="1:8">
       <c r="A223" t="s">
-        <v>621</v>
+        <v>645</v>
       </c>
       <c r="B223" t="s">
-        <v>622</v>
+        <v>646</v>
       </c>
       <c r="C223" t="s">
-        <v>623</v>
+        <v>647</v>
       </c>
       <c r="D223">
         <v>0</v>
@@ -8618,18 +8897,18 @@
         <v>0.75000000000000011</v>
       </c>
       <c r="G223">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="224" spans="1:8">
       <c r="A224" t="s">
-        <v>624</v>
+        <v>648</v>
       </c>
       <c r="B224" t="s">
-        <v>625</v>
+        <v>649</v>
       </c>
       <c r="C224" t="s">
-        <v>626</v>
+        <v>650</v>
       </c>
       <c r="D224">
         <v>0</v>
@@ -8641,18 +8920,21 @@
         <v>0.74799494219653184</v>
       </c>
       <c r="G224">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H224" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="225" spans="1:8">
       <c r="A225" t="s">
-        <v>627</v>
+        <v>652</v>
       </c>
       <c r="B225" t="s">
-        <v>628</v>
+        <v>653</v>
       </c>
       <c r="C225" t="s">
-        <v>629</v>
+        <v>654</v>
       </c>
       <c r="D225">
         <v>0</v>
@@ -8666,16 +8948,19 @@
       <c r="G225">
         <v>0</v>
       </c>
+      <c r="H225" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="226" spans="1:8">
       <c r="A226" t="s">
-        <v>630</v>
+        <v>656</v>
       </c>
       <c r="B226" t="s">
-        <v>631</v>
+        <v>657</v>
       </c>
       <c r="C226" t="s">
-        <v>632</v>
+        <v>658</v>
       </c>
       <c r="D226">
         <v>0</v>
@@ -8689,16 +8974,19 @@
       <c r="G226">
         <v>0</v>
       </c>
+      <c r="H226" t="s">
+        <v>659</v>
+      </c>
     </row>
     <row r="227" spans="1:8">
       <c r="A227" t="s">
-        <v>633</v>
+        <v>660</v>
       </c>
       <c r="B227" t="s">
-        <v>634</v>
+        <v>661</v>
       </c>
       <c r="C227" t="s">
-        <v>635</v>
+        <v>662</v>
       </c>
       <c r="D227">
         <v>0</v>
@@ -8710,18 +8998,21 @@
         <v>0.67824669807608662</v>
       </c>
       <c r="G227">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H227" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="228" spans="1:8">
       <c r="A228" t="s">
-        <v>636</v>
+        <v>664</v>
       </c>
       <c r="B228" t="s">
-        <v>637</v>
+        <v>665</v>
       </c>
       <c r="C228" t="s">
-        <v>638</v>
+        <v>666</v>
       </c>
       <c r="D228">
         <v>0</v>
@@ -8735,13 +9026,16 @@
       <c r="G228">
         <v>0</v>
       </c>
+      <c r="H228" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="229" spans="1:8">
       <c r="A229" t="s">
-        <v>639</v>
+        <v>668</v>
       </c>
       <c r="B229" t="s">
-        <v>640</v>
+        <v>669</v>
       </c>
       <c r="C229" t="s">
         <v>53</v>
@@ -8764,13 +9058,13 @@
     </row>
     <row r="230" spans="1:8">
       <c r="A230" t="s">
-        <v>641</v>
+        <v>670</v>
       </c>
       <c r="B230" t="s">
-        <v>642</v>
+        <v>671</v>
       </c>
       <c r="C230" t="s">
-        <v>643</v>
+        <v>672</v>
       </c>
       <c r="D230">
         <v>0</v>
@@ -8782,18 +9076,21 @@
         <v>0.62203487013952297</v>
       </c>
       <c r="G230">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H230" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="231" spans="1:8">
       <c r="A231" t="s">
-        <v>644</v>
+        <v>674</v>
       </c>
       <c r="B231" t="s">
-        <v>645</v>
+        <v>675</v>
       </c>
       <c r="C231" t="s">
-        <v>646</v>
+        <v>676</v>
       </c>
       <c r="D231">
         <v>0</v>
@@ -8807,16 +9104,19 @@
       <c r="G231">
         <v>0</v>
       </c>
+      <c r="H231" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="232" spans="1:8">
       <c r="A232" t="s">
-        <v>647</v>
+        <v>677</v>
       </c>
       <c r="B232" t="s">
-        <v>648</v>
+        <v>678</v>
       </c>
       <c r="C232" t="s">
-        <v>649</v>
+        <v>679</v>
       </c>
       <c r="D232">
         <v>0</v>
@@ -8830,16 +9130,19 @@
       <c r="G232">
         <v>0</v>
       </c>
+      <c r="H232" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="233" spans="1:8">
       <c r="A233" t="s">
-        <v>650</v>
+        <v>680</v>
       </c>
       <c r="B233" t="s">
-        <v>651</v>
+        <v>681</v>
       </c>
       <c r="C233" t="s">
-        <v>652</v>
+        <v>682</v>
       </c>
       <c r="D233">
         <v>0</v>
@@ -8853,16 +9156,19 @@
       <c r="G233">
         <v>0</v>
       </c>
+      <c r="H233" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="234" spans="1:8">
       <c r="A234" t="s">
-        <v>653</v>
+        <v>684</v>
       </c>
       <c r="B234" t="s">
-        <v>654</v>
+        <v>685</v>
       </c>
       <c r="C234" t="s">
-        <v>655</v>
+        <v>686</v>
       </c>
       <c r="D234">
         <v>0</v>
@@ -8876,16 +9182,19 @@
       <c r="G234">
         <v>0</v>
       </c>
+      <c r="H234" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="235" spans="1:8">
       <c r="A235" t="s">
-        <v>656</v>
+        <v>688</v>
       </c>
       <c r="B235" t="s">
-        <v>657</v>
+        <v>689</v>
       </c>
       <c r="C235" t="s">
-        <v>658</v>
+        <v>690</v>
       </c>
       <c r="D235">
         <v>0</v>
@@ -8899,16 +9208,19 @@
       <c r="G235">
         <v>0</v>
       </c>
+      <c r="H235" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="236" spans="1:8">
       <c r="A236" t="s">
-        <v>659</v>
+        <v>692</v>
       </c>
       <c r="B236" t="s">
-        <v>660</v>
+        <v>693</v>
       </c>
       <c r="C236" t="s">
-        <v>661</v>
+        <v>694</v>
       </c>
       <c r="D236">
         <v>0</v>
@@ -8922,16 +9234,19 @@
       <c r="G236">
         <v>0</v>
       </c>
+      <c r="H236" t="s">
+        <v>695</v>
+      </c>
     </row>
     <row r="237" spans="1:8">
       <c r="A237" t="s">
-        <v>662</v>
+        <v>696</v>
       </c>
       <c r="B237" t="s">
-        <v>663</v>
+        <v>697</v>
       </c>
       <c r="C237" t="s">
-        <v>664</v>
+        <v>698</v>
       </c>
       <c r="D237">
         <v>0</v>
@@ -8945,16 +9260,19 @@
       <c r="G237">
         <v>0</v>
       </c>
+      <c r="H237" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="238" spans="1:8">
       <c r="A238" t="s">
-        <v>665</v>
+        <v>700</v>
       </c>
       <c r="B238" t="s">
-        <v>666</v>
+        <v>701</v>
       </c>
       <c r="C238" t="s">
-        <v>667</v>
+        <v>702</v>
       </c>
       <c r="D238">
         <v>0</v>
@@ -8968,16 +9286,19 @@
       <c r="G238">
         <v>0</v>
       </c>
+      <c r="H238" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="239" spans="1:8">
       <c r="A239" t="s">
-        <v>668</v>
+        <v>704</v>
       </c>
       <c r="B239" t="s">
-        <v>669</v>
+        <v>705</v>
       </c>
       <c r="C239" t="s">
-        <v>670</v>
+        <v>706</v>
       </c>
       <c r="D239">
         <v>0</v>
@@ -8991,16 +9312,19 @@
       <c r="G239">
         <v>0</v>
       </c>
+      <c r="H239" t="s">
+        <v>707</v>
+      </c>
     </row>
     <row r="240" spans="1:8">
       <c r="A240" t="s">
-        <v>671</v>
+        <v>708</v>
       </c>
       <c r="B240" t="s">
-        <v>672</v>
+        <v>709</v>
       </c>
       <c r="C240" t="s">
-        <v>673</v>
+        <v>710</v>
       </c>
       <c r="D240">
         <v>0</v>
@@ -9014,16 +9338,19 @@
       <c r="G240">
         <v>0</v>
       </c>
-    </row>
-    <row r="241" spans="1:7">
+      <c r="H240" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8">
       <c r="A241" t="s">
-        <v>674</v>
+        <v>712</v>
       </c>
       <c r="B241" t="s">
-        <v>675</v>
+        <v>713</v>
       </c>
       <c r="C241" t="s">
-        <v>676</v>
+        <v>714</v>
       </c>
       <c r="D241">
         <v>0</v>
@@ -9037,16 +9364,19 @@
       <c r="G241">
         <v>0</v>
       </c>
-    </row>
-    <row r="242" spans="1:7">
+      <c r="H241" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8">
       <c r="A242" t="s">
-        <v>677</v>
+        <v>716</v>
       </c>
       <c r="B242" t="s">
-        <v>678</v>
+        <v>717</v>
       </c>
       <c r="C242" t="s">
-        <v>679</v>
+        <v>718</v>
       </c>
       <c r="D242">
         <v>0</v>
@@ -9060,16 +9390,19 @@
       <c r="G242">
         <v>0</v>
       </c>
-    </row>
-    <row r="243" spans="1:7">
+      <c r="H242" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8">
       <c r="A243" t="s">
-        <v>680</v>
+        <v>720</v>
       </c>
       <c r="B243" t="s">
-        <v>681</v>
+        <v>721</v>
       </c>
       <c r="C243" t="s">
-        <v>682</v>
+        <v>722</v>
       </c>
       <c r="D243">
         <v>0</v>
@@ -9081,18 +9414,21 @@
         <v>0.74341696106277533</v>
       </c>
       <c r="G243">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="244" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H243" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8">
       <c r="A244" t="s">
-        <v>683</v>
+        <v>724</v>
       </c>
       <c r="B244" t="s">
-        <v>684</v>
+        <v>725</v>
       </c>
       <c r="C244" t="s">
-        <v>685</v>
+        <v>726</v>
       </c>
       <c r="D244">
         <v>0</v>
@@ -9107,15 +9443,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:7">
+    <row r="245" spans="1:8">
       <c r="A245" t="s">
-        <v>686</v>
+        <v>727</v>
       </c>
       <c r="B245" t="s">
-        <v>687</v>
+        <v>728</v>
       </c>
       <c r="C245" t="s">
-        <v>688</v>
+        <v>729</v>
       </c>
       <c r="D245">
         <v>0</v>
@@ -9130,15 +9466,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:7">
+    <row r="246" spans="1:8">
       <c r="A246" t="s">
-        <v>689</v>
+        <v>730</v>
       </c>
       <c r="B246" t="s">
-        <v>690</v>
+        <v>731</v>
       </c>
       <c r="C246" t="s">
-        <v>691</v>
+        <v>732</v>
       </c>
       <c r="D246">
         <v>0</v>
@@ -9153,15 +9489,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:7">
+    <row r="247" spans="1:8">
       <c r="A247" t="s">
-        <v>692</v>
+        <v>733</v>
       </c>
       <c r="B247" t="s">
-        <v>693</v>
+        <v>734</v>
       </c>
       <c r="C247" t="s">
-        <v>694</v>
+        <v>735</v>
       </c>
       <c r="D247">
         <v>0</v>
@@ -9176,15 +9512,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:7">
+    <row r="248" spans="1:8">
       <c r="A248" t="s">
-        <v>695</v>
+        <v>736</v>
       </c>
       <c r="B248" t="s">
-        <v>696</v>
+        <v>737</v>
       </c>
       <c r="C248" t="s">
-        <v>697</v>
+        <v>738</v>
       </c>
       <c r="D248">
         <v>0</v>
@@ -9199,15 +9535,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:7">
+    <row r="249" spans="1:8">
       <c r="A249" t="s">
-        <v>698</v>
+        <v>739</v>
       </c>
       <c r="B249" t="s">
-        <v>699</v>
+        <v>740</v>
       </c>
       <c r="C249" t="s">
-        <v>700</v>
+        <v>741</v>
       </c>
       <c r="D249">
         <v>0</v>
@@ -9222,15 +9558,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:7">
+    <row r="250" spans="1:8">
       <c r="A250" t="s">
-        <v>701</v>
+        <v>742</v>
       </c>
       <c r="B250" t="s">
-        <v>702</v>
+        <v>743</v>
       </c>
       <c r="C250" t="s">
-        <v>703</v>
+        <v>744</v>
       </c>
       <c r="D250">
         <v>0</v>
@@ -9245,15 +9581,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:7">
+    <row r="251" spans="1:8">
       <c r="A251" t="s">
-        <v>704</v>
+        <v>745</v>
       </c>
       <c r="B251" t="s">
-        <v>705</v>
+        <v>746</v>
       </c>
       <c r="C251" t="s">
-        <v>706</v>
+        <v>747</v>
       </c>
       <c r="D251">
         <v>0</v>
@@ -9268,15 +9604,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:7">
+    <row r="252" spans="1:8">
       <c r="A252" t="s">
-        <v>707</v>
+        <v>748</v>
       </c>
       <c r="B252" t="s">
-        <v>708</v>
+        <v>749</v>
       </c>
       <c r="C252" t="s">
-        <v>709</v>
+        <v>750</v>
       </c>
       <c r="D252">
         <v>0</v>
@@ -9291,15 +9627,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:7">
+    <row r="253" spans="1:8">
       <c r="A253" t="s">
-        <v>710</v>
+        <v>751</v>
       </c>
       <c r="B253" t="s">
-        <v>711</v>
+        <v>752</v>
       </c>
       <c r="C253" t="s">
-        <v>712</v>
+        <v>753</v>
       </c>
       <c r="D253">
         <v>0</v>
@@ -9314,15 +9650,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:7">
+    <row r="254" spans="1:8">
       <c r="A254" t="s">
-        <v>713</v>
+        <v>754</v>
       </c>
       <c r="B254" t="s">
-        <v>714</v>
+        <v>755</v>
       </c>
       <c r="C254" t="s">
-        <v>715</v>
+        <v>756</v>
       </c>
       <c r="D254">
         <v>0</v>
@@ -9337,15 +9673,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:7">
+    <row r="255" spans="1:8">
       <c r="A255" t="s">
-        <v>716</v>
+        <v>757</v>
       </c>
       <c r="B255" t="s">
-        <v>717</v>
+        <v>758</v>
       </c>
       <c r="C255" t="s">
-        <v>718</v>
+        <v>759</v>
       </c>
       <c r="D255">
         <v>0</v>
@@ -9360,15 +9696,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:7">
+    <row r="256" spans="1:8">
       <c r="A256" t="s">
-        <v>719</v>
+        <v>760</v>
       </c>
       <c r="B256" t="s">
-        <v>720</v>
+        <v>761</v>
       </c>
       <c r="C256" t="s">
-        <v>721</v>
+        <v>762</v>
       </c>
       <c r="D256">
         <v>0</v>
@@ -9385,13 +9721,13 @@
     </row>
     <row r="257" spans="1:7">
       <c r="A257" t="s">
-        <v>722</v>
+        <v>763</v>
       </c>
       <c r="B257" t="s">
-        <v>723</v>
+        <v>764</v>
       </c>
       <c r="C257" t="s">
-        <v>724</v>
+        <v>765</v>
       </c>
       <c r="D257">
         <v>0</v>
@@ -9408,13 +9744,13 @@
     </row>
     <row r="258" spans="1:7">
       <c r="A258" t="s">
-        <v>725</v>
+        <v>766</v>
       </c>
       <c r="B258" t="s">
-        <v>726</v>
+        <v>767</v>
       </c>
       <c r="C258" t="s">
-        <v>727</v>
+        <v>768</v>
       </c>
       <c r="D258">
         <v>0</v>
@@ -9431,13 +9767,13 @@
     </row>
     <row r="259" spans="1:7">
       <c r="A259" t="s">
-        <v>728</v>
+        <v>769</v>
       </c>
       <c r="B259" t="s">
-        <v>729</v>
+        <v>770</v>
       </c>
       <c r="C259" t="s">
-        <v>730</v>
+        <v>771</v>
       </c>
       <c r="D259">
         <v>0</v>
@@ -9454,13 +9790,13 @@
     </row>
     <row r="260" spans="1:7">
       <c r="A260" t="s">
-        <v>731</v>
+        <v>772</v>
       </c>
       <c r="B260" t="s">
-        <v>732</v>
+        <v>773</v>
       </c>
       <c r="C260" t="s">
-        <v>733</v>
+        <v>774</v>
       </c>
       <c r="D260">
         <v>0</v>
@@ -9477,13 +9813,13 @@
     </row>
     <row r="261" spans="1:7">
       <c r="A261" t="s">
-        <v>734</v>
+        <v>775</v>
       </c>
       <c r="B261" t="s">
-        <v>735</v>
+        <v>776</v>
       </c>
       <c r="C261" t="s">
-        <v>736</v>
+        <v>777</v>
       </c>
       <c r="D261">
         <v>0</v>
@@ -9500,13 +9836,13 @@
     </row>
     <row r="262" spans="1:7">
       <c r="A262" t="s">
-        <v>737</v>
+        <v>778</v>
       </c>
       <c r="B262" t="s">
-        <v>738</v>
+        <v>779</v>
       </c>
       <c r="C262" t="s">
-        <v>739</v>
+        <v>780</v>
       </c>
       <c r="D262">
         <v>0</v>
@@ -9523,13 +9859,13 @@
     </row>
     <row r="263" spans="1:7">
       <c r="A263" t="s">
-        <v>740</v>
+        <v>781</v>
       </c>
       <c r="B263" t="s">
-        <v>741</v>
+        <v>782</v>
       </c>
       <c r="C263" t="s">
-        <v>742</v>
+        <v>783</v>
       </c>
       <c r="D263">
         <v>0</v>
@@ -9546,13 +9882,13 @@
     </row>
     <row r="264" spans="1:7">
       <c r="A264" t="s">
-        <v>743</v>
+        <v>784</v>
       </c>
       <c r="B264" t="s">
-        <v>744</v>
+        <v>785</v>
       </c>
       <c r="C264" t="s">
-        <v>745</v>
+        <v>786</v>
       </c>
       <c r="D264">
         <v>0</v>
@@ -9569,13 +9905,13 @@
     </row>
     <row r="265" spans="1:7">
       <c r="A265" t="s">
-        <v>746</v>
+        <v>787</v>
       </c>
       <c r="B265" t="s">
-        <v>747</v>
+        <v>788</v>
       </c>
       <c r="C265" t="s">
-        <v>748</v>
+        <v>789</v>
       </c>
       <c r="D265">
         <v>0</v>
@@ -9592,13 +9928,13 @@
     </row>
     <row r="266" spans="1:7">
       <c r="A266" t="s">
-        <v>749</v>
+        <v>790</v>
       </c>
       <c r="B266" t="s">
-        <v>750</v>
+        <v>791</v>
       </c>
       <c r="C266" t="s">
-        <v>751</v>
+        <v>792</v>
       </c>
       <c r="D266">
         <v>0</v>
@@ -9615,13 +9951,13 @@
     </row>
     <row r="267" spans="1:7">
       <c r="A267" t="s">
-        <v>752</v>
+        <v>793</v>
       </c>
       <c r="B267" t="s">
-        <v>753</v>
+        <v>794</v>
       </c>
       <c r="C267" t="s">
-        <v>754</v>
+        <v>795</v>
       </c>
       <c r="D267">
         <v>0</v>
@@ -9638,13 +9974,13 @@
     </row>
     <row r="268" spans="1:7">
       <c r="A268" t="s">
-        <v>755</v>
+        <v>796</v>
       </c>
       <c r="B268" t="s">
-        <v>756</v>
+        <v>797</v>
       </c>
       <c r="C268" t="s">
-        <v>757</v>
+        <v>798</v>
       </c>
       <c r="D268">
         <v>0</v>
@@ -9661,13 +9997,13 @@
     </row>
     <row r="269" spans="1:7">
       <c r="A269" t="s">
-        <v>758</v>
+        <v>799</v>
       </c>
       <c r="B269" t="s">
-        <v>759</v>
+        <v>800</v>
       </c>
       <c r="C269" t="s">
-        <v>760</v>
+        <v>801</v>
       </c>
       <c r="D269">
         <v>0</v>
@@ -9684,13 +10020,13 @@
     </row>
     <row r="270" spans="1:7">
       <c r="A270" t="s">
-        <v>761</v>
+        <v>802</v>
       </c>
       <c r="B270" t="s">
-        <v>762</v>
+        <v>803</v>
       </c>
       <c r="C270" t="s">
-        <v>763</v>
+        <v>804</v>
       </c>
       <c r="D270">
         <v>0</v>
@@ -9707,13 +10043,13 @@
     </row>
     <row r="271" spans="1:7">
       <c r="A271" t="s">
-        <v>764</v>
+        <v>805</v>
       </c>
       <c r="B271" t="s">
-        <v>765</v>
+        <v>806</v>
       </c>
       <c r="C271" t="s">
-        <v>766</v>
+        <v>807</v>
       </c>
       <c r="D271">
         <v>0</v>
@@ -9730,13 +10066,13 @@
     </row>
     <row r="272" spans="1:7">
       <c r="A272" t="s">
-        <v>767</v>
+        <v>808</v>
       </c>
       <c r="B272" t="s">
-        <v>768</v>
+        <v>809</v>
       </c>
       <c r="C272" t="s">
-        <v>769</v>
+        <v>810</v>
       </c>
       <c r="D272">
         <v>0</v>
@@ -9753,13 +10089,13 @@
     </row>
     <row r="273" spans="1:8">
       <c r="A273" t="s">
-        <v>770</v>
+        <v>811</v>
       </c>
       <c r="B273" t="s">
-        <v>771</v>
+        <v>812</v>
       </c>
       <c r="C273" t="s">
-        <v>772</v>
+        <v>813</v>
       </c>
       <c r="D273">
         <v>0</v>
@@ -9776,13 +10112,13 @@
     </row>
     <row r="274" spans="1:8">
       <c r="A274" t="s">
-        <v>773</v>
+        <v>814</v>
       </c>
       <c r="B274" t="s">
-        <v>774</v>
+        <v>815</v>
       </c>
       <c r="C274" t="s">
-        <v>775</v>
+        <v>816</v>
       </c>
       <c r="D274">
         <v>0</v>
@@ -9799,13 +10135,13 @@
     </row>
     <row r="275" spans="1:8">
       <c r="A275" t="s">
-        <v>776</v>
+        <v>817</v>
       </c>
       <c r="B275" t="s">
-        <v>777</v>
+        <v>818</v>
       </c>
       <c r="C275" t="s">
-        <v>778</v>
+        <v>819</v>
       </c>
       <c r="D275">
         <v>0</v>
@@ -9822,13 +10158,13 @@
     </row>
     <row r="276" spans="1:8">
       <c r="A276" t="s">
-        <v>779</v>
+        <v>820</v>
       </c>
       <c r="B276" t="s">
-        <v>780</v>
+        <v>821</v>
       </c>
       <c r="C276" t="s">
-        <v>781</v>
+        <v>822</v>
       </c>
       <c r="D276">
         <v>0</v>
@@ -9845,13 +10181,13 @@
     </row>
     <row r="277" spans="1:8">
       <c r="A277" t="s">
-        <v>782</v>
+        <v>823</v>
       </c>
       <c r="B277" t="s">
-        <v>783</v>
+        <v>824</v>
       </c>
       <c r="C277" t="s">
-        <v>784</v>
+        <v>825</v>
       </c>
       <c r="D277">
         <v>0</v>
@@ -9868,13 +10204,13 @@
     </row>
     <row r="278" spans="1:8">
       <c r="A278" t="s">
-        <v>785</v>
+        <v>826</v>
       </c>
       <c r="B278" t="s">
-        <v>786</v>
+        <v>827</v>
       </c>
       <c r="C278" t="s">
-        <v>787</v>
+        <v>828</v>
       </c>
       <c r="D278">
         <v>0</v>
@@ -9891,10 +10227,10 @@
     </row>
     <row r="279" spans="1:8">
       <c r="A279" t="s">
-        <v>788</v>
+        <v>829</v>
       </c>
       <c r="B279" t="s">
-        <v>789</v>
+        <v>830</v>
       </c>
       <c r="C279" t="s">
         <v>53</v>
@@ -9917,13 +10253,13 @@
     </row>
     <row r="280" spans="1:8">
       <c r="A280" t="s">
-        <v>790</v>
+        <v>831</v>
       </c>
       <c r="B280" t="s">
-        <v>791</v>
+        <v>832</v>
       </c>
       <c r="C280" t="s">
-        <v>792</v>
+        <v>833</v>
       </c>
       <c r="D280">
         <v>0</v>
@@ -9940,13 +10276,13 @@
     </row>
     <row r="281" spans="1:8">
       <c r="A281" t="s">
-        <v>793</v>
+        <v>834</v>
       </c>
       <c r="B281" t="s">
-        <v>794</v>
+        <v>835</v>
       </c>
       <c r="C281" t="s">
-        <v>795</v>
+        <v>836</v>
       </c>
       <c r="D281">
         <v>0</v>
@@ -9963,13 +10299,13 @@
     </row>
     <row r="282" spans="1:8">
       <c r="A282" t="s">
-        <v>796</v>
+        <v>837</v>
       </c>
       <c r="B282" t="s">
-        <v>797</v>
+        <v>838</v>
       </c>
       <c r="C282" t="s">
-        <v>798</v>
+        <v>839</v>
       </c>
       <c r="D282">
         <v>0</v>
@@ -9986,13 +10322,13 @@
     </row>
     <row r="283" spans="1:8">
       <c r="A283" t="s">
-        <v>799</v>
+        <v>840</v>
       </c>
       <c r="B283" t="s">
-        <v>800</v>
+        <v>841</v>
       </c>
       <c r="C283" t="s">
-        <v>801</v>
+        <v>842</v>
       </c>
       <c r="D283">
         <v>0</v>
@@ -10009,13 +10345,13 @@
     </row>
     <row r="284" spans="1:8">
       <c r="A284" t="s">
-        <v>802</v>
+        <v>843</v>
       </c>
       <c r="B284" t="s">
-        <v>803</v>
+        <v>844</v>
       </c>
       <c r="C284" t="s">
-        <v>804</v>
+        <v>845</v>
       </c>
       <c r="D284">
         <v>0</v>
@@ -10032,13 +10368,13 @@
     </row>
     <row r="285" spans="1:8">
       <c r="A285" t="s">
-        <v>805</v>
+        <v>846</v>
       </c>
       <c r="B285" t="s">
-        <v>806</v>
+        <v>847</v>
       </c>
       <c r="C285" t="s">
-        <v>807</v>
+        <v>848</v>
       </c>
       <c r="D285">
         <v>0</v>
@@ -10055,13 +10391,13 @@
     </row>
     <row r="286" spans="1:8">
       <c r="A286" t="s">
-        <v>808</v>
+        <v>849</v>
       </c>
       <c r="B286" t="s">
-        <v>809</v>
+        <v>850</v>
       </c>
       <c r="C286" t="s">
-        <v>810</v>
+        <v>851</v>
       </c>
       <c r="D286">
         <v>0</v>
@@ -10078,13 +10414,13 @@
     </row>
     <row r="287" spans="1:8">
       <c r="A287" t="s">
-        <v>811</v>
+        <v>852</v>
       </c>
       <c r="B287" t="s">
-        <v>812</v>
+        <v>853</v>
       </c>
       <c r="C287" t="s">
-        <v>813</v>
+        <v>854</v>
       </c>
       <c r="D287">
         <v>0</v>
@@ -10101,13 +10437,13 @@
     </row>
     <row r="288" spans="1:8">
       <c r="A288" t="s">
-        <v>814</v>
+        <v>855</v>
       </c>
       <c r="B288" t="s">
-        <v>815</v>
+        <v>856</v>
       </c>
       <c r="C288" t="s">
-        <v>816</v>
+        <v>857</v>
       </c>
       <c r="D288">
         <v>0</v>
@@ -10124,10 +10460,10 @@
     </row>
     <row r="289" spans="1:8">
       <c r="A289" t="s">
-        <v>817</v>
+        <v>858</v>
       </c>
       <c r="B289" t="s">
-        <v>818</v>
+        <v>859</v>
       </c>
       <c r="C289" t="s">
         <v>53</v>
@@ -10150,13 +10486,13 @@
     </row>
     <row r="290" spans="1:8">
       <c r="A290" t="s">
-        <v>819</v>
+        <v>860</v>
       </c>
       <c r="B290" t="s">
-        <v>820</v>
+        <v>861</v>
       </c>
       <c r="C290" t="s">
-        <v>821</v>
+        <v>862</v>
       </c>
       <c r="D290">
         <v>0</v>
@@ -10173,13 +10509,13 @@
     </row>
     <row r="291" spans="1:8">
       <c r="A291" t="s">
-        <v>822</v>
+        <v>863</v>
       </c>
       <c r="B291" t="s">
-        <v>823</v>
+        <v>864</v>
       </c>
       <c r="C291" t="s">
-        <v>824</v>
+        <v>865</v>
       </c>
       <c r="D291">
         <v>0</v>
@@ -10196,13 +10532,13 @@
     </row>
     <row r="292" spans="1:8">
       <c r="A292" t="s">
-        <v>825</v>
+        <v>866</v>
       </c>
       <c r="B292" t="s">
-        <v>826</v>
+        <v>867</v>
       </c>
       <c r="C292" t="s">
-        <v>827</v>
+        <v>868</v>
       </c>
       <c r="D292">
         <v>0</v>
@@ -10219,13 +10555,13 @@
     </row>
     <row r="293" spans="1:8">
       <c r="A293" t="s">
-        <v>828</v>
+        <v>869</v>
       </c>
       <c r="B293" t="s">
-        <v>829</v>
+        <v>870</v>
       </c>
       <c r="C293" t="s">
-        <v>829</v>
+        <v>870</v>
       </c>
       <c r="D293">
         <v>1</v>
@@ -10242,13 +10578,13 @@
     </row>
     <row r="294" spans="1:8">
       <c r="A294" t="s">
-        <v>830</v>
+        <v>871</v>
       </c>
       <c r="B294" t="s">
-        <v>831</v>
+        <v>872</v>
       </c>
       <c r="C294" t="s">
-        <v>832</v>
+        <v>873</v>
       </c>
       <c r="D294">
         <v>0</v>
@@ -10265,13 +10601,13 @@
     </row>
     <row r="295" spans="1:8">
       <c r="A295" t="s">
-        <v>833</v>
+        <v>874</v>
       </c>
       <c r="B295" t="s">
-        <v>834</v>
+        <v>875</v>
       </c>
       <c r="C295" t="s">
-        <v>835</v>
+        <v>876</v>
       </c>
       <c r="D295">
         <v>0</v>
@@ -10288,13 +10624,13 @@
     </row>
     <row r="296" spans="1:8">
       <c r="A296" t="s">
-        <v>836</v>
+        <v>877</v>
       </c>
       <c r="B296" t="s">
-        <v>837</v>
+        <v>878</v>
       </c>
       <c r="C296" t="s">
-        <v>838</v>
+        <v>879</v>
       </c>
       <c r="D296">
         <v>0</v>
@@ -10311,10 +10647,10 @@
     </row>
     <row r="297" spans="1:8">
       <c r="A297" t="s">
-        <v>839</v>
+        <v>880</v>
       </c>
       <c r="B297" t="s">
-        <v>840</v>
+        <v>881</v>
       </c>
       <c r="C297" t="s">
         <v>53</v>
@@ -10337,13 +10673,13 @@
     </row>
     <row r="298" spans="1:8">
       <c r="A298" t="s">
-        <v>841</v>
+        <v>882</v>
       </c>
       <c r="B298" t="s">
-        <v>842</v>
+        <v>883</v>
       </c>
       <c r="C298" t="s">
-        <v>843</v>
+        <v>884</v>
       </c>
       <c r="D298">
         <v>0</v>
@@ -10360,10 +10696,10 @@
     </row>
     <row r="299" spans="1:8">
       <c r="A299" t="s">
-        <v>844</v>
+        <v>885</v>
       </c>
       <c r="B299" t="s">
-        <v>845</v>
+        <v>886</v>
       </c>
       <c r="C299" t="s">
         <v>53</v>
@@ -10386,13 +10722,13 @@
     </row>
     <row r="300" spans="1:8">
       <c r="A300" t="s">
-        <v>846</v>
+        <v>887</v>
       </c>
       <c r="B300" t="s">
-        <v>847</v>
+        <v>888</v>
       </c>
       <c r="C300" t="s">
-        <v>848</v>
+        <v>889</v>
       </c>
       <c r="D300">
         <v>0</v>
@@ -10409,13 +10745,13 @@
     </row>
     <row r="301" spans="1:8">
       <c r="A301" t="s">
-        <v>849</v>
+        <v>890</v>
       </c>
       <c r="B301" t="s">
-        <v>850</v>
+        <v>891</v>
       </c>
       <c r="C301" t="s">
-        <v>851</v>
+        <v>892</v>
       </c>
       <c r="D301">
         <v>0</v>
@@ -10432,10 +10768,10 @@
     </row>
     <row r="302" spans="1:8">
       <c r="A302" t="s">
-        <v>852</v>
+        <v>893</v>
       </c>
       <c r="B302" t="s">
-        <v>853</v>
+        <v>894</v>
       </c>
       <c r="C302" t="s">
         <v>53</v>
@@ -10458,13 +10794,13 @@
     </row>
     <row r="303" spans="1:8">
       <c r="A303" t="s">
-        <v>854</v>
+        <v>895</v>
       </c>
       <c r="B303" t="s">
-        <v>855</v>
+        <v>896</v>
       </c>
       <c r="C303" t="s">
-        <v>856</v>
+        <v>897</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -10481,13 +10817,13 @@
     </row>
     <row r="304" spans="1:8">
       <c r="A304" t="s">
-        <v>857</v>
+        <v>898</v>
       </c>
       <c r="B304" t="s">
-        <v>858</v>
+        <v>899</v>
       </c>
       <c r="C304" t="s">
-        <v>859</v>
+        <v>900</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -10504,13 +10840,13 @@
     </row>
     <row r="305" spans="1:8">
       <c r="A305" t="s">
-        <v>860</v>
+        <v>901</v>
       </c>
       <c r="B305" t="s">
-        <v>861</v>
+        <v>902</v>
       </c>
       <c r="C305" t="s">
-        <v>862</v>
+        <v>903</v>
       </c>
       <c r="D305">
         <v>0</v>
@@ -10527,13 +10863,13 @@
     </row>
     <row r="306" spans="1:8">
       <c r="A306" t="s">
-        <v>863</v>
+        <v>904</v>
       </c>
       <c r="B306" t="s">
-        <v>864</v>
+        <v>905</v>
       </c>
       <c r="C306" t="s">
-        <v>865</v>
+        <v>906</v>
       </c>
       <c r="D306">
         <v>0</v>
@@ -10550,13 +10886,13 @@
     </row>
     <row r="307" spans="1:8">
       <c r="A307" t="s">
-        <v>866</v>
+        <v>907</v>
       </c>
       <c r="B307" t="s">
-        <v>867</v>
+        <v>908</v>
       </c>
       <c r="C307" t="s">
-        <v>868</v>
+        <v>909</v>
       </c>
       <c r="D307">
         <v>0</v>
@@ -10573,13 +10909,13 @@
     </row>
     <row r="308" spans="1:8">
       <c r="A308" t="s">
-        <v>869</v>
+        <v>910</v>
       </c>
       <c r="B308" t="s">
-        <v>870</v>
+        <v>911</v>
       </c>
       <c r="C308" t="s">
-        <v>871</v>
+        <v>912</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -10596,13 +10932,13 @@
     </row>
     <row r="309" spans="1:8">
       <c r="A309" t="s">
-        <v>872</v>
+        <v>913</v>
       </c>
       <c r="B309" t="s">
-        <v>873</v>
+        <v>914</v>
       </c>
       <c r="C309" t="s">
-        <v>874</v>
+        <v>915</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -10619,10 +10955,10 @@
     </row>
     <row r="310" spans="1:8">
       <c r="A310" t="s">
-        <v>875</v>
+        <v>916</v>
       </c>
       <c r="B310" t="s">
-        <v>876</v>
+        <v>917</v>
       </c>
       <c r="C310" t="s">
         <v>53</v>
@@ -10645,13 +10981,13 @@
     </row>
     <row r="311" spans="1:8">
       <c r="A311" t="s">
-        <v>877</v>
+        <v>918</v>
       </c>
       <c r="B311" t="s">
-        <v>878</v>
+        <v>919</v>
       </c>
       <c r="C311" t="s">
-        <v>879</v>
+        <v>920</v>
       </c>
       <c r="D311">
         <v>0</v>
@@ -10668,13 +11004,13 @@
     </row>
     <row r="312" spans="1:8">
       <c r="A312" t="s">
-        <v>880</v>
+        <v>921</v>
       </c>
       <c r="B312" t="s">
-        <v>881</v>
+        <v>922</v>
       </c>
       <c r="C312" t="s">
-        <v>882</v>
+        <v>923</v>
       </c>
       <c r="D312">
         <v>0</v>
@@ -10691,13 +11027,13 @@
     </row>
     <row r="313" spans="1:8">
       <c r="A313" t="s">
-        <v>883</v>
+        <v>924</v>
       </c>
       <c r="B313" t="s">
-        <v>884</v>
+        <v>925</v>
       </c>
       <c r="C313" t="s">
-        <v>885</v>
+        <v>926</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -10714,13 +11050,13 @@
     </row>
     <row r="314" spans="1:8">
       <c r="A314" t="s">
-        <v>886</v>
+        <v>927</v>
       </c>
       <c r="B314" t="s">
-        <v>887</v>
+        <v>928</v>
       </c>
       <c r="C314" t="s">
-        <v>888</v>
+        <v>929</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -10737,13 +11073,13 @@
     </row>
     <row r="315" spans="1:8">
       <c r="A315" t="s">
-        <v>889</v>
+        <v>930</v>
       </c>
       <c r="B315" t="s">
-        <v>890</v>
+        <v>931</v>
       </c>
       <c r="C315" t="s">
-        <v>891</v>
+        <v>932</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -10760,13 +11096,13 @@
     </row>
     <row r="316" spans="1:8">
       <c r="A316" t="s">
-        <v>892</v>
+        <v>933</v>
       </c>
       <c r="B316" t="s">
-        <v>893</v>
+        <v>934</v>
       </c>
       <c r="C316" t="s">
-        <v>894</v>
+        <v>935</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -10783,13 +11119,13 @@
     </row>
     <row r="317" spans="1:8">
       <c r="A317" t="s">
-        <v>895</v>
+        <v>936</v>
       </c>
       <c r="B317" t="s">
-        <v>896</v>
+        <v>937</v>
       </c>
       <c r="C317" t="s">
-        <v>897</v>
+        <v>938</v>
       </c>
       <c r="D317">
         <v>0</v>
@@ -10806,13 +11142,13 @@
     </row>
     <row r="318" spans="1:8">
       <c r="A318" t="s">
-        <v>898</v>
+        <v>939</v>
       </c>
       <c r="B318" t="s">
-        <v>899</v>
+        <v>940</v>
       </c>
       <c r="C318" t="s">
-        <v>900</v>
+        <v>941</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -10829,13 +11165,13 @@
     </row>
     <row r="319" spans="1:8">
       <c r="A319" t="s">
-        <v>901</v>
+        <v>942</v>
       </c>
       <c r="B319" t="s">
-        <v>902</v>
+        <v>943</v>
       </c>
       <c r="C319" t="s">
-        <v>903</v>
+        <v>944</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -10852,13 +11188,13 @@
     </row>
     <row r="320" spans="1:8">
       <c r="A320" t="s">
-        <v>904</v>
+        <v>945</v>
       </c>
       <c r="B320" t="s">
-        <v>905</v>
+        <v>946</v>
       </c>
       <c r="C320" t="s">
-        <v>906</v>
+        <v>947</v>
       </c>
       <c r="D320">
         <v>0</v>
@@ -10873,15 +11209,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:7">
+    <row r="321" spans="1:8">
       <c r="A321" t="s">
-        <v>907</v>
+        <v>948</v>
       </c>
       <c r="B321" t="s">
-        <v>908</v>
+        <v>949</v>
       </c>
       <c r="C321" t="s">
-        <v>909</v>
+        <v>950</v>
       </c>
       <c r="D321">
         <v>0</v>
@@ -10896,15 +11232,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:7">
+    <row r="322" spans="1:8">
       <c r="A322" t="s">
-        <v>910</v>
+        <v>951</v>
       </c>
       <c r="B322" t="s">
-        <v>911</v>
+        <v>952</v>
       </c>
       <c r="C322" t="s">
-        <v>912</v>
+        <v>953</v>
       </c>
       <c r="D322">
         <v>0</v>
@@ -10919,15 +11255,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:7">
+    <row r="323" spans="1:8">
       <c r="A323" t="s">
-        <v>913</v>
+        <v>954</v>
       </c>
       <c r="B323" t="s">
-        <v>914</v>
+        <v>955</v>
       </c>
       <c r="C323" t="s">
-        <v>915</v>
+        <v>956</v>
       </c>
       <c r="D323">
         <v>0</v>
@@ -10942,15 +11278,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:7">
+    <row r="324" spans="1:8">
       <c r="A324" t="s">
-        <v>916</v>
+        <v>957</v>
       </c>
       <c r="B324" t="s">
-        <v>917</v>
+        <v>958</v>
       </c>
       <c r="C324" t="s">
-        <v>918</v>
+        <v>959</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -10965,15 +11301,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:7">
+    <row r="325" spans="1:8">
       <c r="A325" t="s">
-        <v>919</v>
+        <v>960</v>
       </c>
       <c r="B325" t="s">
-        <v>920</v>
+        <v>961</v>
       </c>
       <c r="C325" t="s">
-        <v>921</v>
+        <v>962</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -10987,16 +11323,19 @@
       <c r="G325">
         <v>0</v>
       </c>
-    </row>
-    <row r="326" spans="1:7">
+      <c r="H325" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="326" spans="1:8">
       <c r="A326" t="s">
-        <v>922</v>
+        <v>964</v>
       </c>
       <c r="B326" t="s">
-        <v>923</v>
+        <v>965</v>
       </c>
       <c r="C326" t="s">
-        <v>923</v>
+        <v>965</v>
       </c>
       <c r="D326">
         <v>1</v>
@@ -11011,15 +11350,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:7">
+    <row r="327" spans="1:8">
       <c r="A327" t="s">
-        <v>924</v>
+        <v>966</v>
       </c>
       <c r="B327" t="s">
-        <v>925</v>
+        <v>967</v>
       </c>
       <c r="C327" t="s">
-        <v>926</v>
+        <v>968</v>
       </c>
       <c r="D327">
         <v>0</v>
@@ -11032,6 +11371,9 @@
       </c>
       <c r="G327">
         <v>0</v>
+      </c>
+      <c r="H327" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiunte nuove analisi su CodeGPT
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/AnalisiCodeGPT.xlsx
+++ b/HE/W_in_progress/AnalisiCodeGPT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95340D39-3610-42DF-A9C8-691BBBF39B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{593FB464-7EC6-4870-B613-74B3C57B8767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="969">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="985">
   <si>
     <t>IN</t>
   </si>
@@ -2214,6 +2214,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity PulseGenerator is Generic ( N : natural := 8 ); Port ( Clk : in STD_LOGIC; Reset : in STD_LOGIC; Pulse_Width : in STD_LOGIC_VECTOR (N-1 downto 0); Pulse_Out : out STD_LOGIC_VECTOR (N-1 downto 0)); end PulseGenerator; architecture Behavioral of PulseGenerator is signal pulse_out : STD_LOGIC_VECTOR (N-1 downto 0); begin process (Clk, Reset) begin if Reset = '1' then pulse_out &lt;= (others =&gt; '0'); elsif rising_edge(Clk) then if Pulse_Width = '1' then pulse_out &lt;= Pulse_Out(N-1 downto 0); else pulse_out &lt;= Pulse_Out(N-2 downto 0); end if ; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non è un generatore di impulsi</t>
+  </si>
+  <si>
     <t>Define a magnitude comparator of K-bit with the signals A (K-bit) and B (K-bit) as input and the signals A_GT_B, A_EQ_B, and A_LT_B as output.</t>
   </si>
   <si>
@@ -2223,6 +2226,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity magnitude_comparator is Port ( A : in STD_LOGIC; B : in STD_LOGIC; A_GT_B : out STD_LOGIC; A_EQ_B : out STD_LOGIC; A_LT_B : out STD_LOGIC; A_LT_B : out STD_LOGIC); end magnitude_comparator; architecture Behavioral of magnitude_comparator is begin process (A, B) variable temp : STD_LOGIC := '0'; begin temp := A; if (A_GT_B = '1') then temp := A_GT_B; if (A_EQ_B = '1') then temp := A_EQ_B; if (A_LT_B = '1') then temp := A_LT_B; if (A_LT_B = '1') then temp := A_LT_B; end if ; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non è un comparatore di magnitude</t>
+  </si>
+  <si>
     <t>Define a pseudo-random number generator of N-bit with the signals clock and seed_value (N-bit) as input and the signal random_number (N-bit) as output.</t>
   </si>
   <si>
@@ -2232,6 +2238,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity pseudo_random_generator is Generic (N : natural := 8); Port ( Clock : in STD_LOGIC; Seed_Value : in STD_LOGIC_VECTOR (N-1 downto 0); Random_Number : out STD_LOGIC_VECTOR (N-1 downto 0)); end pseudo_random_generator; architecture Behavioral of pseudo_random_generator is begin process (Clock, Seed_Value) variable temp : STD_LOGIC_VECTOR (N-1 downto 0); begin if (rising_edge(Clock)) then temp := Seed_Value; if (temp = '1') then temp := '0'; end if ; end if ; end process ; Random_Number &lt;= temp; end Behavioral;</t>
   </si>
   <si>
+    <t>Non genera numeri pseudo casuali</t>
+  </si>
+  <si>
     <t>Create a configurable clock divider</t>
   </si>
   <si>
@@ -2241,6 +2250,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity clock_divider is Port ( Clock : in STD_LOGIC; Divisore : in STD_LOGIC; Divisore_cu : in STD_LOGIC; Divisore_cu : in STD_LOGIC; Clock_Out : out STD_LOGIC; Divisore_Out : out STD_LOGIC); end clock_divider; architecture Behavioral of clock_divider is signal clock_out_temp : STD_LOGIC := '0'; begin process (Clock, Divisore, Divisore_cu) begin if (Clock = '1') then clock_out &lt;= '1'; elsif (Divisore = '1') then divisore_cu &lt;= '0'; divisore_cu &lt;= '0'; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non un divisore di frequenza</t>
+  </si>
+  <si>
     <t>Write an astable multivibrator with the signals clk and reset as input and the signal oscillating_out as output.</t>
   </si>
   <si>
@@ -2250,6 +2262,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity Multivibrator is Generic (clk : in STD_LOGIC; reset : in STD_LOGIC; oscillating_out : out STD_LOGIC); end Multivibrator; architecture Behavioral of Multivibrator is signal clk_temp : STD_LOGIC := '0'; signal oscillating_out_temp : STD_LOGIC := '0'; begin process (clk, reset) begin if reset = '1' then clk_temp &lt;= '0'; elsif rising_edge(clk) then if reset = '0' then oscillating_out_temp &lt;= '0'; elsif oscillating_out_temp = '1' then oscillating_out_temp &lt;= '0'; end if ; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non è un oscillatore (multivibratore)</t>
+  </si>
+  <si>
     <t>Define a rotating priority encoder with the signal request (N-bit) as input and the signals grant (log2N-bit), valid, and rotation_bit as output.</t>
   </si>
   <si>
@@ -2259,6 +2274,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity PriorityEncoder is Generic (N : natural := 8); Port ( Request : in STD_LOGIC_VECTOR (N-1 downto 0); Grant : in STD_LOGIC_VECTOR (log2(N)-1 downto 0); Valid : out STD_LOGIC_VECTOR (log2(N)-1 downto 0)); end PriorityEncoder; architecture Behavioral of PriorityEncoder is begin process (Request) variable temp : unsigned(N-1 downto 0); begin if Request = '1' then temp := unsigned(N); grant &lt;= '0'; valid &lt;= '1'; rotation_bit &lt;= '1'; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Varie incoerenze, non è un priority encoder</t>
+  </si>
+  <si>
     <t>Generate a floating-point adder of N-bit with the signals A (N-bit) and B (N-bit) as input and the signal sum (N-bit) as output.</t>
   </si>
   <si>
@@ -2268,6 +2286,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity FloatingPointAdder is Generic ( N : natural := 8 ); Port ( A : in STD_LOGIC_VECTOR (N-1 downto 0); B : in STD_LOGIC_VECTOR (N-1 downto 0); Sum : out STD_LOGIC_VECTOR (N-1 downto 0)); end FloatingPointAdder; architecture Behavioral of FloatingPointAdder is begin Sum &lt;= A * B; end Behavioral;</t>
   </si>
   <si>
+    <t>Non effettua la somma tra numeri in virgola mobile</t>
+  </si>
+  <si>
     <t>Design a 4-bit digital comparator</t>
   </si>
   <si>
@@ -2286,6 +2307,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity 2-to-1_Multiplexer is Port ( Data0 : in STD_LOGIC; Data1 : in STD_LOGIC; Select : in STD_LOGIC; Data_Out : out STD_LOGIC); end 2-to-1_Multiplexer; architecture Behavioral of 2-to-1_Multiplexer is begin Data_Out &lt;= Data0 when Select = '1' else '0'; end Behavioral;</t>
   </si>
   <si>
+    <t>non un vero multiplexer</t>
+  </si>
+  <si>
     <t>Implement an SPI master using a process.</t>
   </si>
   <si>
@@ -2295,6 +2319,9 @@
     <t>process(clk_period, reset_period, reset_value) begin if rising_edge(clk_period) then if reset_period = '1' then clock &lt;= '0'; reset &lt;= '1'; elsif reset_period = '0' then clock &lt;= '0'; reset &lt;= '0'; end if; end if; end process;</t>
   </si>
   <si>
+    <t>Non è un master SPI</t>
+  </si>
+  <si>
     <t>Detect falling edge of a signal using a process.</t>
   </si>
   <si>
@@ -2313,6 +2340,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity UniversalShiftRegister is Generic ( P : natural := 8 ); Port ( Clock : in STD_LOGIC; ShiftEnable : in STD_LOGIC; ShiftDirection : in STD_LOGIC; SerialIn : in STD_LOGIC; ParallelOut : out STD_LOGIC; SerialOut : out STD_LOGIC); end UniversalShiftRegister; architecture Behavioral of UniversalShiftRegister is signal shift_reg : std_logic_vector(P-1 downto 0); begin process (Clock, ShiftEnable, ShiftDirection) begin if ShiftEnable = '1' then shift_reg &lt;= (others =&gt; '0'); elsif ShiftDirection = '1' then shift_reg &lt;= (others =&gt; '0'); elsif ShiftDirection = '0' then shift_reg &lt;= (others =&gt; '0'); end if ; end process ; parallel_out &lt;= shift_reg(P-1 downto 0); serial_out &lt;= shift_reg(P-2 downto 0); end Behavioral;</t>
   </si>
   <si>
+    <t>Non vi è alcuna logica di shift</t>
+  </si>
+  <si>
     <t>Implement a basic priority encoder</t>
   </si>
   <si>
@@ -2331,6 +2361,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity ring_counter is Generic (N : natural := 8); Port ( Clock : in STD_LOGIC; Reset : in STD_LOGIC; Ring_Count : out STD_LOGIC_VECTOR (N-1 downto 0)); end ring_counter; architecture Behavioral of ring_counter is signal ring_count : std_logic_vector(N-1 downto 0); begin process (Clock, Reset) begin if Reset = '1' then ring_count &lt;= (others =&gt; '0'); elsif rising_edge(Clock) then ring_count &lt;= ring_count + 1; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non si comporta in maniera circolare</t>
+  </si>
+  <si>
     <t>Implement a binary to BCD converter</t>
   </si>
   <si>
@@ -2340,6 +2373,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity BCDConverter is Generic (log2B-1 downto 0) Port ( A : in STD_LOGIC_VECTOR (log2B-1 downto 0); B : in STD_LOGIC_VECTOR (log2B-1 downto 0); BCD : out STD_LOGIC_VECTOR (log2B-1 downto 0)); end BCDConverter; architecture Behavioral of BCDConverter is begin process (A, B) variable temp : STD_LOGIC_VECTOR (log2B-1 downto 0); begin temp := A; BCD(log2B-1 downto 0) := temp; BCD(log2B-1 downto 0) := temp; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non fa la conversione</t>
+  </si>
+  <si>
     <t>Create a pulse generator that outputs a single pulse every N clock cycles</t>
   </si>
   <si>
@@ -2349,6 +2385,9 @@
     <t>component pulse_generator is port ( clock_frequency_in : in STD_LOGIC_VECTOR (0 to 100); pulse_frequency_out : in STD_LOGIC_VECTOR (0 to 100); pulse_frequency_out &lt;= clock_frequency_in + 1; pulse_frequency_out &lt;= pulse_frequency_out - 1 ); end component;</t>
   </si>
   <si>
+    <t>Non è quello che ho chiesto</t>
+  </si>
+  <si>
     <t>Define a binary to BCD converter of (N/3)+1-digit with the signal binary_value (N-bit) as input and the signal BCD_value ((N/3)+1-digit) as output.</t>
   </si>
   <si>
@@ -2367,6 +2406,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity Dual_Port_RAM is Generic ( K : natural := 8; L : natural := 16 ); Port ( Clock : in STD_LOGIC; Write_Enable : in STD_LOGIC; Read_Enable : in STD_LOGIC; Write_Address : in STD_LOGIC_VECTOR (log2K-1 downto 0); Read_Address : in STD_LOGIC_VECTOR (log2K-1 downto 0); Data_In : in STD_LOGIC_VECTOR (L-1 downto 0); Data_Out : out STD_LOGIC_VECTOR (L-1 downto 0)); end Dual_Port_RAM; architecture Behavioral of Dual_Port_RAM is signal Data_In, Data_Out_L, Data_In_L, Data_Out_L_L, Data_Out_L_L_in : STD_LOGIC_VECTOR (L-1 downto 0); begin process (Clock, Write_Enable, Read_Enable, Write_Address, Read_Address) begin if Write_Address = '1' then Data_In &lt;= Data_In_L; Data_Out_L &lt;= Data_Out_L_L; Data_Out_L_L &lt;= Data_Out_L_L_in; end if ; end process ; Data_Out &lt;= Data_In; Data_Out_L &lt;= Data_Out; end Behavioral;</t>
   </si>
   <si>
+    <t>Non ci sono alcune cose. ma l'idea tutto sommato c'è</t>
+  </si>
+  <si>
     <t>Generate a dual-port memory of K x L with the signals clock, write, address_w (log2K-bit), address_r (log2K-bit), and data_write (L-bit) as input and the signal data_read (L-bit) as output.</t>
   </si>
   <si>
@@ -2376,6 +2418,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity Dual_Port_Memory is Generic ( K : natural := 8; L : natural := 16 ); Port ( Clock : in STD_LOGIC; Write : in STD_LOGIC; Address_W : in STD_LOGIC_VECTOR (log2K-1 downto 0); Address_R : in STD_LOGIC_VECTOR (log2K-1 downto 0); Data_Write : in STD_LOGIC_VECTOR (L-1 downto 0); Data_Read : out STD_LOGIC_VECTOR (L-1 downto 0)); end Dual_Port_Memory; architecture Behavioral of Dual_Port_Memory is signal data_read : STD_LOGIC_VECTOR (L-1 downto 0); begin process (Clock, Write) begin if rising_edge(Clock) then if Write = '1' then Data_Read &lt;= Data_Write; Data_Write &lt;= Data_Write + 1; elsif Write = '0' then Data_Read &lt;= Data_Write - 1; Data_Write &lt;= Data_Write - 1; end if ; end if ; end process ; Data_Read &lt;= Data_Read + 1; end Behavioral;</t>
   </si>
   <si>
+    <t>Più o meno</t>
+  </si>
+  <si>
     <t>Create a 4-bit binary counter that increments on each clock pulse and resets asynchronously</t>
   </si>
   <si>
@@ -2383,6 +2428,9 @@
   </si>
   <si>
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity binary_counter is Port ( Clock : in STD_LOGIC; Increment : in STD_LOGIC; Reset : in STD_LOGIC; Data : out STD_LOGIC_VECTOR (3 downto 0)); end binary_counter; architecture Behavioral of binary_counter is signal count : unsigned(3 downto 0) := (others =&gt; '0'); begin process (Clock, Increment) begin if rising_edge(Clock) then if Reset = '1' then count &lt;= (others =&gt; '0'); elsif Count = unsigned(3 downto 0) then count &lt;= (others =&gt; '0'); end if ; end if ; end process ; Data &lt;= count; end Behavioral;</t>
+  </si>
+  <si>
+    <t>Non incrementa il contatore</t>
   </si>
   <si>
     <t>Define a finite impulse response filter of N-bit with the signals clock, reset, data_in (N-bit), and coefficients (M x N-bit) as input and the signal filtered_output (N-bit) as output.</t>
@@ -3310,8 +3358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="H245" sqref="H245"/>
+    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
+      <selection activeCell="H264" sqref="H264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9442,16 +9490,19 @@
       <c r="G244">
         <v>0</v>
       </c>
+      <c r="H244" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="245" spans="1:8">
       <c r="A245" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B245" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C245" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="D245">
         <v>0</v>
@@ -9465,16 +9516,19 @@
       <c r="G245">
         <v>0</v>
       </c>
+      <c r="H245" t="s">
+        <v>731</v>
+      </c>
     </row>
     <row r="246" spans="1:8">
       <c r="A246" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="B246" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="C246" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="D246">
         <v>0</v>
@@ -9488,16 +9542,19 @@
       <c r="G246">
         <v>0</v>
       </c>
+      <c r="H246" t="s">
+        <v>735</v>
+      </c>
     </row>
     <row r="247" spans="1:8">
       <c r="A247" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="B247" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="C247" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
       <c r="D247">
         <v>0</v>
@@ -9511,16 +9568,19 @@
       <c r="G247">
         <v>0</v>
       </c>
+      <c r="H247" t="s">
+        <v>739</v>
+      </c>
     </row>
     <row r="248" spans="1:8">
       <c r="A248" t="s">
-        <v>736</v>
+        <v>740</v>
       </c>
       <c r="B248" t="s">
-        <v>737</v>
+        <v>741</v>
       </c>
       <c r="C248" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
       <c r="D248">
         <v>0</v>
@@ -9534,16 +9594,19 @@
       <c r="G248">
         <v>0</v>
       </c>
+      <c r="H248" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="249" spans="1:8">
       <c r="A249" t="s">
-        <v>739</v>
+        <v>744</v>
       </c>
       <c r="B249" t="s">
-        <v>740</v>
+        <v>745</v>
       </c>
       <c r="C249" t="s">
-        <v>741</v>
+        <v>746</v>
       </c>
       <c r="D249">
         <v>0</v>
@@ -9557,16 +9620,19 @@
       <c r="G249">
         <v>0</v>
       </c>
+      <c r="H249" t="s">
+        <v>747</v>
+      </c>
     </row>
     <row r="250" spans="1:8">
       <c r="A250" t="s">
-        <v>742</v>
+        <v>748</v>
       </c>
       <c r="B250" t="s">
-        <v>743</v>
+        <v>749</v>
       </c>
       <c r="C250" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="D250">
         <v>0</v>
@@ -9580,16 +9646,19 @@
       <c r="G250">
         <v>0</v>
       </c>
+      <c r="H250" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="251" spans="1:8">
       <c r="A251" t="s">
-        <v>745</v>
+        <v>752</v>
       </c>
       <c r="B251" t="s">
-        <v>746</v>
+        <v>753</v>
       </c>
       <c r="C251" t="s">
-        <v>747</v>
+        <v>754</v>
       </c>
       <c r="D251">
         <v>0</v>
@@ -9603,16 +9672,19 @@
       <c r="G251">
         <v>0</v>
       </c>
+      <c r="H251" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="252" spans="1:8">
       <c r="A252" t="s">
-        <v>748</v>
+        <v>755</v>
       </c>
       <c r="B252" t="s">
-        <v>749</v>
+        <v>756</v>
       </c>
       <c r="C252" t="s">
-        <v>750</v>
+        <v>757</v>
       </c>
       <c r="D252">
         <v>0</v>
@@ -9626,16 +9698,19 @@
       <c r="G252">
         <v>0</v>
       </c>
+      <c r="H252" t="s">
+        <v>758</v>
+      </c>
     </row>
     <row r="253" spans="1:8">
       <c r="A253" t="s">
-        <v>751</v>
+        <v>759</v>
       </c>
       <c r="B253" t="s">
-        <v>752</v>
+        <v>760</v>
       </c>
       <c r="C253" t="s">
-        <v>753</v>
+        <v>761</v>
       </c>
       <c r="D253">
         <v>0</v>
@@ -9649,16 +9724,19 @@
       <c r="G253">
         <v>0</v>
       </c>
+      <c r="H253" t="s">
+        <v>762</v>
+      </c>
     </row>
     <row r="254" spans="1:8">
       <c r="A254" t="s">
-        <v>754</v>
+        <v>763</v>
       </c>
       <c r="B254" t="s">
-        <v>755</v>
+        <v>764</v>
       </c>
       <c r="C254" t="s">
-        <v>756</v>
+        <v>765</v>
       </c>
       <c r="D254">
         <v>0</v>
@@ -9672,16 +9750,19 @@
       <c r="G254">
         <v>0</v>
       </c>
+      <c r="H254" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="255" spans="1:8">
       <c r="A255" t="s">
-        <v>757</v>
+        <v>766</v>
       </c>
       <c r="B255" t="s">
-        <v>758</v>
+        <v>767</v>
       </c>
       <c r="C255" t="s">
-        <v>759</v>
+        <v>768</v>
       </c>
       <c r="D255">
         <v>0</v>
@@ -9695,16 +9776,19 @@
       <c r="G255">
         <v>0</v>
       </c>
+      <c r="H255" t="s">
+        <v>769</v>
+      </c>
     </row>
     <row r="256" spans="1:8">
       <c r="A256" t="s">
-        <v>760</v>
+        <v>770</v>
       </c>
       <c r="B256" t="s">
-        <v>761</v>
+        <v>771</v>
       </c>
       <c r="C256" t="s">
-        <v>762</v>
+        <v>772</v>
       </c>
       <c r="D256">
         <v>0</v>
@@ -9718,16 +9802,19 @@
       <c r="G256">
         <v>0</v>
       </c>
-    </row>
-    <row r="257" spans="1:7">
+      <c r="H256" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8">
       <c r="A257" t="s">
-        <v>763</v>
+        <v>773</v>
       </c>
       <c r="B257" t="s">
-        <v>764</v>
+        <v>774</v>
       </c>
       <c r="C257" t="s">
-        <v>765</v>
+        <v>775</v>
       </c>
       <c r="D257">
         <v>0</v>
@@ -9741,16 +9828,19 @@
       <c r="G257">
         <v>0</v>
       </c>
-    </row>
-    <row r="258" spans="1:7">
+      <c r="H257" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8">
       <c r="A258" t="s">
-        <v>766</v>
+        <v>777</v>
       </c>
       <c r="B258" t="s">
-        <v>767</v>
+        <v>778</v>
       </c>
       <c r="C258" t="s">
-        <v>768</v>
+        <v>779</v>
       </c>
       <c r="D258">
         <v>0</v>
@@ -9764,16 +9854,19 @@
       <c r="G258">
         <v>0</v>
       </c>
-    </row>
-    <row r="259" spans="1:7">
+      <c r="H258" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8">
       <c r="A259" t="s">
-        <v>769</v>
+        <v>781</v>
       </c>
       <c r="B259" t="s">
-        <v>770</v>
+        <v>782</v>
       </c>
       <c r="C259" t="s">
-        <v>771</v>
+        <v>783</v>
       </c>
       <c r="D259">
         <v>0</v>
@@ -9787,16 +9880,19 @@
       <c r="G259">
         <v>0</v>
       </c>
-    </row>
-    <row r="260" spans="1:7">
+      <c r="H259" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8">
       <c r="A260" t="s">
-        <v>772</v>
+        <v>785</v>
       </c>
       <c r="B260" t="s">
-        <v>773</v>
+        <v>786</v>
       </c>
       <c r="C260" t="s">
-        <v>774</v>
+        <v>787</v>
       </c>
       <c r="D260">
         <v>0</v>
@@ -9810,16 +9906,19 @@
       <c r="G260">
         <v>0</v>
       </c>
-    </row>
-    <row r="261" spans="1:7">
+      <c r="H260" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8">
       <c r="A261" t="s">
-        <v>775</v>
+        <v>788</v>
       </c>
       <c r="B261" t="s">
-        <v>776</v>
+        <v>789</v>
       </c>
       <c r="C261" t="s">
-        <v>777</v>
+        <v>790</v>
       </c>
       <c r="D261">
         <v>0</v>
@@ -9831,18 +9930,21 @@
         <v>0.52194715692300564</v>
       </c>
       <c r="G261">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="262" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H261" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8">
       <c r="A262" t="s">
-        <v>778</v>
+        <v>792</v>
       </c>
       <c r="B262" t="s">
-        <v>779</v>
+        <v>793</v>
       </c>
       <c r="C262" t="s">
-        <v>780</v>
+        <v>794</v>
       </c>
       <c r="D262">
         <v>0</v>
@@ -9854,18 +9956,21 @@
         <v>0.60069532508803947</v>
       </c>
       <c r="G262">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="263" spans="1:7">
+        <v>1</v>
+      </c>
+      <c r="H262" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8">
       <c r="A263" t="s">
-        <v>781</v>
+        <v>796</v>
       </c>
       <c r="B263" t="s">
-        <v>782</v>
+        <v>797</v>
       </c>
       <c r="C263" t="s">
-        <v>783</v>
+        <v>798</v>
       </c>
       <c r="D263">
         <v>0</v>
@@ -9879,16 +9984,19 @@
       <c r="G263">
         <v>0</v>
       </c>
-    </row>
-    <row r="264" spans="1:7">
+      <c r="H263" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8">
       <c r="A264" t="s">
-        <v>784</v>
+        <v>800</v>
       </c>
       <c r="B264" t="s">
-        <v>785</v>
+        <v>801</v>
       </c>
       <c r="C264" t="s">
-        <v>786</v>
+        <v>802</v>
       </c>
       <c r="D264">
         <v>0</v>
@@ -9903,15 +10011,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:7">
+    <row r="265" spans="1:8">
       <c r="A265" t="s">
-        <v>787</v>
+        <v>803</v>
       </c>
       <c r="B265" t="s">
-        <v>788</v>
+        <v>804</v>
       </c>
       <c r="C265" t="s">
-        <v>789</v>
+        <v>805</v>
       </c>
       <c r="D265">
         <v>0</v>
@@ -9926,15 +10034,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:7">
+    <row r="266" spans="1:8">
       <c r="A266" t="s">
-        <v>790</v>
+        <v>806</v>
       </c>
       <c r="B266" t="s">
-        <v>791</v>
+        <v>807</v>
       </c>
       <c r="C266" t="s">
-        <v>792</v>
+        <v>808</v>
       </c>
       <c r="D266">
         <v>0</v>
@@ -9949,15 +10057,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:7">
+    <row r="267" spans="1:8">
       <c r="A267" t="s">
-        <v>793</v>
+        <v>809</v>
       </c>
       <c r="B267" t="s">
-        <v>794</v>
+        <v>810</v>
       </c>
       <c r="C267" t="s">
-        <v>795</v>
+        <v>811</v>
       </c>
       <c r="D267">
         <v>0</v>
@@ -9972,15 +10080,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:7">
+    <row r="268" spans="1:8">
       <c r="A268" t="s">
-        <v>796</v>
+        <v>812</v>
       </c>
       <c r="B268" t="s">
-        <v>797</v>
+        <v>813</v>
       </c>
       <c r="C268" t="s">
-        <v>798</v>
+        <v>814</v>
       </c>
       <c r="D268">
         <v>0</v>
@@ -9995,15 +10103,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:7">
+    <row r="269" spans="1:8">
       <c r="A269" t="s">
-        <v>799</v>
+        <v>815</v>
       </c>
       <c r="B269" t="s">
-        <v>800</v>
+        <v>816</v>
       </c>
       <c r="C269" t="s">
-        <v>801</v>
+        <v>817</v>
       </c>
       <c r="D269">
         <v>0</v>
@@ -10018,15 +10126,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:7">
+    <row r="270" spans="1:8">
       <c r="A270" t="s">
-        <v>802</v>
+        <v>818</v>
       </c>
       <c r="B270" t="s">
-        <v>803</v>
+        <v>819</v>
       </c>
       <c r="C270" t="s">
-        <v>804</v>
+        <v>820</v>
       </c>
       <c r="D270">
         <v>0</v>
@@ -10041,15 +10149,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:7">
+    <row r="271" spans="1:8">
       <c r="A271" t="s">
-        <v>805</v>
+        <v>821</v>
       </c>
       <c r="B271" t="s">
-        <v>806</v>
+        <v>822</v>
       </c>
       <c r="C271" t="s">
-        <v>807</v>
+        <v>823</v>
       </c>
       <c r="D271">
         <v>0</v>
@@ -10064,15 +10172,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:7">
+    <row r="272" spans="1:8">
       <c r="A272" t="s">
-        <v>808</v>
+        <v>824</v>
       </c>
       <c r="B272" t="s">
-        <v>809</v>
+        <v>825</v>
       </c>
       <c r="C272" t="s">
-        <v>810</v>
+        <v>826</v>
       </c>
       <c r="D272">
         <v>0</v>
@@ -10089,13 +10197,13 @@
     </row>
     <row r="273" spans="1:8">
       <c r="A273" t="s">
-        <v>811</v>
+        <v>827</v>
       </c>
       <c r="B273" t="s">
-        <v>812</v>
+        <v>828</v>
       </c>
       <c r="C273" t="s">
-        <v>813</v>
+        <v>829</v>
       </c>
       <c r="D273">
         <v>0</v>
@@ -10112,13 +10220,13 @@
     </row>
     <row r="274" spans="1:8">
       <c r="A274" t="s">
-        <v>814</v>
+        <v>830</v>
       </c>
       <c r="B274" t="s">
-        <v>815</v>
+        <v>831</v>
       </c>
       <c r="C274" t="s">
-        <v>816</v>
+        <v>832</v>
       </c>
       <c r="D274">
         <v>0</v>
@@ -10135,13 +10243,13 @@
     </row>
     <row r="275" spans="1:8">
       <c r="A275" t="s">
-        <v>817</v>
+        <v>833</v>
       </c>
       <c r="B275" t="s">
-        <v>818</v>
+        <v>834</v>
       </c>
       <c r="C275" t="s">
-        <v>819</v>
+        <v>835</v>
       </c>
       <c r="D275">
         <v>0</v>
@@ -10158,13 +10266,13 @@
     </row>
     <row r="276" spans="1:8">
       <c r="A276" t="s">
-        <v>820</v>
+        <v>836</v>
       </c>
       <c r="B276" t="s">
-        <v>821</v>
+        <v>837</v>
       </c>
       <c r="C276" t="s">
-        <v>822</v>
+        <v>838</v>
       </c>
       <c r="D276">
         <v>0</v>
@@ -10181,13 +10289,13 @@
     </row>
     <row r="277" spans="1:8">
       <c r="A277" t="s">
-        <v>823</v>
+        <v>839</v>
       </c>
       <c r="B277" t="s">
-        <v>824</v>
+        <v>840</v>
       </c>
       <c r="C277" t="s">
-        <v>825</v>
+        <v>841</v>
       </c>
       <c r="D277">
         <v>0</v>
@@ -10204,13 +10312,13 @@
     </row>
     <row r="278" spans="1:8">
       <c r="A278" t="s">
-        <v>826</v>
+        <v>842</v>
       </c>
       <c r="B278" t="s">
-        <v>827</v>
+        <v>843</v>
       </c>
       <c r="C278" t="s">
-        <v>828</v>
+        <v>844</v>
       </c>
       <c r="D278">
         <v>0</v>
@@ -10227,10 +10335,10 @@
     </row>
     <row r="279" spans="1:8">
       <c r="A279" t="s">
-        <v>829</v>
+        <v>845</v>
       </c>
       <c r="B279" t="s">
-        <v>830</v>
+        <v>846</v>
       </c>
       <c r="C279" t="s">
         <v>53</v>
@@ -10253,13 +10361,13 @@
     </row>
     <row r="280" spans="1:8">
       <c r="A280" t="s">
-        <v>831</v>
+        <v>847</v>
       </c>
       <c r="B280" t="s">
-        <v>832</v>
+        <v>848</v>
       </c>
       <c r="C280" t="s">
-        <v>833</v>
+        <v>849</v>
       </c>
       <c r="D280">
         <v>0</v>
@@ -10276,13 +10384,13 @@
     </row>
     <row r="281" spans="1:8">
       <c r="A281" t="s">
-        <v>834</v>
+        <v>850</v>
       </c>
       <c r="B281" t="s">
-        <v>835</v>
+        <v>851</v>
       </c>
       <c r="C281" t="s">
-        <v>836</v>
+        <v>852</v>
       </c>
       <c r="D281">
         <v>0</v>
@@ -10299,13 +10407,13 @@
     </row>
     <row r="282" spans="1:8">
       <c r="A282" t="s">
-        <v>837</v>
+        <v>853</v>
       </c>
       <c r="B282" t="s">
-        <v>838</v>
+        <v>854</v>
       </c>
       <c r="C282" t="s">
-        <v>839</v>
+        <v>855</v>
       </c>
       <c r="D282">
         <v>0</v>
@@ -10322,13 +10430,13 @@
     </row>
     <row r="283" spans="1:8">
       <c r="A283" t="s">
-        <v>840</v>
+        <v>856</v>
       </c>
       <c r="B283" t="s">
-        <v>841</v>
+        <v>857</v>
       </c>
       <c r="C283" t="s">
-        <v>842</v>
+        <v>858</v>
       </c>
       <c r="D283">
         <v>0</v>
@@ -10345,13 +10453,13 @@
     </row>
     <row r="284" spans="1:8">
       <c r="A284" t="s">
-        <v>843</v>
+        <v>859</v>
       </c>
       <c r="B284" t="s">
-        <v>844</v>
+        <v>860</v>
       </c>
       <c r="C284" t="s">
-        <v>845</v>
+        <v>861</v>
       </c>
       <c r="D284">
         <v>0</v>
@@ -10368,13 +10476,13 @@
     </row>
     <row r="285" spans="1:8">
       <c r="A285" t="s">
-        <v>846</v>
+        <v>862</v>
       </c>
       <c r="B285" t="s">
-        <v>847</v>
+        <v>863</v>
       </c>
       <c r="C285" t="s">
-        <v>848</v>
+        <v>864</v>
       </c>
       <c r="D285">
         <v>0</v>
@@ -10391,13 +10499,13 @@
     </row>
     <row r="286" spans="1:8">
       <c r="A286" t="s">
-        <v>849</v>
+        <v>865</v>
       </c>
       <c r="B286" t="s">
-        <v>850</v>
+        <v>866</v>
       </c>
       <c r="C286" t="s">
-        <v>851</v>
+        <v>867</v>
       </c>
       <c r="D286">
         <v>0</v>
@@ -10414,13 +10522,13 @@
     </row>
     <row r="287" spans="1:8">
       <c r="A287" t="s">
-        <v>852</v>
+        <v>868</v>
       </c>
       <c r="B287" t="s">
-        <v>853</v>
+        <v>869</v>
       </c>
       <c r="C287" t="s">
-        <v>854</v>
+        <v>870</v>
       </c>
       <c r="D287">
         <v>0</v>
@@ -10437,13 +10545,13 @@
     </row>
     <row r="288" spans="1:8">
       <c r="A288" t="s">
-        <v>855</v>
+        <v>871</v>
       </c>
       <c r="B288" t="s">
-        <v>856</v>
+        <v>872</v>
       </c>
       <c r="C288" t="s">
-        <v>857</v>
+        <v>873</v>
       </c>
       <c r="D288">
         <v>0</v>
@@ -10460,10 +10568,10 @@
     </row>
     <row r="289" spans="1:8">
       <c r="A289" t="s">
-        <v>858</v>
+        <v>874</v>
       </c>
       <c r="B289" t="s">
-        <v>859</v>
+        <v>875</v>
       </c>
       <c r="C289" t="s">
         <v>53</v>
@@ -10486,13 +10594,13 @@
     </row>
     <row r="290" spans="1:8">
       <c r="A290" t="s">
-        <v>860</v>
+        <v>876</v>
       </c>
       <c r="B290" t="s">
-        <v>861</v>
+        <v>877</v>
       </c>
       <c r="C290" t="s">
-        <v>862</v>
+        <v>878</v>
       </c>
       <c r="D290">
         <v>0</v>
@@ -10509,13 +10617,13 @@
     </row>
     <row r="291" spans="1:8">
       <c r="A291" t="s">
-        <v>863</v>
+        <v>879</v>
       </c>
       <c r="B291" t="s">
-        <v>864</v>
+        <v>880</v>
       </c>
       <c r="C291" t="s">
-        <v>865</v>
+        <v>881</v>
       </c>
       <c r="D291">
         <v>0</v>
@@ -10532,13 +10640,13 @@
     </row>
     <row r="292" spans="1:8">
       <c r="A292" t="s">
-        <v>866</v>
+        <v>882</v>
       </c>
       <c r="B292" t="s">
-        <v>867</v>
+        <v>883</v>
       </c>
       <c r="C292" t="s">
-        <v>868</v>
+        <v>884</v>
       </c>
       <c r="D292">
         <v>0</v>
@@ -10555,13 +10663,13 @@
     </row>
     <row r="293" spans="1:8">
       <c r="A293" t="s">
-        <v>869</v>
+        <v>885</v>
       </c>
       <c r="B293" t="s">
-        <v>870</v>
+        <v>886</v>
       </c>
       <c r="C293" t="s">
-        <v>870</v>
+        <v>886</v>
       </c>
       <c r="D293">
         <v>1</v>
@@ -10578,13 +10686,13 @@
     </row>
     <row r="294" spans="1:8">
       <c r="A294" t="s">
-        <v>871</v>
+        <v>887</v>
       </c>
       <c r="B294" t="s">
-        <v>872</v>
+        <v>888</v>
       </c>
       <c r="C294" t="s">
-        <v>873</v>
+        <v>889</v>
       </c>
       <c r="D294">
         <v>0</v>
@@ -10601,13 +10709,13 @@
     </row>
     <row r="295" spans="1:8">
       <c r="A295" t="s">
-        <v>874</v>
+        <v>890</v>
       </c>
       <c r="B295" t="s">
-        <v>875</v>
+        <v>891</v>
       </c>
       <c r="C295" t="s">
-        <v>876</v>
+        <v>892</v>
       </c>
       <c r="D295">
         <v>0</v>
@@ -10624,13 +10732,13 @@
     </row>
     <row r="296" spans="1:8">
       <c r="A296" t="s">
-        <v>877</v>
+        <v>893</v>
       </c>
       <c r="B296" t="s">
-        <v>878</v>
+        <v>894</v>
       </c>
       <c r="C296" t="s">
-        <v>879</v>
+        <v>895</v>
       </c>
       <c r="D296">
         <v>0</v>
@@ -10647,10 +10755,10 @@
     </row>
     <row r="297" spans="1:8">
       <c r="A297" t="s">
-        <v>880</v>
+        <v>896</v>
       </c>
       <c r="B297" t="s">
-        <v>881</v>
+        <v>897</v>
       </c>
       <c r="C297" t="s">
         <v>53</v>
@@ -10673,13 +10781,13 @@
     </row>
     <row r="298" spans="1:8">
       <c r="A298" t="s">
-        <v>882</v>
+        <v>898</v>
       </c>
       <c r="B298" t="s">
-        <v>883</v>
+        <v>899</v>
       </c>
       <c r="C298" t="s">
-        <v>884</v>
+        <v>900</v>
       </c>
       <c r="D298">
         <v>0</v>
@@ -10696,10 +10804,10 @@
     </row>
     <row r="299" spans="1:8">
       <c r="A299" t="s">
-        <v>885</v>
+        <v>901</v>
       </c>
       <c r="B299" t="s">
-        <v>886</v>
+        <v>902</v>
       </c>
       <c r="C299" t="s">
         <v>53</v>
@@ -10722,13 +10830,13 @@
     </row>
     <row r="300" spans="1:8">
       <c r="A300" t="s">
-        <v>887</v>
+        <v>903</v>
       </c>
       <c r="B300" t="s">
-        <v>888</v>
+        <v>904</v>
       </c>
       <c r="C300" t="s">
-        <v>889</v>
+        <v>905</v>
       </c>
       <c r="D300">
         <v>0</v>
@@ -10745,13 +10853,13 @@
     </row>
     <row r="301" spans="1:8">
       <c r="A301" t="s">
-        <v>890</v>
+        <v>906</v>
       </c>
       <c r="B301" t="s">
-        <v>891</v>
+        <v>907</v>
       </c>
       <c r="C301" t="s">
-        <v>892</v>
+        <v>908</v>
       </c>
       <c r="D301">
         <v>0</v>
@@ -10768,10 +10876,10 @@
     </row>
     <row r="302" spans="1:8">
       <c r="A302" t="s">
-        <v>893</v>
+        <v>909</v>
       </c>
       <c r="B302" t="s">
-        <v>894</v>
+        <v>910</v>
       </c>
       <c r="C302" t="s">
         <v>53</v>
@@ -10794,13 +10902,13 @@
     </row>
     <row r="303" spans="1:8">
       <c r="A303" t="s">
-        <v>895</v>
+        <v>911</v>
       </c>
       <c r="B303" t="s">
-        <v>896</v>
+        <v>912</v>
       </c>
       <c r="C303" t="s">
-        <v>897</v>
+        <v>913</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -10817,13 +10925,13 @@
     </row>
     <row r="304" spans="1:8">
       <c r="A304" t="s">
-        <v>898</v>
+        <v>914</v>
       </c>
       <c r="B304" t="s">
-        <v>899</v>
+        <v>915</v>
       </c>
       <c r="C304" t="s">
-        <v>900</v>
+        <v>916</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -10840,13 +10948,13 @@
     </row>
     <row r="305" spans="1:8">
       <c r="A305" t="s">
-        <v>901</v>
+        <v>917</v>
       </c>
       <c r="B305" t="s">
-        <v>902</v>
+        <v>918</v>
       </c>
       <c r="C305" t="s">
-        <v>903</v>
+        <v>919</v>
       </c>
       <c r="D305">
         <v>0</v>
@@ -10863,13 +10971,13 @@
     </row>
     <row r="306" spans="1:8">
       <c r="A306" t="s">
-        <v>904</v>
+        <v>920</v>
       </c>
       <c r="B306" t="s">
-        <v>905</v>
+        <v>921</v>
       </c>
       <c r="C306" t="s">
-        <v>906</v>
+        <v>922</v>
       </c>
       <c r="D306">
         <v>0</v>
@@ -10886,13 +10994,13 @@
     </row>
     <row r="307" spans="1:8">
       <c r="A307" t="s">
-        <v>907</v>
+        <v>923</v>
       </c>
       <c r="B307" t="s">
-        <v>908</v>
+        <v>924</v>
       </c>
       <c r="C307" t="s">
-        <v>909</v>
+        <v>925</v>
       </c>
       <c r="D307">
         <v>0</v>
@@ -10909,13 +11017,13 @@
     </row>
     <row r="308" spans="1:8">
       <c r="A308" t="s">
-        <v>910</v>
+        <v>926</v>
       </c>
       <c r="B308" t="s">
-        <v>911</v>
+        <v>927</v>
       </c>
       <c r="C308" t="s">
-        <v>912</v>
+        <v>928</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -10932,13 +11040,13 @@
     </row>
     <row r="309" spans="1:8">
       <c r="A309" t="s">
-        <v>913</v>
+        <v>929</v>
       </c>
       <c r="B309" t="s">
-        <v>914</v>
+        <v>930</v>
       </c>
       <c r="C309" t="s">
-        <v>915</v>
+        <v>931</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -10955,10 +11063,10 @@
     </row>
     <row r="310" spans="1:8">
       <c r="A310" t="s">
-        <v>916</v>
+        <v>932</v>
       </c>
       <c r="B310" t="s">
-        <v>917</v>
+        <v>933</v>
       </c>
       <c r="C310" t="s">
         <v>53</v>
@@ -10981,13 +11089,13 @@
     </row>
     <row r="311" spans="1:8">
       <c r="A311" t="s">
-        <v>918</v>
+        <v>934</v>
       </c>
       <c r="B311" t="s">
-        <v>919</v>
+        <v>935</v>
       </c>
       <c r="C311" t="s">
-        <v>920</v>
+        <v>936</v>
       </c>
       <c r="D311">
         <v>0</v>
@@ -11004,13 +11112,13 @@
     </row>
     <row r="312" spans="1:8">
       <c r="A312" t="s">
-        <v>921</v>
+        <v>937</v>
       </c>
       <c r="B312" t="s">
-        <v>922</v>
+        <v>938</v>
       </c>
       <c r="C312" t="s">
-        <v>923</v>
+        <v>939</v>
       </c>
       <c r="D312">
         <v>0</v>
@@ -11027,13 +11135,13 @@
     </row>
     <row r="313" spans="1:8">
       <c r="A313" t="s">
-        <v>924</v>
+        <v>940</v>
       </c>
       <c r="B313" t="s">
-        <v>925</v>
+        <v>941</v>
       </c>
       <c r="C313" t="s">
-        <v>926</v>
+        <v>942</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -11050,13 +11158,13 @@
     </row>
     <row r="314" spans="1:8">
       <c r="A314" t="s">
-        <v>927</v>
+        <v>943</v>
       </c>
       <c r="B314" t="s">
-        <v>928</v>
+        <v>944</v>
       </c>
       <c r="C314" t="s">
-        <v>929</v>
+        <v>945</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -11073,13 +11181,13 @@
     </row>
     <row r="315" spans="1:8">
       <c r="A315" t="s">
-        <v>930</v>
+        <v>946</v>
       </c>
       <c r="B315" t="s">
-        <v>931</v>
+        <v>947</v>
       </c>
       <c r="C315" t="s">
-        <v>932</v>
+        <v>948</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -11096,13 +11204,13 @@
     </row>
     <row r="316" spans="1:8">
       <c r="A316" t="s">
-        <v>933</v>
+        <v>949</v>
       </c>
       <c r="B316" t="s">
-        <v>934</v>
+        <v>950</v>
       </c>
       <c r="C316" t="s">
-        <v>935</v>
+        <v>951</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -11119,13 +11227,13 @@
     </row>
     <row r="317" spans="1:8">
       <c r="A317" t="s">
-        <v>936</v>
+        <v>952</v>
       </c>
       <c r="B317" t="s">
-        <v>937</v>
+        <v>953</v>
       </c>
       <c r="C317" t="s">
-        <v>938</v>
+        <v>954</v>
       </c>
       <c r="D317">
         <v>0</v>
@@ -11142,13 +11250,13 @@
     </row>
     <row r="318" spans="1:8">
       <c r="A318" t="s">
-        <v>939</v>
+        <v>955</v>
       </c>
       <c r="B318" t="s">
-        <v>940</v>
+        <v>956</v>
       </c>
       <c r="C318" t="s">
-        <v>941</v>
+        <v>957</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -11165,13 +11273,13 @@
     </row>
     <row r="319" spans="1:8">
       <c r="A319" t="s">
-        <v>942</v>
+        <v>958</v>
       </c>
       <c r="B319" t="s">
-        <v>943</v>
+        <v>959</v>
       </c>
       <c r="C319" t="s">
-        <v>944</v>
+        <v>960</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -11188,13 +11296,13 @@
     </row>
     <row r="320" spans="1:8">
       <c r="A320" t="s">
-        <v>945</v>
+        <v>961</v>
       </c>
       <c r="B320" t="s">
-        <v>946</v>
+        <v>962</v>
       </c>
       <c r="C320" t="s">
-        <v>947</v>
+        <v>963</v>
       </c>
       <c r="D320">
         <v>0</v>
@@ -11211,13 +11319,13 @@
     </row>
     <row r="321" spans="1:8">
       <c r="A321" t="s">
-        <v>948</v>
+        <v>964</v>
       </c>
       <c r="B321" t="s">
-        <v>949</v>
+        <v>965</v>
       </c>
       <c r="C321" t="s">
-        <v>950</v>
+        <v>966</v>
       </c>
       <c r="D321">
         <v>0</v>
@@ -11234,13 +11342,13 @@
     </row>
     <row r="322" spans="1:8">
       <c r="A322" t="s">
-        <v>951</v>
+        <v>967</v>
       </c>
       <c r="B322" t="s">
-        <v>952</v>
+        <v>968</v>
       </c>
       <c r="C322" t="s">
-        <v>953</v>
+        <v>969</v>
       </c>
       <c r="D322">
         <v>0</v>
@@ -11257,13 +11365,13 @@
     </row>
     <row r="323" spans="1:8">
       <c r="A323" t="s">
-        <v>954</v>
+        <v>970</v>
       </c>
       <c r="B323" t="s">
-        <v>955</v>
+        <v>971</v>
       </c>
       <c r="C323" t="s">
-        <v>956</v>
+        <v>972</v>
       </c>
       <c r="D323">
         <v>0</v>
@@ -11280,13 +11388,13 @@
     </row>
     <row r="324" spans="1:8">
       <c r="A324" t="s">
-        <v>957</v>
+        <v>973</v>
       </c>
       <c r="B324" t="s">
-        <v>958</v>
+        <v>974</v>
       </c>
       <c r="C324" t="s">
-        <v>959</v>
+        <v>975</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -11303,13 +11411,13 @@
     </row>
     <row r="325" spans="1:8">
       <c r="A325" t="s">
-        <v>960</v>
+        <v>976</v>
       </c>
       <c r="B325" t="s">
-        <v>961</v>
+        <v>977</v>
       </c>
       <c r="C325" t="s">
-        <v>962</v>
+        <v>978</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -11324,18 +11432,18 @@
         <v>0</v>
       </c>
       <c r="H325" t="s">
-        <v>963</v>
+        <v>979</v>
       </c>
     </row>
     <row r="326" spans="1:8">
       <c r="A326" t="s">
-        <v>964</v>
+        <v>980</v>
       </c>
       <c r="B326" t="s">
-        <v>965</v>
+        <v>981</v>
       </c>
       <c r="C326" t="s">
-        <v>965</v>
+        <v>981</v>
       </c>
       <c r="D326">
         <v>1</v>
@@ -11352,13 +11460,13 @@
     </row>
     <row r="327" spans="1:8">
       <c r="A327" t="s">
-        <v>966</v>
+        <v>982</v>
       </c>
       <c r="B327" t="s">
-        <v>967</v>
+        <v>983</v>
       </c>
       <c r="C327" t="s">
-        <v>968</v>
+        <v>984</v>
       </c>
       <c r="D327">
         <v>0</v>

</xml_diff>

<commit_message>
Completate le analisi su codeGPT
</commit_message>
<xml_diff>
--- a/HE/W_in_progress/AnalisiCodeGPT.xlsx
+++ b/HE/W_in_progress/AnalisiCodeGPT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{593FB464-7EC6-4870-B613-74B3C57B8767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DB1C564-68DA-4A95-9EE9-C64242F8A7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="985">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="1010">
   <si>
     <t>IN</t>
   </si>
@@ -2442,6 +2442,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity FiniteFrequencyFilter is Generic ( N : natural := 8 ); Port ( Clock : in STD_LOGIC; Reset : in STD_LOGIC; Data_In : in STD_LOGIC_VECTOR (N-1 downto 0); Coefficients : in STD_LOGIC_VECTOR (M x N-1 downto 0); Filtered_Output : out STD_LOGIC_VECTOR (N-1 downto 0)); end FiniteFrequencyFilter; architecture Behavioral of FiniteFrequencyFilter is signal Filtered_Output : STD_LOGIC_VECTOR (N-1 downto 0); begin process (Clock, Reset) begin if Reset = '1' then Filtered_Output &lt;= Data_In; elsif rising_edge(Clock) then Filtered_Output &lt;= Filtered_In; end if ; end process ; Filtered_Output &lt;= Filtered_Output + Coefficients; end Behavioral;</t>
   </si>
   <si>
+    <t>non è un filtro FIR</t>
+  </si>
+  <si>
     <t>Implement a basic clock gating circuit</t>
   </si>
   <si>
@@ -2460,6 +2463,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity FloatingPointMultiplier is Generic ( N : natural := 8 ); Port ( A : in STD_LOGIC_VECTOR (N-1 downto 0); B : in STD_LOGIC_VECTOR (N-1 downto 0); Product : out STD_LOGIC_VECTOR (N-1 downto 0)); end FloatingPointMultiplier; architecture Behavioral of FloatingPointMultiplier is begin Product &lt;= A * B; end Behavioral;</t>
   </si>
   <si>
+    <t>Struttura di base c'è, non precisissimo ma va bene</t>
+  </si>
+  <si>
     <t>Define a BCD to binary converter of (N/3)+1-digit with the signal BCD_value ((N/3)+1-digit) as input and the signal binary_value (N-bit) as output.</t>
   </si>
   <si>
@@ -2469,6 +2475,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity BCD_to_BinaryConverter is Generic (N : natural := 8); Port ( BCD_Value : in std_logic_vector (N/3)+1-digit ); end BCD_to_BinaryConverter; architecture Behavioral of BCD_to_BinaryConverter is signal binary_value : std_logic_vector (N-1 downto 0); begin process (BCD_Value) begin if rising_edge(BCD_Value) then binary_value &lt;= (others =&gt; '0'); elsif BCD_Value = '1' then binary_value &lt;= (others =&gt; '0'); elsif BCD_Value = '0' then binary_value &lt;= '0'; end if ; end process ; Binary_Value &lt;= binary_value; end Behavioral;</t>
   </si>
   <si>
+    <t>Manca la logica di conversione</t>
+  </si>
+  <si>
     <t>Create a basic frequency meter</t>
   </si>
   <si>
@@ -2478,6 +2487,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity basic_frequency_meter is Port ( Clock : in STD_LOGIC; Reset : in STD_LOGIC; Duty_Cycle : in STD_LOGIC_VECTOR (1 downto 0); Data : out STD_LOGIC_VECTOR (7 downto 0)); end basic_frequency_meter; architecture Behavioral of basic_frequency_meter is signal count : integer range 0 to 7 := 0; begin process (Clock, Reset) begin if Reset = '1' then count &lt;= 0; elsif rising_edge(Clock) then if Count = 7 then count &lt;= 0; end if ; Data &lt;= '0'; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non è un misuratore di frequenza</t>
+  </si>
+  <si>
     <t>Write a digital differentiator of N-bit with the signals clk and input_data (N-bit) as input and the signal differentiated_data (N-bit) as output.</t>
   </si>
   <si>
@@ -2487,6 +2499,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity Digital_Differentiator is Generic(N : natural := 8); Port ( Clk : in STD_LOGIC; Input_Data : in STD_LOGIC_VECTOR (N-1 downto 0); Differentiated_Data : out STD_LOGIC_VECTOR (N-1 downto 0)); end Digital_Differentiator; architecture Behavioral of Digital_Differentiator is signal temp : STD_LOGIC_VECTOR (N-1 downto 0); begin process (Clk, Input_Data) begin if rising_edge(Clk) then temp := Input_Data; Differentiated_Data &lt;= temp; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non fa la differenziazione</t>
+  </si>
+  <si>
     <t>Define a digital integrator of N-bit with the signals clock, reset, and data_in (N-bit) as input and the signal integrated_output (N-bit) as output.</t>
   </si>
   <si>
@@ -2496,6 +2511,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity DigitalIntegrator is Generic(N : natural := 8); Port ( Clock : in STD_LOGIC; Reset : in STD_LOGIC; Data_In : in STD_LOGIC_VECTOR (N-1 downto 0); Integrated_Output : out STD_LOGIC_VECTOR (N-1 downto 0)); end DigitalIntegrator; architecture Behavioral of DigitalIntegrator is signal integrated_output : STD_LOGIC_VECTOR (N-1 downto 0); begin process (Clock, Reset) begin if Reset = '1' then integrated_output &lt;= Data_In; elsif rising_edge(Clock) then integrated_output &lt;= integrated_in; end if ; end process ; integrated_output &lt;= integrated_out; end Behavioral;</t>
   </si>
   <si>
+    <t>Non effettua l'integrazione</t>
+  </si>
+  <si>
     <t>Define a CRC generator of N-bit with the signals data_in (N-bit) and polynomial (M-bit) as input and the signal CRC_value (M-bit) as output.</t>
   </si>
   <si>
@@ -2505,6 +2523,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity CRC_Generator is Generic (N : natural := 8); Port ( Data_In : in STD_LOGIC_VECTOR (N-1 downto 0); Polynomial : in STD_LOGIC_VECTOR (M-1 downto 0); CRC_Value : out STD_LOGIC_VECTOR (M-1 downto 0)); end CRC_Generator; architecture Behavioral of CRC_Generator is begin process (Data_In, Polynomial) variable temp : STD_LOGIC_VECTOR (M-1 downto 0); begin temp := Polynomial; for i in 0 to N-1 loop temp(i) := Data_In(i); if temp(i) = '1' then temp(i) := '0'; else temp(i) := '1'; end if ; end loop ; CRC_Value &lt;= temp; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non implementa un calcolo del CRC valido</t>
+  </si>
+  <si>
     <t>Generate a priority encoder of 2^M-to-M with the signal requests (2^M-bit) as input and the signals encoded (M-bit) and valid as output.</t>
   </si>
   <si>
@@ -2514,6 +2535,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity PriorityEncoder is Generic (2^M-1 downto 0) Port ( Requests : in STD_LOGIC_VECTOR (2**M-1 downto 0); Encoded : out STD_LOGIC_VECTOR (M-1 downto 0)); end PriorityEncoder; architecture Behavioral of PriorityEncoder is begin Encoded &lt;= Requests(2**M-1 downto 0); Valid &lt;= Requests(M-1 downto 0); end Behavioral;</t>
   </si>
   <si>
+    <t>Non è un priority encoder</t>
+  </si>
+  <si>
     <t>Define an unsigned divider of N-bit with the signals dividend (N-bit) and divisor (N-bit) as input and the signals quotient (N-bit) and remainder (N-bit) as output.</t>
   </si>
   <si>
@@ -2523,6 +2547,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity unsigned_divider is Generic(N : natural := 8); Port (Dividend : in signed(N-1 downto 0); Divisor : in signed(N-1 downto 0); Quotient : out signed(N-1 downto 0)); end unsigned_divider; architecture Behavioral of unsigned_divider is begin process (Dividend, Divisor) variable quotient : unsigned(N-1 downto 0); variable remainder : unsigned(N-1 downto 0); begin quotient := quotient + divisor; remainder := remainder + dividend; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non c'è la logica di divisione</t>
+  </si>
+  <si>
     <t>Implement a basic I2C master controller</t>
   </si>
   <si>
@@ -2532,6 +2559,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity I2C_master is Generic ( Clock : in STD_LOGIC; Reset : in STD_LOGIC; Data_In : in STD_LOGIC_VECTOR (1 downto 0); Data_Out : out STD_LOGIC_VECTOR (1 downto 0)); end I2C_master; architecture Behavioral of I2C_master is signal data_out : STD_LOGIC_VECTOR (1 downto 0); begin process (Clock, Reset) begin if Reset = '1' then Data_Out &lt;= '0'; elsif rising_edge(Clock) then Data_Out &lt;= '1'; elsif Data_In = '1' then Data_Out &lt;= '0'; end if ; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non viene gestito il protocollo</t>
+  </si>
+  <si>
     <t>Create a basic DDS (Direct Digital Synthesis) waveform generator</t>
   </si>
   <si>
@@ -2541,6 +2571,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity DDS is Generic ( Clock : in STD_LOGIC; Reset : in STD_LOGIC; Data_In : in STD_LOGIC_VECTOR (1 downto 0); Data_Out : out STD_LOGIC_VECTOR (1 downto 0)); end DDS; architecture Behavioral of DDS is begin process (Clock, Reset) variable temp : STD_LOGIC_VECTOR (1 downto 0); begin temp := (others =&gt; '0'); for i in 0 to 15 loop temp(i) := (others =&gt; '0'); if temp(i) = '1' then temp(i) := '0'; end if ; end loop ; Data_Out &lt;= temp; end process ; end Behavioral;</t>
   </si>
   <si>
+    <t>Non è un DDS</t>
+  </si>
+  <si>
     <t>Write a comparator circuit of K-bit with the signals value1 (K-bit) and value2 (K-bit) as input and the signals greater, equal, and smaller as output.</t>
   </si>
   <si>
@@ -2550,6 +2583,9 @@
     <t>library IEEE; use IEEE.STD_LOGIC_1164.ALL; entity ComparatorCircuit is Generic ( K : natural := 8 ); Port ( Value1 : in STD_LOGIC_VECTOR (K-1 downto 0); Value2 : in STD_LOGIC_VECTOR (K-1 downto 0); Greater : out STD_LOGIC; Equal : out STD_LOGIC); Smaller : out STD_LOGIC; end ComparatorCircuit; architecture Behavioral of ComparatorCircuit is begin Greater &lt;= value1(K-1 downto 0); Equal &lt;= value2(K-1 downto 0); Smaller &lt;= value1(K-1 downto 0); end Behavioral;</t>
   </si>
   <si>
+    <t>Non fa la comparazione</t>
+  </si>
+  <si>
     <t>if rising edge of clk_i; when the case is other_st; set cathodes_dot signal to the concatenation of cathodes and the complement of dot signal</t>
   </si>
   <si>
@@ -2559,6 +2595,9 @@
     <t>case clk_i is when other_st =&gt; cathodes_dot &lt;= dot; when other_st =&gt; cathodes &lt;= cathodes_dot &amp; dot;</t>
   </si>
   <si>
+    <t>Non fa la if iniziale</t>
+  </si>
+  <si>
     <t>declare a signal t_tick_o of type std_logic; S signal is set to the result of an XOR operation between CIN and the XOR operation between OP_A and OP_B.</t>
   </si>
   <si>
@@ -2568,6 +2607,9 @@
     <t>signal t_tick_o : std_logic; S &lt;= CIN or OP_A or OP_B;</t>
   </si>
   <si>
+    <t>Ho chiesto una xor e non una or</t>
+  </si>
+  <si>
     <t>plaintext64 is a std_logic_vector signal of 64 bit initialized to all 0; data_out_reg, data_out_nxt are std_logic signals</t>
   </si>
   <si>
@@ -2610,6 +2652,9 @@
     <t>constant CLK_DIV : integer := 100; constant PRVA : std_logic_vector(DAC_D_OUT_LEN - 1 downto 0);</t>
   </si>
   <si>
+    <t>manca la seconda parte</t>
+  </si>
+  <si>
     <t>i_cs_re_tk is a signal of type std_logic used for something related to rising edge and timekeeping; define an output std_logic_vector of 8 bit called anodes</t>
   </si>
   <si>
@@ -2688,6 +2733,9 @@
     <t>if rising_edge(clk_i) then if( rst_n_i = '0') then i_bit_counter &lt;= DAC_D_IN_LEN - 1; i_cmd_state &lt;= idle_st; i_done &lt;= '0'; i_cs &lt;= '1'; i_sda &lt;= '0'; i_ldac &lt;= '1'; i_ldac_cnt &lt;= 0; end if; end if; end if;</t>
   </si>
   <si>
+    <t>Mancano le ultime richieste</t>
+  </si>
+  <si>
     <t>define the constant count_max_value of type integer and initialize it to CLKIN_freq divided by CLKOUT_freq minus 1; set sda_o signal to i_sda when rst_n_i signal is high, otherwise set it to low</t>
   </si>
   <si>
@@ -2703,6 +2751,9 @@
     <t>wait for 100 ns; wait for 10 ns; signal a : std_logic_vector(0); wait for 10 ns; signal rst_n : std_logic := '1';</t>
   </si>
   <si>
+    <t>manca il process</t>
+  </si>
+  <si>
     <t>unita_operativa is a component with X, Y as input std_logic_vectors of 8 bits, clock, reset as input std_logic signals, loadAQ, shift, loadM, sub, selM, selAQ, selF, count_in as input std_logic signals, count as output std_logic_vector of 3 bits, P as output std_logic_vector of 16 bits; set the first bit of signal_19 to signal_20; map signal done_o to the output port t_done</t>
   </si>
   <si>
@@ -2760,6 +2811,9 @@
     <t>signal current_state : state := secondo;</t>
   </si>
   <si>
+    <t>mancanodelle richieste</t>
+  </si>
+  <si>
     <t>Map sda_i to t_sda, which is an input signal of type std_logic; i_cmd_state is a signal of type cmd_state; component add_round_key is made up of round_key_in, data_in as input std_logic_vector of 64 bit and data_out as output std_logic_vector of 64 bit</t>
   </si>
   <si>
@@ -2775,6 +2829,9 @@
     <t>process(clk_process) begin if rising_edge(clk_process) then if enable = '0' then TbClockA &lt;= count_reg when '0' else count_reg + 1; end if; end if; end process; shift_register &lt;= series_series(count_reg - 1 downto 0);</t>
   </si>
   <si>
+    <t>Non fa le wait</t>
+  </si>
+  <si>
     <t>map data_2_o to t_dac_val_2; if bits 21-14 of BAR signal are equal to hexadecimal '2B'; Use the select statement with GPIO_enable signal to determine whether to output data from GPIO_write signal or keep it high impedance (Z).Report an error message with failure severity if the output signal does not equal '0'</t>
   </si>
   <si>
@@ -2784,6 +2841,9 @@
     <t>data_2_o =&gt; t_dac_val_2; if BAR(21 downto 14) = x"2B" then ; end if; if GPIO_enable = GPIO_write then ; end if; report an error;</t>
   </si>
   <si>
+    <t>Mancano delle richieste</t>
+  </si>
+  <si>
     <t>declare control as a std_logic_vector signal with 2 bit initialized to all '0'; reg_key_in is an input std_logic_vector of 80 bit</t>
   </si>
   <si>
@@ -2820,6 +2880,9 @@
     <t>signal enable : std_logic := '1'; when '0' =&gt; b0 when '1' else a1 when '1' else '-' when others; component counter is port(clk : in std_logic; en : in std_logic; rst : in std_logic; count : in std_logic_vector(3 downto 0); end component;; signal counter : std_logic := '1';</t>
   </si>
   <si>
+    <t>Mancano delle cose di struttura, ma va bene</t>
+  </si>
+  <si>
     <t>Wait until s0_arready is high; enable is an input signal of type std_logic; This is an behavioral architecture for the entity named counter.</t>
   </si>
   <si>
@@ -2844,6 +2907,9 @@
     <t>signal temp_selF : std_logic; case flag_code is when FLAG_1 =&gt; temp_selF(2); when FLAG_2 =&gt; temp_selF(3); when FLAG_3 =&gt; temp_selF(4); when FLAG_4 =&gt; temp_selF(5); when others =&gt; temp_selF &lt;= '0';</t>
   </si>
   <si>
+    <t>Roba in più ma va bene</t>
+  </si>
+  <si>
     <t>u1 is a std_logic signal initialized to '0'; the signal output_val is set to the AND operation between val1 and val2; if the bit 21 to 14 of bar signal are equal to the hexadecimal value "2B"</t>
   </si>
   <si>
@@ -2880,6 +2946,9 @@
     <t>entity TbClockA is port ( clock_in : in STD_LOGIC; reset_in : in STD_LOGIC; addr_strobe_in : in STD_LOGIC; anodes_out : out STD_LOGIC_VECTOR (7 downto 0); cathodes_out : out STD_LOGIC_VECTOR (7 downto 0)); end TbClockA; signal temp_stop_cu : std_logic := 0;; signal temp_stop_cu : std_logic := '0';</t>
   </si>
   <si>
+    <t>Nome sbagliato, ma dichiarazione fatta bene</t>
+  </si>
+  <si>
     <t>Define an entity named ripple_carry with input signals X and Y each of size 8 bits, s_in as a single bit input signal, c_out as a single bit output signal, and Z as an output std_logic_vector of size 8 bits; using the selected signal assignment, the signal c.a_request.be is set to c.sys_master_ctrl_out.be when the signal c.b_request_complete is equal to '1', r.b_request.be when the signal c.b_request_complete is equal to '0', otherwise 'X'; define the ieee standard library</t>
   </si>
   <si>
@@ -2898,6 +2967,9 @@
     <t>i_start_counter &lt;= START_DLY - 1; i_start_counter &lt;= i_start_counter + 1; t_start &lt;= '0'; y &lt;= a0 when ciao = '0' else a1 when ciao = '1' else '-'; end i_start_counter;</t>
   </si>
   <si>
+    <t>Non fa la if</t>
+  </si>
+  <si>
     <t>Generate two signals clkena with two bits, set both bits to '1' if clk2xen is not equal to 0; round_key_temp is a std_logic_vector signal of 64 bit; define the component sbox</t>
   </si>
   <si>
@@ -2950,6 +3022,9 @@
   </si>
   <si>
     <t>case a is when "00" =&gt; y &lt;= "1000"; when "01" =&gt; y &lt;= "0100"; when "10" =&gt; y &lt;= "0010"; when "11" =&gt; y &lt;= "0001"; when others =&gt; y &lt;= (others =&gt; '0'); end case; reg_count_nxt &lt;= clock_multiplier - 1;</t>
+  </si>
+  <si>
+    <t>Ultima richiesta non soddisfatta</t>
   </si>
   <si>
     <t>Set data_1_o output to i_data_1_out when rst_n_i is high, otherwise set it to all '0'; set the signal x to the concatenation of signals y and z; i_data_3_out is a std_logic_vector of DOUT_LEN bits</t>
@@ -3358,8 +3433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
-      <selection activeCell="H264" sqref="H264"/>
+    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="J327" sqref="J327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10010,16 +10085,19 @@
       <c r="G264">
         <v>0</v>
       </c>
+      <c r="H264" t="s">
+        <v>803</v>
+      </c>
     </row>
     <row r="265" spans="1:8">
       <c r="A265" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B265" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C265" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="D265">
         <v>0</v>
@@ -10033,16 +10111,19 @@
       <c r="G265">
         <v>0</v>
       </c>
+      <c r="H265" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="266" spans="1:8">
       <c r="A266" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="B266" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C266" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="D266">
         <v>0</v>
@@ -10054,18 +10135,21 @@
         <v>0.4997417355371902</v>
       </c>
       <c r="G266">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H266" t="s">
+        <v>810</v>
       </c>
     </row>
     <row r="267" spans="1:8">
       <c r="A267" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="B267" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="C267" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="D267">
         <v>0</v>
@@ -10079,16 +10163,19 @@
       <c r="G267">
         <v>0</v>
       </c>
+      <c r="H267" t="s">
+        <v>814</v>
+      </c>
     </row>
     <row r="268" spans="1:8">
       <c r="A268" t="s">
-        <v>812</v>
+        <v>815</v>
       </c>
       <c r="B268" t="s">
-        <v>813</v>
+        <v>816</v>
       </c>
       <c r="C268" t="s">
-        <v>814</v>
+        <v>817</v>
       </c>
       <c r="D268">
         <v>0</v>
@@ -10102,16 +10189,19 @@
       <c r="G268">
         <v>0</v>
       </c>
+      <c r="H268" t="s">
+        <v>818</v>
+      </c>
     </row>
     <row r="269" spans="1:8">
       <c r="A269" t="s">
-        <v>815</v>
+        <v>819</v>
       </c>
       <c r="B269" t="s">
-        <v>816</v>
+        <v>820</v>
       </c>
       <c r="C269" t="s">
-        <v>817</v>
+        <v>821</v>
       </c>
       <c r="D269">
         <v>0</v>
@@ -10125,16 +10215,19 @@
       <c r="G269">
         <v>0</v>
       </c>
+      <c r="H269" t="s">
+        <v>822</v>
+      </c>
     </row>
     <row r="270" spans="1:8">
       <c r="A270" t="s">
-        <v>818</v>
+        <v>823</v>
       </c>
       <c r="B270" t="s">
-        <v>819</v>
+        <v>824</v>
       </c>
       <c r="C270" t="s">
-        <v>820</v>
+        <v>825</v>
       </c>
       <c r="D270">
         <v>0</v>
@@ -10148,16 +10241,19 @@
       <c r="G270">
         <v>0</v>
       </c>
+      <c r="H270" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="271" spans="1:8">
       <c r="A271" t="s">
-        <v>821</v>
+        <v>827</v>
       </c>
       <c r="B271" t="s">
-        <v>822</v>
+        <v>828</v>
       </c>
       <c r="C271" t="s">
-        <v>823</v>
+        <v>829</v>
       </c>
       <c r="D271">
         <v>0</v>
@@ -10171,16 +10267,19 @@
       <c r="G271">
         <v>0</v>
       </c>
+      <c r="H271" t="s">
+        <v>830</v>
+      </c>
     </row>
     <row r="272" spans="1:8">
       <c r="A272" t="s">
-        <v>824</v>
+        <v>831</v>
       </c>
       <c r="B272" t="s">
-        <v>825</v>
+        <v>832</v>
       </c>
       <c r="C272" t="s">
-        <v>826</v>
+        <v>833</v>
       </c>
       <c r="D272">
         <v>0</v>
@@ -10194,16 +10293,19 @@
       <c r="G272">
         <v>0</v>
       </c>
+      <c r="H272" t="s">
+        <v>834</v>
+      </c>
     </row>
     <row r="273" spans="1:8">
       <c r="A273" t="s">
-        <v>827</v>
+        <v>835</v>
       </c>
       <c r="B273" t="s">
-        <v>828</v>
+        <v>836</v>
       </c>
       <c r="C273" t="s">
-        <v>829</v>
+        <v>837</v>
       </c>
       <c r="D273">
         <v>0</v>
@@ -10217,16 +10319,19 @@
       <c r="G273">
         <v>0</v>
       </c>
+      <c r="H273" t="s">
+        <v>838</v>
+      </c>
     </row>
     <row r="274" spans="1:8">
       <c r="A274" t="s">
-        <v>830</v>
+        <v>839</v>
       </c>
       <c r="B274" t="s">
-        <v>831</v>
+        <v>840</v>
       </c>
       <c r="C274" t="s">
-        <v>832</v>
+        <v>841</v>
       </c>
       <c r="D274">
         <v>0</v>
@@ -10240,16 +10345,19 @@
       <c r="G274">
         <v>0</v>
       </c>
+      <c r="H274" t="s">
+        <v>842</v>
+      </c>
     </row>
     <row r="275" spans="1:8">
       <c r="A275" t="s">
-        <v>833</v>
+        <v>843</v>
       </c>
       <c r="B275" t="s">
-        <v>834</v>
+        <v>844</v>
       </c>
       <c r="C275" t="s">
-        <v>835</v>
+        <v>845</v>
       </c>
       <c r="D275">
         <v>0</v>
@@ -10263,16 +10371,19 @@
       <c r="G275">
         <v>0</v>
       </c>
+      <c r="H275" t="s">
+        <v>846</v>
+      </c>
     </row>
     <row r="276" spans="1:8">
       <c r="A276" t="s">
-        <v>836</v>
+        <v>847</v>
       </c>
       <c r="B276" t="s">
-        <v>837</v>
+        <v>848</v>
       </c>
       <c r="C276" t="s">
-        <v>838</v>
+        <v>849</v>
       </c>
       <c r="D276">
         <v>0</v>
@@ -10286,16 +10397,19 @@
       <c r="G276">
         <v>0</v>
       </c>
+      <c r="H276" t="s">
+        <v>850</v>
+      </c>
     </row>
     <row r="277" spans="1:8">
       <c r="A277" t="s">
-        <v>839</v>
+        <v>851</v>
       </c>
       <c r="B277" t="s">
-        <v>840</v>
+        <v>852</v>
       </c>
       <c r="C277" t="s">
-        <v>841</v>
+        <v>853</v>
       </c>
       <c r="D277">
         <v>0</v>
@@ -10309,16 +10423,19 @@
       <c r="G277">
         <v>0</v>
       </c>
+      <c r="H277" t="s">
+        <v>854</v>
+      </c>
     </row>
     <row r="278" spans="1:8">
       <c r="A278" t="s">
-        <v>842</v>
+        <v>855</v>
       </c>
       <c r="B278" t="s">
-        <v>843</v>
+        <v>856</v>
       </c>
       <c r="C278" t="s">
-        <v>844</v>
+        <v>857</v>
       </c>
       <c r="D278">
         <v>0</v>
@@ -10332,13 +10449,16 @@
       <c r="G278">
         <v>0</v>
       </c>
+      <c r="H278" t="s">
+        <v>858</v>
+      </c>
     </row>
     <row r="279" spans="1:8">
       <c r="A279" t="s">
-        <v>845</v>
+        <v>859</v>
       </c>
       <c r="B279" t="s">
-        <v>846</v>
+        <v>860</v>
       </c>
       <c r="C279" t="s">
         <v>53</v>
@@ -10361,13 +10481,13 @@
     </row>
     <row r="280" spans="1:8">
       <c r="A280" t="s">
-        <v>847</v>
+        <v>861</v>
       </c>
       <c r="B280" t="s">
-        <v>848</v>
+        <v>862</v>
       </c>
       <c r="C280" t="s">
-        <v>849</v>
+        <v>863</v>
       </c>
       <c r="D280">
         <v>0</v>
@@ -10379,18 +10499,21 @@
         <v>0.74125709678503038</v>
       </c>
       <c r="G280">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H280" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="281" spans="1:8">
       <c r="A281" t="s">
-        <v>850</v>
+        <v>864</v>
       </c>
       <c r="B281" t="s">
-        <v>851</v>
+        <v>865</v>
       </c>
       <c r="C281" t="s">
-        <v>852</v>
+        <v>866</v>
       </c>
       <c r="D281">
         <v>0</v>
@@ -10404,16 +10527,19 @@
       <c r="G281">
         <v>0</v>
       </c>
+      <c r="H281" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="282" spans="1:8">
       <c r="A282" t="s">
-        <v>853</v>
+        <v>867</v>
       </c>
       <c r="B282" t="s">
-        <v>854</v>
+        <v>868</v>
       </c>
       <c r="C282" t="s">
-        <v>855</v>
+        <v>869</v>
       </c>
       <c r="D282">
         <v>0</v>
@@ -10425,18 +10551,18 @@
         <v>0.95492485549132944</v>
       </c>
       <c r="G282">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="283" spans="1:8">
       <c r="A283" t="s">
-        <v>856</v>
+        <v>870</v>
       </c>
       <c r="B283" t="s">
-        <v>857</v>
+        <v>871</v>
       </c>
       <c r="C283" t="s">
-        <v>858</v>
+        <v>872</v>
       </c>
       <c r="D283">
         <v>0</v>
@@ -10450,16 +10576,19 @@
       <c r="G283">
         <v>0</v>
       </c>
+      <c r="H283" t="s">
+        <v>873</v>
+      </c>
     </row>
     <row r="284" spans="1:8">
       <c r="A284" t="s">
-        <v>859</v>
+        <v>874</v>
       </c>
       <c r="B284" t="s">
-        <v>860</v>
+        <v>875</v>
       </c>
       <c r="C284" t="s">
-        <v>861</v>
+        <v>876</v>
       </c>
       <c r="D284">
         <v>0</v>
@@ -10473,16 +10602,19 @@
       <c r="G284">
         <v>0</v>
       </c>
+      <c r="H284" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="285" spans="1:8">
       <c r="A285" t="s">
-        <v>862</v>
+        <v>877</v>
       </c>
       <c r="B285" t="s">
-        <v>863</v>
+        <v>878</v>
       </c>
       <c r="C285" t="s">
-        <v>864</v>
+        <v>879</v>
       </c>
       <c r="D285">
         <v>0</v>
@@ -10496,16 +10628,19 @@
       <c r="G285">
         <v>0</v>
       </c>
+      <c r="H285" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="286" spans="1:8">
       <c r="A286" t="s">
-        <v>865</v>
+        <v>880</v>
       </c>
       <c r="B286" t="s">
-        <v>866</v>
+        <v>881</v>
       </c>
       <c r="C286" t="s">
-        <v>867</v>
+        <v>882</v>
       </c>
       <c r="D286">
         <v>0</v>
@@ -10519,16 +10654,19 @@
       <c r="G286">
         <v>0</v>
       </c>
+      <c r="H286" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="287" spans="1:8">
       <c r="A287" t="s">
-        <v>868</v>
+        <v>883</v>
       </c>
       <c r="B287" t="s">
-        <v>869</v>
+        <v>884</v>
       </c>
       <c r="C287" t="s">
-        <v>870</v>
+        <v>885</v>
       </c>
       <c r="D287">
         <v>0</v>
@@ -10542,16 +10680,19 @@
       <c r="G287">
         <v>0</v>
       </c>
+      <c r="H287" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="288" spans="1:8">
       <c r="A288" t="s">
-        <v>871</v>
+        <v>886</v>
       </c>
       <c r="B288" t="s">
-        <v>872</v>
+        <v>887</v>
       </c>
       <c r="C288" t="s">
-        <v>873</v>
+        <v>888</v>
       </c>
       <c r="D288">
         <v>0</v>
@@ -10565,13 +10706,16 @@
       <c r="G288">
         <v>0</v>
       </c>
+      <c r="H288" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="289" spans="1:8">
       <c r="A289" t="s">
-        <v>874</v>
+        <v>889</v>
       </c>
       <c r="B289" t="s">
-        <v>875</v>
+        <v>890</v>
       </c>
       <c r="C289" t="s">
         <v>53</v>
@@ -10594,13 +10738,13 @@
     </row>
     <row r="290" spans="1:8">
       <c r="A290" t="s">
-        <v>876</v>
+        <v>891</v>
       </c>
       <c r="B290" t="s">
-        <v>877</v>
+        <v>892</v>
       </c>
       <c r="C290" t="s">
-        <v>878</v>
+        <v>893</v>
       </c>
       <c r="D290">
         <v>0</v>
@@ -10614,16 +10758,19 @@
       <c r="G290">
         <v>0</v>
       </c>
+      <c r="H290" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="291" spans="1:8">
       <c r="A291" t="s">
-        <v>879</v>
+        <v>894</v>
       </c>
       <c r="B291" t="s">
-        <v>880</v>
+        <v>895</v>
       </c>
       <c r="C291" t="s">
-        <v>881</v>
+        <v>896</v>
       </c>
       <c r="D291">
         <v>0</v>
@@ -10635,18 +10782,18 @@
         <v>0.9443483275663207</v>
       </c>
       <c r="G291">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="292" spans="1:8">
       <c r="A292" t="s">
-        <v>882</v>
+        <v>897</v>
       </c>
       <c r="B292" t="s">
-        <v>883</v>
+        <v>898</v>
       </c>
       <c r="C292" t="s">
-        <v>884</v>
+        <v>899</v>
       </c>
       <c r="D292">
         <v>0</v>
@@ -10660,16 +10807,19 @@
       <c r="G292">
         <v>0</v>
       </c>
+      <c r="H292" t="s">
+        <v>900</v>
+      </c>
     </row>
     <row r="293" spans="1:8">
       <c r="A293" t="s">
-        <v>885</v>
+        <v>901</v>
       </c>
       <c r="B293" t="s">
-        <v>886</v>
+        <v>902</v>
       </c>
       <c r="C293" t="s">
-        <v>886</v>
+        <v>902</v>
       </c>
       <c r="D293">
         <v>1</v>
@@ -10686,13 +10836,13 @@
     </row>
     <row r="294" spans="1:8">
       <c r="A294" t="s">
-        <v>887</v>
+        <v>903</v>
       </c>
       <c r="B294" t="s">
-        <v>888</v>
+        <v>904</v>
       </c>
       <c r="C294" t="s">
-        <v>889</v>
+        <v>905</v>
       </c>
       <c r="D294">
         <v>0</v>
@@ -10706,16 +10856,19 @@
       <c r="G294">
         <v>0</v>
       </c>
+      <c r="H294" t="s">
+        <v>906</v>
+      </c>
     </row>
     <row r="295" spans="1:8">
       <c r="A295" t="s">
-        <v>890</v>
+        <v>907</v>
       </c>
       <c r="B295" t="s">
-        <v>891</v>
+        <v>908</v>
       </c>
       <c r="C295" t="s">
-        <v>892</v>
+        <v>909</v>
       </c>
       <c r="D295">
         <v>0</v>
@@ -10729,16 +10882,19 @@
       <c r="G295">
         <v>0</v>
       </c>
+      <c r="H295" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="296" spans="1:8">
       <c r="A296" t="s">
-        <v>893</v>
+        <v>910</v>
       </c>
       <c r="B296" t="s">
-        <v>894</v>
+        <v>911</v>
       </c>
       <c r="C296" t="s">
-        <v>895</v>
+        <v>912</v>
       </c>
       <c r="D296">
         <v>0</v>
@@ -10752,13 +10908,16 @@
       <c r="G296">
         <v>0</v>
       </c>
+      <c r="H296" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="297" spans="1:8">
       <c r="A297" t="s">
-        <v>896</v>
+        <v>913</v>
       </c>
       <c r="B297" t="s">
-        <v>897</v>
+        <v>914</v>
       </c>
       <c r="C297" t="s">
         <v>53</v>
@@ -10781,13 +10940,13 @@
     </row>
     <row r="298" spans="1:8">
       <c r="A298" t="s">
-        <v>898</v>
+        <v>915</v>
       </c>
       <c r="B298" t="s">
-        <v>899</v>
+        <v>916</v>
       </c>
       <c r="C298" t="s">
-        <v>900</v>
+        <v>917</v>
       </c>
       <c r="D298">
         <v>0</v>
@@ -10801,13 +10960,16 @@
       <c r="G298">
         <v>0</v>
       </c>
+      <c r="H298" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="299" spans="1:8">
       <c r="A299" t="s">
-        <v>901</v>
+        <v>918</v>
       </c>
       <c r="B299" t="s">
-        <v>902</v>
+        <v>919</v>
       </c>
       <c r="C299" t="s">
         <v>53</v>
@@ -10830,13 +10992,13 @@
     </row>
     <row r="300" spans="1:8">
       <c r="A300" t="s">
-        <v>903</v>
+        <v>920</v>
       </c>
       <c r="B300" t="s">
-        <v>904</v>
+        <v>921</v>
       </c>
       <c r="C300" t="s">
-        <v>905</v>
+        <v>922</v>
       </c>
       <c r="D300">
         <v>0</v>
@@ -10850,16 +11012,19 @@
       <c r="G300">
         <v>0</v>
       </c>
+      <c r="H300" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="301" spans="1:8">
       <c r="A301" t="s">
-        <v>906</v>
+        <v>923</v>
       </c>
       <c r="B301" t="s">
-        <v>907</v>
+        <v>924</v>
       </c>
       <c r="C301" t="s">
-        <v>908</v>
+        <v>925</v>
       </c>
       <c r="D301">
         <v>0</v>
@@ -10873,13 +11038,16 @@
       <c r="G301">
         <v>0</v>
       </c>
+      <c r="H301" t="s">
+        <v>926</v>
+      </c>
     </row>
     <row r="302" spans="1:8">
       <c r="A302" t="s">
-        <v>909</v>
+        <v>927</v>
       </c>
       <c r="B302" t="s">
-        <v>910</v>
+        <v>928</v>
       </c>
       <c r="C302" t="s">
         <v>53</v>
@@ -10902,13 +11070,13 @@
     </row>
     <row r="303" spans="1:8">
       <c r="A303" t="s">
-        <v>911</v>
+        <v>929</v>
       </c>
       <c r="B303" t="s">
-        <v>912</v>
+        <v>930</v>
       </c>
       <c r="C303" t="s">
-        <v>913</v>
+        <v>931</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -10922,16 +11090,19 @@
       <c r="G303">
         <v>0</v>
       </c>
+      <c r="H303" t="s">
+        <v>932</v>
+      </c>
     </row>
     <row r="304" spans="1:8">
       <c r="A304" t="s">
-        <v>914</v>
+        <v>933</v>
       </c>
       <c r="B304" t="s">
-        <v>915</v>
+        <v>934</v>
       </c>
       <c r="C304" t="s">
-        <v>916</v>
+        <v>935</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -10945,16 +11116,19 @@
       <c r="G304">
         <v>0</v>
       </c>
+      <c r="H304" t="s">
+        <v>936</v>
+      </c>
     </row>
     <row r="305" spans="1:8">
       <c r="A305" t="s">
-        <v>917</v>
+        <v>937</v>
       </c>
       <c r="B305" t="s">
-        <v>918</v>
+        <v>938</v>
       </c>
       <c r="C305" t="s">
-        <v>919</v>
+        <v>939</v>
       </c>
       <c r="D305">
         <v>0</v>
@@ -10968,16 +11142,19 @@
       <c r="G305">
         <v>0</v>
       </c>
+      <c r="H305" t="s">
+        <v>936</v>
+      </c>
     </row>
     <row r="306" spans="1:8">
       <c r="A306" t="s">
-        <v>920</v>
+        <v>940</v>
       </c>
       <c r="B306" t="s">
-        <v>921</v>
+        <v>941</v>
       </c>
       <c r="C306" t="s">
-        <v>922</v>
+        <v>942</v>
       </c>
       <c r="D306">
         <v>0</v>
@@ -10991,16 +11168,19 @@
       <c r="G306">
         <v>0</v>
       </c>
+      <c r="H306" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="307" spans="1:8">
       <c r="A307" t="s">
-        <v>923</v>
+        <v>943</v>
       </c>
       <c r="B307" t="s">
-        <v>924</v>
+        <v>944</v>
       </c>
       <c r="C307" t="s">
-        <v>925</v>
+        <v>945</v>
       </c>
       <c r="D307">
         <v>0</v>
@@ -11014,16 +11194,19 @@
       <c r="G307">
         <v>0</v>
       </c>
+      <c r="H307" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="308" spans="1:8">
       <c r="A308" t="s">
-        <v>926</v>
+        <v>946</v>
       </c>
       <c r="B308" t="s">
-        <v>927</v>
+        <v>947</v>
       </c>
       <c r="C308" t="s">
-        <v>928</v>
+        <v>948</v>
       </c>
       <c r="D308">
         <v>0</v>
@@ -11035,18 +11218,21 @@
         <v>0.61783047343251962</v>
       </c>
       <c r="G308">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H308" t="s">
+        <v>949</v>
       </c>
     </row>
     <row r="309" spans="1:8">
       <c r="A309" t="s">
-        <v>929</v>
+        <v>950</v>
       </c>
       <c r="B309" t="s">
-        <v>930</v>
+        <v>951</v>
       </c>
       <c r="C309" t="s">
-        <v>931</v>
+        <v>952</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -11060,13 +11246,16 @@
       <c r="G309">
         <v>0</v>
       </c>
+      <c r="H309" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="310" spans="1:8">
       <c r="A310" t="s">
-        <v>932</v>
+        <v>953</v>
       </c>
       <c r="B310" t="s">
-        <v>933</v>
+        <v>954</v>
       </c>
       <c r="C310" t="s">
         <v>53</v>
@@ -11089,13 +11278,13 @@
     </row>
     <row r="311" spans="1:8">
       <c r="A311" t="s">
-        <v>934</v>
+        <v>955</v>
       </c>
       <c r="B311" t="s">
-        <v>935</v>
+        <v>956</v>
       </c>
       <c r="C311" t="s">
-        <v>936</v>
+        <v>957</v>
       </c>
       <c r="D311">
         <v>0</v>
@@ -11107,18 +11296,21 @@
         <v>0.68142446290683267</v>
       </c>
       <c r="G311">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H311" t="s">
+        <v>958</v>
       </c>
     </row>
     <row r="312" spans="1:8">
       <c r="A312" t="s">
-        <v>937</v>
+        <v>959</v>
       </c>
       <c r="B312" t="s">
-        <v>938</v>
+        <v>960</v>
       </c>
       <c r="C312" t="s">
-        <v>939</v>
+        <v>961</v>
       </c>
       <c r="D312">
         <v>0</v>
@@ -11132,16 +11324,19 @@
       <c r="G312">
         <v>0</v>
       </c>
+      <c r="H312" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="313" spans="1:8">
       <c r="A313" t="s">
-        <v>940</v>
+        <v>962</v>
       </c>
       <c r="B313" t="s">
-        <v>941</v>
+        <v>963</v>
       </c>
       <c r="C313" t="s">
-        <v>942</v>
+        <v>964</v>
       </c>
       <c r="D313">
         <v>0</v>
@@ -11153,18 +11348,18 @@
         <v>0.99993750000000003</v>
       </c>
       <c r="G313">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="314" spans="1:8">
       <c r="A314" t="s">
-        <v>943</v>
+        <v>965</v>
       </c>
       <c r="B314" t="s">
-        <v>944</v>
+        <v>966</v>
       </c>
       <c r="C314" t="s">
-        <v>945</v>
+        <v>967</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -11178,16 +11373,19 @@
       <c r="G314">
         <v>0</v>
       </c>
+      <c r="H314" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="315" spans="1:8">
       <c r="A315" t="s">
-        <v>946</v>
+        <v>968</v>
       </c>
       <c r="B315" t="s">
-        <v>947</v>
+        <v>969</v>
       </c>
       <c r="C315" t="s">
-        <v>948</v>
+        <v>970</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -11199,18 +11397,21 @@
         <v>0.93186712099431501</v>
       </c>
       <c r="G315">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H315" t="s">
+        <v>971</v>
       </c>
     </row>
     <row r="316" spans="1:8">
       <c r="A316" t="s">
-        <v>949</v>
+        <v>972</v>
       </c>
       <c r="B316" t="s">
-        <v>950</v>
+        <v>973</v>
       </c>
       <c r="C316" t="s">
-        <v>951</v>
+        <v>974</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -11224,16 +11425,19 @@
       <c r="G316">
         <v>0</v>
       </c>
+      <c r="H316" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="317" spans="1:8">
       <c r="A317" t="s">
-        <v>952</v>
+        <v>975</v>
       </c>
       <c r="B317" t="s">
-        <v>953</v>
+        <v>976</v>
       </c>
       <c r="C317" t="s">
-        <v>954</v>
+        <v>977</v>
       </c>
       <c r="D317">
         <v>0</v>
@@ -11247,16 +11451,19 @@
       <c r="G317">
         <v>0</v>
       </c>
+      <c r="H317" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="318" spans="1:8">
       <c r="A318" t="s">
-        <v>955</v>
+        <v>979</v>
       </c>
       <c r="B318" t="s">
-        <v>956</v>
+        <v>980</v>
       </c>
       <c r="C318" t="s">
-        <v>957</v>
+        <v>981</v>
       </c>
       <c r="D318">
         <v>0</v>
@@ -11270,16 +11477,19 @@
       <c r="G318">
         <v>0</v>
       </c>
+      <c r="H318" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="319" spans="1:8">
       <c r="A319" t="s">
-        <v>958</v>
+        <v>982</v>
       </c>
       <c r="B319" t="s">
-        <v>959</v>
+        <v>983</v>
       </c>
       <c r="C319" t="s">
-        <v>960</v>
+        <v>984</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -11293,16 +11503,19 @@
       <c r="G319">
         <v>0</v>
       </c>
+      <c r="H319" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="320" spans="1:8">
       <c r="A320" t="s">
-        <v>961</v>
+        <v>985</v>
       </c>
       <c r="B320" t="s">
-        <v>962</v>
+        <v>986</v>
       </c>
       <c r="C320" t="s">
-        <v>963</v>
+        <v>987</v>
       </c>
       <c r="D320">
         <v>0</v>
@@ -11316,16 +11529,19 @@
       <c r="G320">
         <v>0</v>
       </c>
+      <c r="H320" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="321" spans="1:8">
       <c r="A321" t="s">
-        <v>964</v>
+        <v>988</v>
       </c>
       <c r="B321" t="s">
-        <v>965</v>
+        <v>989</v>
       </c>
       <c r="C321" t="s">
-        <v>966</v>
+        <v>990</v>
       </c>
       <c r="D321">
         <v>0</v>
@@ -11339,16 +11555,19 @@
       <c r="G321">
         <v>0</v>
       </c>
+      <c r="H321" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="322" spans="1:8">
       <c r="A322" t="s">
-        <v>967</v>
+        <v>991</v>
       </c>
       <c r="B322" t="s">
-        <v>968</v>
+        <v>992</v>
       </c>
       <c r="C322" t="s">
-        <v>969</v>
+        <v>993</v>
       </c>
       <c r="D322">
         <v>0</v>
@@ -11362,16 +11581,19 @@
       <c r="G322">
         <v>0</v>
       </c>
+      <c r="H322" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="323" spans="1:8">
       <c r="A323" t="s">
-        <v>970</v>
+        <v>994</v>
       </c>
       <c r="B323" t="s">
-        <v>971</v>
+        <v>995</v>
       </c>
       <c r="C323" t="s">
-        <v>972</v>
+        <v>996</v>
       </c>
       <c r="D323">
         <v>0</v>
@@ -11385,16 +11607,19 @@
       <c r="G323">
         <v>0</v>
       </c>
+      <c r="H323" t="s">
+        <v>997</v>
+      </c>
     </row>
     <row r="324" spans="1:8">
       <c r="A324" t="s">
-        <v>973</v>
+        <v>998</v>
       </c>
       <c r="B324" t="s">
-        <v>974</v>
+        <v>999</v>
       </c>
       <c r="C324" t="s">
-        <v>975</v>
+        <v>1000</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -11408,16 +11633,19 @@
       <c r="G324">
         <v>0</v>
       </c>
+      <c r="H324" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="325" spans="1:8">
       <c r="A325" t="s">
-        <v>976</v>
+        <v>1001</v>
       </c>
       <c r="B325" t="s">
-        <v>977</v>
+        <v>1002</v>
       </c>
       <c r="C325" t="s">
-        <v>978</v>
+        <v>1003</v>
       </c>
       <c r="D325">
         <v>0</v>
@@ -11432,18 +11660,18 @@
         <v>0</v>
       </c>
       <c r="H325" t="s">
-        <v>979</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="326" spans="1:8">
       <c r="A326" t="s">
-        <v>980</v>
+        <v>1005</v>
       </c>
       <c r="B326" t="s">
-        <v>981</v>
+        <v>1006</v>
       </c>
       <c r="C326" t="s">
-        <v>981</v>
+        <v>1006</v>
       </c>
       <c r="D326">
         <v>1</v>
@@ -11460,13 +11688,13 @@
     </row>
     <row r="327" spans="1:8">
       <c r="A327" t="s">
-        <v>982</v>
+        <v>1007</v>
       </c>
       <c r="B327" t="s">
-        <v>983</v>
+        <v>1008</v>
       </c>
       <c r="C327" t="s">
-        <v>984</v>
+        <v>1009</v>
       </c>
       <c r="D327">
         <v>0</v>

</xml_diff>